<commit_message>
reverse polarity for Indin dykes and Ghost Dike Swarm Laurentia-Slave poles
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B5D26-BE2C-7D45-B2A7-3B856ED44458}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FCE98F-62E7-BE41-8238-0355EE5A9CB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25760" windowHeight="14640" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3177,10 +3177,10 @@
   <dimension ref="A1:BK102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A103" sqref="A103:XFD254"/>
+      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7834,10 +7834,11 @@
         <v>5</v>
       </c>
       <c r="P32" s="103">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Q32" s="103">
-        <v>106</v>
+        <f>106+180</f>
+        <v>286</v>
       </c>
       <c r="R32" s="63">
         <v>6</v>

</xml_diff>

<commit_message>
reverse polarity for select Slave poles
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FCE98F-62E7-BE41-8238-0355EE5A9CB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB5AE1-1479-4747-AA94-C4DE904DD901}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25760" windowHeight="14640" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3177,10 +3177,10 @@
   <dimension ref="A1:BK102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7400,10 +7400,11 @@
         <v>4</v>
       </c>
       <c r="P29" s="4">
-        <v>36</v>
+        <v>-36</v>
       </c>
       <c r="Q29" s="4">
-        <v>76</v>
+        <f>76+180</f>
+        <v>256</v>
       </c>
       <c r="R29" s="4">
         <v>7</v>

</xml_diff>

<commit_message>
start adding values in citation column
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB5AE1-1479-4747-AA94-C4DE904DD901}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF993AC0-329A-A74B-A290-2BC5D20F0023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25760" windowHeight="14640" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-580" yWindow="460" windowWidth="20800" windowHeight="16300" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="586">
   <si>
     <t>abs(I)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1798,16 +1798,82 @@
     <t>Overlaps with Ediacaran poles</t>
   </si>
   <si>
-    <t>2 POLE AUTHORS</t>
-  </si>
-  <si>
-    <t>3 POLE AUTHORS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> POLE AUTHORS</t>
   </si>
   <si>
-    <t>4 POLE AUTHORS</t>
+    <t>Overlap_Comment</t>
+  </si>
+  <si>
+    <t>Pole_citation_code</t>
+  </si>
+  <si>
+    <t>Geochron_citation_code</t>
+  </si>
+  <si>
+    <t>not directly dated; dated elsewhere in domain by \cite{Chiarenzelli1989a}</t>
+  </si>
+  <si>
+    <t>\cite{Bickford2005a}</t>
+  </si>
+  <si>
+    <t>\cite{Symons2000a}</t>
+  </si>
+  <si>
+    <t>\cite{Symons1999a}</t>
+  </si>
+  <si>
+    <t>\cite{Kilian2016a}</t>
+  </si>
+  <si>
+    <t>\cite{Kilian2015a}</t>
+  </si>
+  <si>
+    <t>\cite{Selkin2008a}</t>
+  </si>
+  <si>
+    <t>\cite{Evans2010a}</t>
+  </si>
+  <si>
+    <t>\cite{Halls2008a}</t>
+  </si>
+  <si>
+    <t>\cite{Pullaiah1975b}</t>
+  </si>
+  <si>
+    <t>\cite{Buchan2000a}</t>
+  </si>
+  <si>
+    <t>changed dp/dm to match Buchan1993</t>
+  </si>
+  <si>
+    <t>\cite{Buchan1993a}</t>
+  </si>
+  <si>
+    <t>\cite{Gala1995a}</t>
+  </si>
+  <si>
+    <t>Notes_Changes_from_Leirubakki</t>
+  </si>
+  <si>
+    <t>Gala et al. 1995 make a division between VGPs based on their directions. This division doesn't correspond to lithology. They calculate two distinct poles (as well as an overall mean pole). It is unclear which one of these should be paired with the 1758± Bickford et al. (2005) date. For some reason the A grouping was chosen in the Nordic compilation.</t>
+  </si>
+  <si>
+    <t>Ar-Ar hornblende plateau in \cite{Halls1999a} interpretted as age of remanence</t>
+  </si>
+  <si>
+    <t>\cite{Halls1999a}</t>
+  </si>
+  <si>
+    <t>\cite{McGlynn1974a}</t>
+  </si>
+  <si>
+    <t>\cite{Evans1973a}</t>
+  </si>
+  <si>
+    <t>\cite{Mitchell2014a}</t>
+  </si>
+  <si>
+    <t>\cite{Davis1999a}</t>
   </si>
 </sst>
 </file>
@@ -1819,7 +1885,7 @@
     <numFmt numFmtId="165" formatCode="00.0"/>
     <numFmt numFmtId="166" formatCode="000.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1912,6 +1978,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2164,7 +2235,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2520,14 +2591,8 @@
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2574,6 +2639,78 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="190">
@@ -3174,13 +3311,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK102"/>
+  <dimension ref="A1:AW102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3219,22 +3356,14 @@
     <col min="42" max="42" width="15.5" style="25" customWidth="1"/>
     <col min="43" max="43" width="7.6640625" style="8" customWidth="1"/>
     <col min="44" max="44" width="12.33203125" style="42" customWidth="1"/>
-    <col min="45" max="45" width="12.83203125" style="25" customWidth="1"/>
-    <col min="46" max="46" width="17.6640625" style="31" customWidth="1"/>
-    <col min="47" max="47" width="7" style="31" customWidth="1"/>
-    <col min="48" max="48" width="11.83203125" style="31" customWidth="1"/>
-    <col min="49" max="52" width="25.33203125" style="31"/>
-    <col min="53" max="53" width="7.1640625" style="31" customWidth="1"/>
-    <col min="54" max="54" width="25.33203125" style="31"/>
-    <col min="55" max="55" width="10" style="31" customWidth="1"/>
-    <col min="56" max="56" width="10.6640625" style="31" customWidth="1"/>
-    <col min="57" max="60" width="25.33203125" style="31"/>
-    <col min="61" max="61" width="9.33203125" style="31" customWidth="1"/>
-    <col min="62" max="62" width="10.5" style="31" customWidth="1"/>
-    <col min="63" max="16384" width="25.33203125" style="31"/>
+    <col min="45" max="45" width="35.6640625" style="157" customWidth="1"/>
+    <col min="46" max="46" width="17.6640625" style="146" customWidth="1"/>
+    <col min="47" max="47" width="23.5" style="31" customWidth="1"/>
+    <col min="48" max="48" width="19" style="31" customWidth="1"/>
+    <col min="49" max="16384" width="25.33203125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" s="24" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
@@ -3353,7 +3482,7 @@
         <v>31</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AO1" s="19" t="s">
         <v>24</v>
@@ -3367,65 +3496,23 @@
       <c r="AR1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AS1" s="18" t="s">
+      <c r="AS1" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="AT1" s="18" t="s">
-        <v>560</v>
+      <c r="AT1" s="140" t="s">
+        <v>561</v>
       </c>
       <c r="AU1" s="19" t="s">
-        <v>24</v>
+        <v>562</v>
       </c>
       <c r="AV1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="AW1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="AX1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ1" s="18" t="s">
-        <v>561</v>
-      </c>
-      <c r="BA1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="BB1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="BC1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="BD1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="BE1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF1" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="BG1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="BH1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="BI1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="BJ1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="BK1" s="18" t="s">
-        <v>22</v>
+      <c r="AW1" s="24" t="s">
+        <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="47" t="s">
         <v>453</v>
       </c>
@@ -3568,14 +3655,17 @@
       <c r="AR2" s="79" t="s">
         <v>461</v>
       </c>
-      <c r="AS2" s="67" t="s">
+      <c r="AS2" s="147" t="s">
         <v>462</v>
       </c>
-      <c r="AT2" s="105" t="s">
+      <c r="AT2" s="141" t="s">
         <v>463</v>
       </c>
+      <c r="AU2" s="160" t="s">
+        <v>573</v>
+      </c>
     </row>
-    <row r="3" spans="1:63" s="105" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:49" s="105" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
         <v>453</v>
       </c>
@@ -3713,13 +3803,15 @@
       <c r="AR3" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS3" s="67" t="s">
+      <c r="AS3" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT3" s="11"/>
-      <c r="AU3" s="93"/>
+      <c r="AT3" s="126"/>
+      <c r="AU3" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="4" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="47" t="s">
         <v>453</v>
       </c>
@@ -3857,12 +3949,15 @@
       <c r="AR4" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS4" s="67" t="s">
+      <c r="AS4" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT4" s="105"/>
+      <c r="AT4" s="141"/>
+      <c r="AU4" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="5" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="47" t="s">
         <v>453</v>
       </c>
@@ -4000,13 +4095,15 @@
       <c r="AR5" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS5" s="67" t="s">
+      <c r="AS5" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT5" s="11"/>
-      <c r="AU5" s="93"/>
+      <c r="AT5" s="126"/>
+      <c r="AU5" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="6" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:49" s="108" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="47" t="s">
         <v>453</v>
       </c>
@@ -4057,15 +4154,15 @@
       <c r="Q6" s="73">
         <v>284.3</v>
       </c>
-      <c r="R6" s="70">
-        <v>6</v>
-      </c>
-      <c r="S6" s="70">
-        <v>6</v>
+      <c r="R6" s="101">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S6" s="101">
+        <v>7</v>
       </c>
       <c r="T6" s="70">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5.5497747702046434</v>
       </c>
       <c r="U6" s="68" t="s">
         <v>70</v>
@@ -4146,12 +4243,18 @@
       <c r="AR6" s="79" t="s">
         <v>477</v>
       </c>
-      <c r="AS6" s="67" t="s">
+      <c r="AS6" s="152" t="s">
         <v>478</v>
       </c>
-      <c r="AT6" s="105"/>
+      <c r="AT6" s="141"/>
+      <c r="AU6" s="160" t="s">
+        <v>576</v>
+      </c>
+      <c r="AW6" s="160" t="s">
+        <v>575</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>453</v>
       </c>
@@ -4289,12 +4392,15 @@
       <c r="AR7" s="79" t="s">
         <v>153</v>
       </c>
-      <c r="AS7" s="67" t="s">
+      <c r="AS7" s="147" t="s">
         <v>154</v>
       </c>
-      <c r="AT7" s="105"/>
+      <c r="AT7" s="141"/>
+      <c r="AU7" s="160" t="s">
+        <v>574</v>
+      </c>
     </row>
-    <row r="8" spans="1:63" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="47" t="s">
         <v>453</v>
       </c>
@@ -4434,12 +4540,15 @@
       <c r="AR8" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS8" s="67" t="s">
+      <c r="AS8" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT8" s="105"/>
+      <c r="AT8" s="141"/>
+      <c r="AU8" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="9" spans="1:63" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="47" t="s">
         <v>453</v>
       </c>
@@ -4577,15 +4686,17 @@
       <c r="AR9" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS9" s="67" t="s">
+      <c r="AS9" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT9" s="105" t="s">
+      <c r="AT9" s="141" t="s">
         <v>463</v>
       </c>
-      <c r="AU9" s="108"/>
+      <c r="AU9" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="10" spans="1:63" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="47" t="s">
         <v>453</v>
       </c>
@@ -4723,15 +4834,17 @@
       <c r="AR10" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS10" s="67" t="s">
+      <c r="AS10" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT10" s="11" t="s">
+      <c r="AT10" s="126" t="s">
         <v>392</v>
       </c>
-      <c r="AU10" s="93"/>
+      <c r="AU10" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="47" t="s">
         <v>487</v>
       </c>
@@ -4867,15 +4980,17 @@
       <c r="AR11" s="79" t="s">
         <v>492</v>
       </c>
-      <c r="AS11" s="67" t="s">
+      <c r="AS11" s="147" t="s">
         <v>493</v>
       </c>
-      <c r="AT11" s="11" t="s">
+      <c r="AT11" s="126" t="s">
         <v>392</v>
       </c>
-      <c r="AU11" s="93"/>
+      <c r="AU11" s="161" t="s">
+        <v>572</v>
+      </c>
     </row>
-    <row r="12" spans="1:63" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:49" s="33" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="47" t="s">
         <v>487</v>
       </c>
@@ -5013,15 +5128,17 @@
       <c r="AR12" s="79" t="s">
         <v>492</v>
       </c>
-      <c r="AS12" s="67" t="s">
+      <c r="AS12" s="147" t="s">
         <v>493</v>
       </c>
-      <c r="AT12" s="11" t="s">
+      <c r="AT12" s="126" t="s">
         <v>496</v>
       </c>
-      <c r="AU12" s="93"/>
+      <c r="AU12" s="161" t="s">
+        <v>572</v>
+      </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="47" t="s">
         <v>487</v>
       </c>
@@ -5159,15 +5276,17 @@
       <c r="AR13" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS13" s="67" t="s">
+      <c r="AS13" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT13" s="11" t="s">
+      <c r="AT13" s="126" t="s">
         <v>496</v>
       </c>
-      <c r="AU13" s="93"/>
+      <c r="AU13" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="14" spans="1:63" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="47" t="s">
         <v>487</v>
       </c>
@@ -5303,15 +5422,17 @@
       <c r="AR14" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS14" s="67" t="s">
+      <c r="AS14" s="147" t="s">
         <v>469</v>
       </c>
-      <c r="AT14" s="11" t="s">
+      <c r="AT14" s="126" t="s">
         <v>392</v>
       </c>
-      <c r="AU14" s="93"/>
+      <c r="AU14" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="15" spans="1:63" s="94" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:49" s="94" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>487</v>
       </c>
@@ -5449,13 +5570,15 @@
       <c r="AR15" s="79" t="s">
         <v>468</v>
       </c>
-      <c r="AS15" s="78" t="s">
+      <c r="AS15" s="148" t="s">
         <v>469</v>
       </c>
-      <c r="AT15" s="11"/>
-      <c r="AU15" s="93"/>
+      <c r="AT15" s="126"/>
+      <c r="AU15" s="161" t="s">
+        <v>571</v>
+      </c>
     </row>
-    <row r="16" spans="1:63" s="94" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:49" s="94" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="25" t="s">
         <v>449</v>
       </c>
@@ -5592,11 +5715,11 @@
       <c r="AP16" s="77"/>
       <c r="AQ16" s="65"/>
       <c r="AR16" s="77"/>
-      <c r="AS16" s="77"/>
-      <c r="AT16" s="11"/>
+      <c r="AS16" s="149"/>
+      <c r="AT16" s="126"/>
       <c r="AU16" s="93"/>
     </row>
-    <row r="17" spans="1:47" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="47" t="s">
         <v>536</v>
       </c>
@@ -5608,14 +5731,14 @@
       </c>
       <c r="D17" s="77"/>
       <c r="E17" s="77"/>
-      <c r="F17" s="138"/>
+      <c r="F17" s="136"/>
       <c r="G17" s="71">
         <v>45.2</v>
       </c>
       <c r="H17" s="71">
         <v>249.2</v>
       </c>
-      <c r="I17" s="138"/>
+      <c r="I17" s="136"/>
       <c r="J17" s="65">
         <v>74</v>
       </c>
@@ -5733,26 +5856,28 @@
       <c r="AR17" s="97" t="s">
         <v>541</v>
       </c>
-      <c r="AS17" s="93" t="s">
+      <c r="AS17" s="150" t="s">
         <v>542</v>
       </c>
-      <c r="AT17" s="90" t="s">
+      <c r="AT17" s="142" t="s">
         <v>543</v>
       </c>
-      <c r="AU17" s="87"/>
+      <c r="AU17" s="162" t="s">
+        <v>570</v>
+      </c>
     </row>
-    <row r="18" spans="1:47" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="100" t="s">
         <v>536</v>
       </c>
-      <c r="B18" s="126" t="s">
+      <c r="B18" s="124" t="s">
         <v>544</v>
       </c>
       <c r="C18" s="59" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="62"/>
-      <c r="E18" s="136" t="s">
+      <c r="E18" s="134" t="s">
         <v>545</v>
       </c>
       <c r="F18" s="59">
@@ -5802,7 +5927,7 @@
       <c r="T18" s="63">
         <v>7.6</v>
       </c>
-      <c r="U18" s="139" t="s">
+      <c r="U18" s="137" t="s">
         <v>546</v>
       </c>
       <c r="V18" s="59">
@@ -5859,13 +5984,13 @@
       <c r="AK18" s="2">
         <v>2171</v>
       </c>
-      <c r="AL18" s="127" t="s">
+      <c r="AL18" s="125" t="s">
         <v>547</v>
       </c>
-      <c r="AM18" s="127" t="s">
+      <c r="AM18" s="125" t="s">
         <v>544</v>
       </c>
-      <c r="AN18" s="128" t="s">
+      <c r="AN18" s="126" t="s">
         <v>548</v>
       </c>
       <c r="AO18" s="2">
@@ -5877,16 +6002,18 @@
       <c r="AQ18" s="59">
         <v>424</v>
       </c>
-      <c r="AR18" s="129" t="s">
+      <c r="AR18" s="127" t="s">
         <v>550</v>
       </c>
-      <c r="AS18" s="11" t="s">
+      <c r="AS18" s="126" t="s">
         <v>551</v>
       </c>
-      <c r="AT18" s="90"/>
-      <c r="AU18" s="90"/>
+      <c r="AT18" s="142"/>
+      <c r="AU18" s="90" t="s">
+        <v>569</v>
+      </c>
     </row>
-    <row r="19" spans="1:47" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:49" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="100" t="s">
         <v>536</v>
       </c>
@@ -5900,53 +6027,53 @@
       <c r="E19" s="105" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="137">
-        <v>0</v>
-      </c>
-      <c r="G19" s="137">
+      <c r="F19" s="135">
+        <v>0</v>
+      </c>
+      <c r="G19" s="135">
         <v>44.7</v>
       </c>
-      <c r="H19" s="137">
+      <c r="H19" s="135">
         <v>-108.3</v>
       </c>
-      <c r="I19" s="137">
+      <c r="I19" s="135">
         <v>16</v>
       </c>
-      <c r="J19" s="137">
+      <c r="J19" s="135">
         <v>109</v>
       </c>
-      <c r="K19" s="137">
+      <c r="K19" s="135">
         <v>65.099999999999994</v>
       </c>
-      <c r="L19" s="137">
+      <c r="L19" s="135">
         <v>75.2</v>
       </c>
       <c r="M19" s="101">
         <f t="shared" si="0"/>
         <v>75.2</v>
       </c>
-      <c r="N19" s="137">
+      <c r="N19" s="135">
         <v>21.8</v>
       </c>
-      <c r="O19" s="137">
+      <c r="O19" s="135">
         <v>4.7</v>
       </c>
-      <c r="P19" s="137">
+      <c r="P19" s="135">
         <v>49.2</v>
       </c>
-      <c r="Q19" s="137">
+      <c r="Q19" s="135">
         <v>292</v>
       </c>
-      <c r="R19" s="137">
+      <c r="R19" s="135">
         <v>8.1</v>
       </c>
-      <c r="S19" s="137">
+      <c r="S19" s="135">
         <v>8.1</v>
       </c>
-      <c r="T19" s="137">
+      <c r="T19" s="135">
         <v>8.1</v>
       </c>
-      <c r="U19" s="137" t="s">
+      <c r="U19" s="135" t="s">
         <v>553</v>
       </c>
       <c r="V19" s="64">
@@ -5993,7 +6120,7 @@
       <c r="AH19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AI19" s="130">
+      <c r="AI19" s="128">
         <v>1899</v>
       </c>
       <c r="AJ19" s="2">
@@ -6004,16 +6131,16 @@
         <f>1899+5</f>
         <v>1904</v>
       </c>
-      <c r="AL19" s="127" t="s">
+      <c r="AL19" s="125" t="s">
         <v>554</v>
       </c>
       <c r="AM19" s="100" t="s">
         <v>552</v>
       </c>
-      <c r="AN19" s="131" t="s">
+      <c r="AN19" s="129" t="s">
         <v>555</v>
       </c>
-      <c r="AO19" s="132" t="s">
+      <c r="AO19" s="130" t="s">
         <v>556</v>
       </c>
       <c r="AP19" s="60" t="s">
@@ -6025,15 +6152,17 @@
       <c r="AR19" s="61" t="s">
         <v>557</v>
       </c>
-      <c r="AS19" s="100" t="s">
+      <c r="AS19" s="151" t="s">
         <v>558</v>
       </c>
-      <c r="AT19" s="90" t="s">
+      <c r="AT19" s="142" t="s">
         <v>559</v>
       </c>
-      <c r="AU19" s="90"/>
+      <c r="AU19" s="90" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="25" t="s">
         <v>517</v>
       </c>
@@ -6081,8 +6210,8 @@
       <c r="P20" s="73">
         <v>62.400002000000001</v>
       </c>
-      <c r="Q20" s="73">
-        <v>279.39999399999999</v>
+      <c r="Q20" s="103">
+        <v>275.39999999999998</v>
       </c>
       <c r="R20" s="71">
         <v>7.9</v>
@@ -6174,13 +6303,15 @@
       <c r="AR20" s="79" t="s">
         <v>522</v>
       </c>
-      <c r="AS20" s="78" t="s">
+      <c r="AS20" s="148" t="s">
         <v>523</v>
       </c>
-      <c r="AT20" s="11"/>
-      <c r="AU20" s="93"/>
+      <c r="AT20" s="126"/>
+      <c r="AU20" s="161" t="s">
+        <v>567</v>
+      </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:49" ht="56" x14ac:dyDescent="0.15">
       <c r="A21" s="47" t="s">
         <v>517</v>
       </c>
@@ -6319,13 +6450,18 @@
       <c r="AR21" s="79" t="s">
         <v>527</v>
       </c>
-      <c r="AS21" s="67" t="s">
+      <c r="AS21" s="152" t="s">
         <v>528</v>
       </c>
-      <c r="AT21" s="105"/>
-      <c r="AU21" s="108"/>
+      <c r="AT21" s="141"/>
+      <c r="AU21" s="160" t="s">
+        <v>566</v>
+      </c>
+      <c r="AV21" s="31" t="s">
+        <v>564</v>
+      </c>
     </row>
-    <row r="22" spans="1:47" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="47" t="s">
         <v>517</v>
       </c>
@@ -6445,7 +6581,7 @@
       <c r="AK22" s="66">
         <v>1759</v>
       </c>
-      <c r="AL22" s="77" t="s">
+      <c r="AL22" s="163" t="s">
         <v>531</v>
       </c>
       <c r="AM22" s="67" t="s">
@@ -6464,13 +6600,21 @@
       <c r="AR22" s="79" t="s">
         <v>534</v>
       </c>
-      <c r="AS22" s="67" t="s">
+      <c r="AS22" s="152" t="s">
         <v>535</v>
       </c>
-      <c r="AT22" s="90"/>
-      <c r="AU22" s="87"/>
+      <c r="AT22" s="142"/>
+      <c r="AU22" s="162" t="s">
+        <v>577</v>
+      </c>
+      <c r="AV22" s="33" t="s">
+        <v>565</v>
+      </c>
+      <c r="AW22" s="33" t="s">
+        <v>579</v>
+      </c>
     </row>
-    <row r="23" spans="1:47" s="33" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:49" s="33" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A23" s="47" t="s">
         <v>364</v>
       </c>
@@ -6611,13 +6755,18 @@
       <c r="AR23" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="AS23" s="47" t="s">
+      <c r="AS23" s="153" t="s">
         <v>371</v>
       </c>
-      <c r="AT23" s="11"/>
-      <c r="AU23" s="31"/>
+      <c r="AT23" s="126"/>
+      <c r="AU23" s="31" t="s">
+        <v>581</v>
+      </c>
+      <c r="AV23" s="33" t="s">
+        <v>580</v>
+      </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:49" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="47" t="s">
         <v>364</v>
       </c>
@@ -6758,15 +6907,17 @@
       <c r="AR24" s="42" t="s">
         <v>377</v>
       </c>
-      <c r="AS24" s="47" t="s">
+      <c r="AS24" s="153" t="s">
         <v>378</v>
       </c>
-      <c r="AT24" s="105" t="s">
+      <c r="AT24" s="141" t="s">
         <v>379</v>
       </c>
-      <c r="AU24" s="32"/>
+      <c r="AU24" s="32" t="s">
+        <v>582</v>
+      </c>
     </row>
-    <row r="25" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A25" s="47" t="s">
         <v>364</v>
       </c>
@@ -6907,15 +7058,17 @@
       <c r="AR25" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="AS25" s="47" t="s">
+      <c r="AS25" s="153" t="s">
         <v>385</v>
       </c>
-      <c r="AT25" s="105" t="s">
+      <c r="AT25" s="141" t="s">
         <v>379</v>
       </c>
-      <c r="AU25" s="32"/>
+      <c r="AU25" s="32" t="s">
+        <v>583</v>
+      </c>
     </row>
-    <row r="26" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="47" t="s">
         <v>396</v>
       </c>
@@ -7055,13 +7208,18 @@
       <c r="AR26" s="35" t="s">
         <v>400</v>
       </c>
-      <c r="AS26" s="33" t="s">
+      <c r="AS26" s="154" t="s">
         <v>401</v>
       </c>
-      <c r="AT26" s="105"/>
-      <c r="AU26" s="32"/>
+      <c r="AT26" s="141"/>
+      <c r="AU26" s="32" t="s">
+        <v>584</v>
+      </c>
+      <c r="AV26" s="32" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="27" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:49" s="28" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A27" s="47" t="s">
         <v>396</v>
       </c>
@@ -7201,15 +7359,15 @@
       <c r="AR27" s="35" t="s">
         <v>405</v>
       </c>
-      <c r="AS27" s="31" t="s">
+      <c r="AS27" s="146" t="s">
         <v>406</v>
       </c>
-      <c r="AT27" s="105" t="s">
+      <c r="AT27" s="141" t="s">
         <v>407</v>
       </c>
       <c r="AU27" s="32"/>
     </row>
-    <row r="28" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A28" s="47" t="s">
         <v>396</v>
       </c>
@@ -7349,13 +7507,18 @@
       <c r="AR28" s="35" t="s">
         <v>400</v>
       </c>
-      <c r="AS28" s="33" t="s">
+      <c r="AS28" s="154" t="s">
         <v>401</v>
       </c>
-      <c r="AT28" s="105"/>
-      <c r="AU28" s="32"/>
+      <c r="AT28" s="141"/>
+      <c r="AU28" s="32" t="s">
+        <v>584</v>
+      </c>
+      <c r="AV28" s="32" t="s">
+        <v>584</v>
+      </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:49" ht="98" x14ac:dyDescent="0.15">
       <c r="A29" s="100" t="s">
         <v>396</v>
       </c>
@@ -7492,13 +7655,13 @@
       <c r="AR29" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="AS29" s="3" t="s">
+      <c r="AS29" s="143" t="s">
         <v>416</v>
       </c>
-      <c r="AT29" s="105"/>
+      <c r="AT29" s="141"/>
       <c r="AU29" s="105"/>
     </row>
-    <row r="30" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:49" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A30" s="47" t="s">
         <v>396</v>
       </c>
@@ -7639,13 +7802,13 @@
       <c r="AR30" s="79" t="s">
         <v>422</v>
       </c>
-      <c r="AS30" s="108" t="s">
+      <c r="AS30" s="155" t="s">
         <v>423</v>
       </c>
-      <c r="AT30" s="105"/>
+      <c r="AT30" s="141"/>
       <c r="AU30" s="108"/>
     </row>
-    <row r="31" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:49" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A31" s="47" t="s">
         <v>396</v>
       </c>
@@ -7784,17 +7947,17 @@
       <c r="AR31" s="79" t="s">
         <v>429</v>
       </c>
-      <c r="AS31" s="78" t="s">
+      <c r="AS31" s="148" t="s">
         <v>430</v>
       </c>
-      <c r="AT31" s="105"/>
+      <c r="AT31" s="141"/>
       <c r="AU31" s="108"/>
     </row>
-    <row r="32" spans="1:47" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:49" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="60" t="s">
         <v>396</v>
       </c>
-      <c r="B32" s="141" t="s">
+      <c r="B32" s="139" t="s">
         <v>431</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -7929,15 +8092,15 @@
       <c r="AR32" s="88" t="s">
         <v>415</v>
       </c>
-      <c r="AS32" s="86" t="s">
+      <c r="AS32" s="156" t="s">
         <v>416</v>
       </c>
-      <c r="AT32" s="11" t="s">
+      <c r="AT32" s="126" t="s">
         <v>433</v>
       </c>
       <c r="AU32" s="11"/>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:47" ht="56" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>396</v>
       </c>
@@ -8078,13 +8241,13 @@
       <c r="AR33" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="AS33" s="78" t="s">
+      <c r="AS33" s="148" t="s">
         <v>438</v>
       </c>
-      <c r="AT33" s="11"/>
+      <c r="AT33" s="126"/>
       <c r="AU33" s="93"/>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:47" ht="56" x14ac:dyDescent="0.15">
       <c r="A34" s="25" t="s">
         <v>396</v>
       </c>
@@ -8223,13 +8386,13 @@
       <c r="AR34" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="AS34" s="78" t="s">
+      <c r="AS34" s="148" t="s">
         <v>438</v>
       </c>
-      <c r="AT34" s="11"/>
+      <c r="AT34" s="126"/>
       <c r="AU34" s="93"/>
     </row>
-    <row r="35" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A35" s="25" t="s">
         <v>396</v>
       </c>
@@ -8372,13 +8535,13 @@
       <c r="AR35" s="79" t="s">
         <v>444</v>
       </c>
-      <c r="AS35" s="78" t="s">
+      <c r="AS35" s="148" t="s">
         <v>445</v>
       </c>
-      <c r="AT35" s="11"/>
+      <c r="AT35" s="126"/>
       <c r="AU35" s="93"/>
     </row>
-    <row r="36" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A36" s="25" t="s">
         <v>396</v>
       </c>
@@ -8519,13 +8682,13 @@
       <c r="AR36" s="79" t="s">
         <v>444</v>
       </c>
-      <c r="AS36" s="78" t="s">
+      <c r="AS36" s="148" t="s">
         <v>445</v>
       </c>
-      <c r="AT36" s="11"/>
+      <c r="AT36" s="126"/>
       <c r="AU36" s="93"/>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:47" ht="56" x14ac:dyDescent="0.15">
       <c r="A37" s="25" t="s">
         <v>396</v>
       </c>
@@ -8664,13 +8827,13 @@
       <c r="AR37" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="AS37" s="78" t="s">
+      <c r="AS37" s="148" t="s">
         <v>438</v>
       </c>
-      <c r="AT37" s="11"/>
+      <c r="AT37" s="126"/>
       <c r="AU37" s="93"/>
     </row>
-    <row r="38" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:47" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A38" s="47" t="s">
         <v>74</v>
       </c>
@@ -8811,15 +8974,15 @@
       <c r="AR38" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="AS38" s="25" t="s">
+      <c r="AS38" s="157" t="s">
         <v>81</v>
       </c>
-      <c r="AT38" s="3" t="s">
+      <c r="AT38" s="143" t="s">
         <v>82</v>
       </c>
       <c r="AU38" s="33"/>
     </row>
-    <row r="39" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:47" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A39" s="47" t="s">
         <v>74</v>
       </c>
@@ -8960,13 +9123,13 @@
       <c r="AR39" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="AS39" s="25" t="s">
+      <c r="AS39" s="157" t="s">
         <v>89</v>
       </c>
-      <c r="AT39" s="3"/>
+      <c r="AT39" s="143"/>
       <c r="AU39" s="33"/>
     </row>
-    <row r="40" spans="1:47" s="90" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:47" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A40" s="47" t="s">
         <v>74</v>
       </c>
@@ -9107,13 +9270,13 @@
       <c r="AR40" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="AS40" s="25" t="s">
+      <c r="AS40" s="157" t="s">
         <v>97</v>
       </c>
-      <c r="AT40" s="11"/>
+      <c r="AT40" s="126"/>
       <c r="AU40" s="31"/>
     </row>
-    <row r="41" spans="1:47" s="90" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:47" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="47" t="s">
         <v>74</v>
       </c>
@@ -9254,13 +9417,13 @@
       <c r="AR41" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="AS41" s="25" t="s">
+      <c r="AS41" s="157" t="s">
         <v>104</v>
       </c>
-      <c r="AT41" s="3"/>
+      <c r="AT41" s="143"/>
       <c r="AU41" s="33"/>
     </row>
-    <row r="42" spans="1:47" s="87" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:47" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="47" t="s">
         <v>74</v>
       </c>
@@ -9403,13 +9566,13 @@
       <c r="AR42" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="AS42" s="25" t="s">
+      <c r="AS42" s="157" t="s">
         <v>110</v>
       </c>
-      <c r="AT42" s="11"/>
+      <c r="AT42" s="126"/>
       <c r="AU42" s="31"/>
     </row>
-    <row r="43" spans="1:47" s="87" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:47" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A43" s="47" t="s">
         <v>74</v>
       </c>
@@ -9552,13 +9715,13 @@
       <c r="AR43" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="AS43" s="25" t="s">
+      <c r="AS43" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="AT43" s="3"/>
+      <c r="AT43" s="143"/>
       <c r="AU43" s="33"/>
     </row>
-    <row r="44" spans="1:47" s="93" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:47" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A44" s="47" t="s">
         <v>74</v>
       </c>
@@ -9701,13 +9864,13 @@
       <c r="AR44" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="AS44" s="25" t="s">
+      <c r="AS44" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="AT44" s="3"/>
+      <c r="AT44" s="143"/>
       <c r="AU44" s="33"/>
     </row>
-    <row r="45" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A45" s="47" t="s">
         <v>74</v>
       </c>
@@ -9850,15 +10013,15 @@
       <c r="AR45" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="AS45" s="31" t="s">
+      <c r="AS45" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="AT45" s="3" t="s">
+      <c r="AT45" s="143" t="s">
         <v>127</v>
       </c>
       <c r="AU45" s="33"/>
     </row>
-    <row r="46" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:47" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A46" s="47" t="s">
         <v>74</v>
       </c>
@@ -10001,10 +10164,10 @@
       <c r="AR46" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="AS46" s="25" t="s">
+      <c r="AS46" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="3"/>
+      <c r="AT46" s="143"/>
       <c r="AU46" s="33"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
@@ -10144,10 +10307,10 @@
       <c r="AP47" s="16"/>
       <c r="AQ47" s="37"/>
       <c r="AR47" s="16"/>
-      <c r="AS47" s="16"/>
-      <c r="AT47" s="11"/>
+      <c r="AS47" s="158"/>
+      <c r="AT47" s="126"/>
     </row>
-    <row r="48" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:47" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="47" t="s">
         <v>74</v>
       </c>
@@ -10288,10 +10451,10 @@
       <c r="AR48" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="AS48" s="25" t="s">
+      <c r="AS48" s="157" t="s">
         <v>136</v>
       </c>
-      <c r="AT48" s="11"/>
+      <c r="AT48" s="126"/>
       <c r="AU48" s="31"/>
     </row>
     <row r="49" spans="1:47" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10317,10 +10480,10 @@
       <c r="H49" s="110">
         <v>246.400002</v>
       </c>
-      <c r="I49" s="140">
+      <c r="I49" s="138">
         <v>10</v>
       </c>
-      <c r="J49" s="140">
+      <c r="J49" s="138">
         <v>195</v>
       </c>
       <c r="K49" s="5">
@@ -10435,13 +10598,13 @@
       <c r="AR49" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="AS49" s="25" t="s">
+      <c r="AS49" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="AT49" s="11"/>
+      <c r="AT49" s="126"/>
       <c r="AU49" s="31"/>
     </row>
-    <row r="50" spans="1:47" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:47" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A50" s="47" t="s">
         <v>74</v>
       </c>
@@ -10582,13 +10745,13 @@
       <c r="AR50" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="AS50" s="25" t="s">
+      <c r="AS50" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="AT50" s="11"/>
+      <c r="AT50" s="126"/>
       <c r="AU50" s="31"/>
     </row>
-    <row r="51" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="47" t="s">
         <v>74</v>
       </c>
@@ -10729,13 +10892,13 @@
       <c r="AR51" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="AS51" s="25" t="s">
+      <c r="AS51" s="157" t="s">
         <v>145</v>
       </c>
-      <c r="AT51" s="3"/>
+      <c r="AT51" s="143"/>
       <c r="AU51" s="33"/>
     </row>
-    <row r="52" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:47" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A52" s="47" t="s">
         <v>74</v>
       </c>
@@ -10878,13 +11041,13 @@
       <c r="AR52" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="AS52" s="47" t="s">
+      <c r="AS52" s="153" t="s">
         <v>154</v>
       </c>
-      <c r="AT52" s="3"/>
+      <c r="AT52" s="143"/>
       <c r="AU52" s="33"/>
     </row>
-    <row r="53" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A53" s="47" t="s">
         <v>74</v>
       </c>
@@ -11027,13 +11190,13 @@
       <c r="AR53" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="AS53" s="25" t="s">
+      <c r="AS53" s="157" t="s">
         <v>159</v>
       </c>
-      <c r="AT53" s="11"/>
+      <c r="AT53" s="126"/>
       <c r="AU53" s="31"/>
     </row>
-    <row r="54" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A54" s="47" t="s">
         <v>74</v>
       </c>
@@ -11174,10 +11337,10 @@
       <c r="AR54" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="AS54" s="25" t="s">
+      <c r="AS54" s="157" t="s">
         <v>167</v>
       </c>
-      <c r="AT54" s="90"/>
+      <c r="AT54" s="142"/>
       <c r="AU54" s="28"/>
     </row>
     <row r="55" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11317,8 +11480,8 @@
       <c r="AP55" s="16"/>
       <c r="AQ55" s="37"/>
       <c r="AR55" s="16"/>
-      <c r="AS55" s="16"/>
-      <c r="AT55" s="90"/>
+      <c r="AS55" s="158"/>
+      <c r="AT55" s="142"/>
       <c r="AU55" s="28"/>
     </row>
     <row r="56" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11461,8 +11624,8 @@
       <c r="AR56" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="AS56" s="25"/>
-      <c r="AT56" s="90"/>
+      <c r="AS56" s="157"/>
+      <c r="AT56" s="142"/>
       <c r="AU56" s="28"/>
     </row>
     <row r="57" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11605,8 +11768,8 @@
       <c r="AR57" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="AS57" s="25"/>
-      <c r="AT57" s="90"/>
+      <c r="AS57" s="157"/>
+      <c r="AT57" s="142"/>
       <c r="AU57" s="28"/>
     </row>
     <row r="58" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11749,8 +11912,8 @@
       <c r="AR58" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="AS58" s="25"/>
-      <c r="AT58" s="11"/>
+      <c r="AS58" s="157"/>
+      <c r="AT58" s="126"/>
       <c r="AU58" s="31"/>
     </row>
     <row r="59" spans="1:47" x14ac:dyDescent="0.15">
@@ -11894,7 +12057,7 @@
       <c r="AR59" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="AT59" s="90"/>
+      <c r="AT59" s="142"/>
       <c r="AU59" s="28"/>
     </row>
     <row r="60" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -12037,8 +12200,8 @@
       <c r="AR60" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="AS60" s="25"/>
-      <c r="AT60" s="90"/>
+      <c r="AS60" s="157"/>
+      <c r="AT60" s="142"/>
       <c r="AU60" s="28"/>
     </row>
     <row r="61" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12182,8 +12345,8 @@
       <c r="AR61" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="AS61" s="25"/>
-      <c r="AT61" s="11"/>
+      <c r="AS61" s="157"/>
+      <c r="AT61" s="126"/>
       <c r="AU61" s="31"/>
     </row>
     <row r="62" spans="1:47" x14ac:dyDescent="0.15">
@@ -12326,7 +12489,7 @@
       <c r="AR62" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="AT62" s="11"/>
+      <c r="AT62" s="126"/>
     </row>
     <row r="63" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A63" s="47" t="s">
@@ -12470,9 +12633,9 @@
       <c r="AR63" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="AT63" s="11"/>
+      <c r="AT63" s="126"/>
     </row>
-    <row r="64" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A64" s="47" t="s">
         <v>74</v>
       </c>
@@ -12613,13 +12776,13 @@
       <c r="AR64" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="AS64" s="25" t="s">
+      <c r="AS64" s="157" t="s">
         <v>210</v>
       </c>
-      <c r="AT64" s="90"/>
+      <c r="AT64" s="142"/>
       <c r="AU64" s="28"/>
     </row>
-    <row r="65" spans="1:56" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:48" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="47" t="s">
         <v>74</v>
       </c>
@@ -12760,11 +12923,11 @@
         <v>425</v>
       </c>
       <c r="AR65" s="42"/>
-      <c r="AS65" s="25"/>
-      <c r="AT65" s="90"/>
+      <c r="AS65" s="157"/>
+      <c r="AT65" s="142"/>
       <c r="AU65" s="28"/>
     </row>
-    <row r="66" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A66" s="47" t="s">
         <v>74</v>
       </c>
@@ -12905,12 +13068,12 @@
       <c r="AR66" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="AS66" s="25" t="s">
+      <c r="AS66" s="157" t="s">
         <v>221</v>
       </c>
-      <c r="AT66" s="11"/>
+      <c r="AT66" s="126"/>
     </row>
-    <row r="67" spans="1:56" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A67" s="47" t="s">
         <v>74</v>
       </c>
@@ -13048,10 +13211,10 @@
         <v>47</v>
       </c>
       <c r="AR67" s="35"/>
-      <c r="AT67" s="90"/>
+      <c r="AT67" s="142"/>
       <c r="AU67" s="28"/>
     </row>
-    <row r="68" spans="1:56" s="46" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:48" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="47" t="s">
         <v>74</v>
       </c>
@@ -13194,11 +13357,11 @@
       <c r="AR68" s="35" t="s">
         <v>232</v>
       </c>
-      <c r="AS68" s="25"/>
-      <c r="AT68" s="90"/>
+      <c r="AS68" s="157"/>
+      <c r="AT68" s="142"/>
       <c r="AU68" s="28"/>
     </row>
-    <row r="69" spans="1:56" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:48" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A69" s="100" t="s">
         <v>74</v>
       </c>
@@ -13334,13 +13497,13 @@
       <c r="AR69" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="AS69" s="60" t="s">
+      <c r="AS69" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="AT69" s="90"/>
+      <c r="AT69" s="142"/>
       <c r="AU69" s="90"/>
     </row>
-    <row r="70" spans="1:56" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:48" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A70" s="100" t="s">
         <v>74</v>
       </c>
@@ -13476,13 +13639,13 @@
       <c r="AR70" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="AS70" s="60" t="s">
+      <c r="AS70" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="AT70" s="90"/>
+      <c r="AT70" s="142"/>
       <c r="AU70" s="90"/>
     </row>
-    <row r="71" spans="1:56" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:48" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="47" t="s">
         <v>74</v>
       </c>
@@ -13623,13 +13786,13 @@
       <c r="AR71" s="79" t="s">
         <v>244</v>
       </c>
-      <c r="AS71" s="78" t="s">
+      <c r="AS71" s="148" t="s">
         <v>245</v>
       </c>
-      <c r="AT71" s="90"/>
+      <c r="AT71" s="142"/>
       <c r="AU71" s="87"/>
     </row>
-    <row r="72" spans="1:56" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:48" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="47" t="s">
         <v>74</v>
       </c>
@@ -13772,15 +13935,15 @@
       <c r="AR72" s="79" t="s">
         <v>244</v>
       </c>
-      <c r="AS72" s="78" t="s">
+      <c r="AS72" s="148" t="s">
         <v>245</v>
       </c>
-      <c r="AT72" s="90" t="s">
+      <c r="AT72" s="142" t="s">
         <v>249</v>
       </c>
       <c r="AU72" s="87"/>
     </row>
-    <row r="73" spans="1:56" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:48" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A73" s="47" t="s">
         <v>74</v>
       </c>
@@ -13921,15 +14084,15 @@
       <c r="AR73" s="79" t="s">
         <v>253</v>
       </c>
-      <c r="AS73" s="78" t="s">
+      <c r="AS73" s="148" t="s">
         <v>254</v>
       </c>
-      <c r="AT73" s="11" t="s">
+      <c r="AT73" s="126" t="s">
         <v>255</v>
       </c>
       <c r="AU73" s="93"/>
     </row>
-    <row r="74" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="47" t="s">
         <v>74</v>
       </c>
@@ -14072,22 +14235,14 @@
       <c r="AR74" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="AS74" s="47" t="s">
+      <c r="AS74" s="153" t="s">
         <v>261</v>
       </c>
-      <c r="AT74" s="90"/>
+      <c r="AT74" s="142"/>
       <c r="AU74" s="28"/>
-      <c r="AV74" s="133"/>
-      <c r="AW74" s="133"/>
-      <c r="AX74" s="133"/>
-      <c r="AY74" s="133"/>
-      <c r="AZ74" s="133"/>
-      <c r="BA74" s="133"/>
-      <c r="BB74" s="133"/>
-      <c r="BC74" s="133"/>
-      <c r="BD74" s="133"/>
+      <c r="AV74" s="131"/>
     </row>
-    <row r="75" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="47" t="s">
         <v>74</v>
       </c>
@@ -14221,22 +14376,14 @@
       <c r="AP75" s="16"/>
       <c r="AQ75" s="37"/>
       <c r="AR75" s="16"/>
-      <c r="AS75" s="16"/>
-      <c r="AT75" s="90" t="s">
+      <c r="AS75" s="158"/>
+      <c r="AT75" s="142" t="s">
         <v>264</v>
       </c>
       <c r="AU75" s="28"/>
-      <c r="AV75" s="133"/>
-      <c r="AW75" s="133"/>
-      <c r="AX75" s="133"/>
-      <c r="AY75" s="133"/>
-      <c r="AZ75" s="133"/>
-      <c r="BA75" s="133"/>
-      <c r="BB75" s="133"/>
-      <c r="BC75" s="133"/>
-      <c r="BD75" s="133"/>
+      <c r="AV75" s="131"/>
     </row>
-    <row r="76" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="47" t="s">
         <v>74</v>
       </c>
@@ -14377,23 +14524,15 @@
       <c r="AR76" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="AS76" s="31" t="s">
+      <c r="AS76" s="146" t="s">
         <v>269</v>
       </c>
-      <c r="AT76" s="11" t="s">
+      <c r="AT76" s="126" t="s">
         <v>249</v>
       </c>
-      <c r="AV76" s="133"/>
-      <c r="AW76" s="133"/>
-      <c r="AX76" s="133"/>
-      <c r="AY76" s="133"/>
-      <c r="AZ76" s="133"/>
-      <c r="BA76" s="133"/>
-      <c r="BB76" s="133"/>
-      <c r="BC76" s="133"/>
-      <c r="BD76" s="133"/>
+      <c r="AV76" s="131"/>
     </row>
-    <row r="77" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="47" t="s">
         <v>74</v>
       </c>
@@ -14536,24 +14675,16 @@
       <c r="AR77" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="AS77" s="33" t="s">
+      <c r="AS77" s="154" t="s">
         <v>274</v>
       </c>
-      <c r="AT77" s="11" t="s">
+      <c r="AT77" s="126" t="s">
         <v>249</v>
       </c>
       <c r="AU77" s="28"/>
-      <c r="AV77" s="133"/>
-      <c r="AW77" s="133"/>
-      <c r="AX77" s="133"/>
-      <c r="AY77" s="133"/>
-      <c r="AZ77" s="133"/>
-      <c r="BA77" s="133"/>
-      <c r="BB77" s="133"/>
-      <c r="BC77" s="133"/>
-      <c r="BD77" s="133"/>
+      <c r="AV77" s="131"/>
     </row>
-    <row r="78" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="47" t="s">
         <v>74</v>
       </c>
@@ -14696,22 +14827,14 @@
       <c r="AR78" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="AS78" s="47" t="s">
+      <c r="AS78" s="153" t="s">
         <v>280</v>
       </c>
-      <c r="AT78" s="90"/>
+      <c r="AT78" s="142"/>
       <c r="AU78" s="28"/>
-      <c r="AV78" s="133"/>
-      <c r="AW78" s="133"/>
-      <c r="AX78" s="133"/>
-      <c r="AY78" s="133"/>
-      <c r="AZ78" s="133"/>
-      <c r="BA78" s="133"/>
-      <c r="BB78" s="133"/>
-      <c r="BC78" s="133"/>
-      <c r="BD78" s="133"/>
+      <c r="AV78" s="131"/>
     </row>
-    <row r="79" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="47" t="s">
         <v>74</v>
       </c>
@@ -14852,22 +14975,14 @@
       <c r="AR79" s="89" t="s">
         <v>286</v>
       </c>
-      <c r="AS79" s="47" t="s">
+      <c r="AS79" s="153" t="s">
         <v>287</v>
       </c>
-      <c r="AT79" s="123"/>
+      <c r="AT79" s="144"/>
       <c r="AU79" s="43"/>
-      <c r="AV79" s="133"/>
-      <c r="AW79" s="133"/>
-      <c r="AX79" s="133"/>
-      <c r="AY79" s="133"/>
-      <c r="AZ79" s="133"/>
-      <c r="BA79" s="133"/>
-      <c r="BB79" s="133"/>
-      <c r="BC79" s="133"/>
-      <c r="BD79" s="133"/>
+      <c r="AV79" s="131"/>
     </row>
-    <row r="80" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="47" t="s">
         <v>74</v>
       </c>
@@ -15008,24 +15123,16 @@
       <c r="AR80" s="89" t="s">
         <v>286</v>
       </c>
-      <c r="AS80" s="47" t="s">
+      <c r="AS80" s="153" t="s">
         <v>287</v>
       </c>
-      <c r="AT80" s="105" t="s">
+      <c r="AT80" s="141" t="s">
         <v>290</v>
       </c>
       <c r="AU80" s="32"/>
-      <c r="AV80" s="133"/>
-      <c r="AW80" s="133"/>
-      <c r="AX80" s="133"/>
-      <c r="AY80" s="133"/>
-      <c r="AZ80" s="133"/>
-      <c r="BA80" s="133"/>
-      <c r="BB80" s="133"/>
-      <c r="BC80" s="133"/>
-      <c r="BD80" s="133"/>
+      <c r="AV80" s="131"/>
     </row>
-    <row r="81" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="47" t="s">
         <v>74</v>
       </c>
@@ -15166,22 +15273,14 @@
       <c r="AR81" s="42" t="s">
         <v>294</v>
       </c>
-      <c r="AS81" s="47" t="s">
+      <c r="AS81" s="153" t="s">
         <v>295</v>
       </c>
-      <c r="AT81" s="105"/>
+      <c r="AT81" s="141"/>
       <c r="AU81" s="32"/>
-      <c r="AV81" s="133"/>
-      <c r="AW81" s="133"/>
-      <c r="AX81" s="133"/>
-      <c r="AY81" s="133"/>
-      <c r="AZ81" s="133"/>
-      <c r="BA81" s="133"/>
-      <c r="BB81" s="133"/>
-      <c r="BC81" s="133"/>
-      <c r="BD81" s="133"/>
+      <c r="AV81" s="131"/>
     </row>
-    <row r="82" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="47" t="s">
         <v>74</v>
       </c>
@@ -15324,22 +15423,14 @@
       <c r="AR82" s="42" t="s">
         <v>301</v>
       </c>
-      <c r="AS82" s="47" t="s">
+      <c r="AS82" s="153" t="s">
         <v>302</v>
       </c>
-      <c r="AT82" s="105"/>
+      <c r="AT82" s="141"/>
       <c r="AU82" s="32"/>
-      <c r="AV82" s="133"/>
-      <c r="AW82" s="133"/>
-      <c r="AX82" s="133"/>
-      <c r="AY82" s="133"/>
-      <c r="AZ82" s="133"/>
-      <c r="BA82" s="133"/>
-      <c r="BB82" s="133"/>
-      <c r="BC82" s="133"/>
-      <c r="BD82" s="133"/>
+      <c r="AV82" s="131"/>
     </row>
-    <row r="83" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="47" t="s">
         <v>74</v>
       </c>
@@ -15482,24 +15573,16 @@
       <c r="AR83" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="AS83" s="47" t="s">
+      <c r="AS83" s="153" t="s">
         <v>306</v>
       </c>
-      <c r="AT83" s="105" t="s">
+      <c r="AT83" s="141" t="s">
         <v>290</v>
       </c>
       <c r="AU83" s="32"/>
-      <c r="AV83" s="133"/>
-      <c r="AW83" s="133"/>
-      <c r="AX83" s="133"/>
-      <c r="AY83" s="133"/>
-      <c r="AZ83" s="133"/>
-      <c r="BA83" s="133"/>
-      <c r="BB83" s="133"/>
-      <c r="BC83" s="133"/>
-      <c r="BD83" s="133"/>
+      <c r="AV83" s="131"/>
     </row>
-    <row r="84" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="28" t="s">
         <v>307</v>
       </c>
@@ -15636,24 +15719,16 @@
       <c r="AR84" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="AS84" s="28"/>
-      <c r="AT84" s="105"/>
+      <c r="AS84" s="159"/>
+      <c r="AT84" s="141"/>
       <c r="AU84" s="32"/>
-      <c r="AV84" s="133"/>
-      <c r="AW84" s="133"/>
-      <c r="AX84" s="133"/>
-      <c r="AY84" s="133"/>
-      <c r="AZ84" s="133"/>
-      <c r="BA84" s="133"/>
-      <c r="BB84" s="133"/>
-      <c r="BC84" s="133"/>
-      <c r="BD84" s="133"/>
+      <c r="AV84" s="131"/>
     </row>
-    <row r="85" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B85" s="124" t="s">
+      <c r="B85" s="123" t="s">
         <v>315</v>
       </c>
       <c r="C85" s="38">
@@ -15787,26 +15862,18 @@
       <c r="AR85" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="AS85" s="16" t="s">
+      <c r="AS85" s="158" t="s">
         <v>321</v>
       </c>
-      <c r="AT85" s="105"/>
+      <c r="AT85" s="141"/>
       <c r="AU85" s="32"/>
-      <c r="AV85" s="133"/>
-      <c r="AW85" s="133"/>
-      <c r="AX85" s="133"/>
-      <c r="AY85" s="133"/>
-      <c r="AZ85" s="133"/>
-      <c r="BA85" s="133"/>
-      <c r="BB85" s="133"/>
-      <c r="BC85" s="133"/>
-      <c r="BD85" s="133"/>
+      <c r="AV85" s="131"/>
     </row>
-    <row r="86" spans="1:56" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B86" s="124" t="s">
+      <c r="B86" s="123" t="s">
         <v>322</v>
       </c>
       <c r="C86" s="38">
@@ -15939,26 +16006,18 @@
       <c r="AR86" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="AS86" s="16" t="s">
+      <c r="AS86" s="158" t="s">
         <v>326</v>
       </c>
-      <c r="AT86" s="105"/>
+      <c r="AT86" s="141"/>
       <c r="AU86" s="32"/>
-      <c r="AV86" s="133"/>
-      <c r="AW86" s="133"/>
-      <c r="AX86" s="133"/>
-      <c r="AY86" s="133"/>
-      <c r="AZ86" s="133"/>
-      <c r="BA86" s="133"/>
-      <c r="BB86" s="133"/>
-      <c r="BC86" s="133"/>
-      <c r="BD86" s="133"/>
+      <c r="AV86" s="131"/>
     </row>
-    <row r="87" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B87" s="124" t="s">
+      <c r="B87" s="123" t="s">
         <v>327</v>
       </c>
       <c r="C87" s="38">
@@ -16090,26 +16149,18 @@
       <c r="AR87" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="AS87" s="16" t="s">
+      <c r="AS87" s="158" t="s">
         <v>326</v>
       </c>
-      <c r="AT87" s="105"/>
+      <c r="AT87" s="141"/>
       <c r="AU87" s="32"/>
-      <c r="AV87" s="133"/>
-      <c r="AW87" s="133"/>
-      <c r="AX87" s="133"/>
-      <c r="AY87" s="133"/>
-      <c r="AZ87" s="133"/>
-      <c r="BA87" s="133"/>
-      <c r="BB87" s="133"/>
-      <c r="BC87" s="133"/>
-      <c r="BD87" s="133"/>
+      <c r="AV87" s="131"/>
     </row>
-    <row r="88" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B88" s="124" t="s">
+      <c r="B88" s="123" t="s">
         <v>328</v>
       </c>
       <c r="C88" s="38">
@@ -16241,25 +16292,17 @@
       <c r="AR88" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="AS88" s="16" t="s">
+      <c r="AS88" s="158" t="s">
         <v>333</v>
       </c>
-      <c r="AT88" s="11"/>
-      <c r="AV88" s="133"/>
-      <c r="AW88" s="133"/>
-      <c r="AX88" s="133"/>
-      <c r="AY88" s="133"/>
-      <c r="AZ88" s="133"/>
-      <c r="BA88" s="133"/>
-      <c r="BB88" s="133"/>
-      <c r="BC88" s="133"/>
-      <c r="BD88" s="133"/>
+      <c r="AT88" s="126"/>
+      <c r="AV88" s="131"/>
     </row>
-    <row r="89" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:48" ht="56" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B89" s="124" t="s">
+      <c r="B89" s="123" t="s">
         <v>334</v>
       </c>
       <c r="C89" s="38">
@@ -16391,26 +16434,18 @@
       <c r="AR89" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="AS89" s="16" t="s">
+      <c r="AS89" s="158" t="s">
         <v>338</v>
       </c>
-      <c r="AT89" s="125"/>
+      <c r="AT89" s="145"/>
       <c r="AU89" s="46"/>
-      <c r="AV89" s="133"/>
-      <c r="AW89" s="133"/>
-      <c r="AX89" s="133"/>
-      <c r="AY89" s="133"/>
-      <c r="AZ89" s="133"/>
-      <c r="BA89" s="133"/>
-      <c r="BB89" s="133"/>
-      <c r="BC89" s="133"/>
-      <c r="BD89" s="133"/>
+      <c r="AV89" s="131"/>
     </row>
-    <row r="90" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A90" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B90" s="124" t="s">
+      <c r="B90" s="123" t="s">
         <v>339</v>
       </c>
       <c r="C90" s="38">
@@ -16542,26 +16577,18 @@
       <c r="AR90" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="AS90" s="16" t="s">
+      <c r="AS90" s="158" t="s">
         <v>333</v>
       </c>
-      <c r="AT90" s="105"/>
+      <c r="AT90" s="141"/>
       <c r="AU90" s="32"/>
-      <c r="AV90" s="133"/>
-      <c r="AW90" s="133"/>
-      <c r="AX90" s="133"/>
-      <c r="AY90" s="133"/>
-      <c r="AZ90" s="133"/>
-      <c r="BA90" s="133"/>
-      <c r="BB90" s="133"/>
-      <c r="BC90" s="133"/>
-      <c r="BD90" s="133"/>
+      <c r="AV90" s="131"/>
     </row>
-    <row r="91" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A91" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B91" s="124" t="s">
+      <c r="B91" s="123" t="s">
         <v>341</v>
       </c>
       <c r="C91" s="38">
@@ -16693,25 +16720,17 @@
       <c r="AR91" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="AS91" s="16" t="s">
+      <c r="AS91" s="158" t="s">
         <v>333</v>
       </c>
-      <c r="AT91" s="11"/>
-      <c r="AV91" s="133"/>
-      <c r="AW91" s="133"/>
-      <c r="AX91" s="133"/>
-      <c r="AY91" s="133"/>
-      <c r="AZ91" s="133"/>
-      <c r="BA91" s="133"/>
-      <c r="BB91" s="133"/>
-      <c r="BC91" s="133"/>
-      <c r="BD91" s="133"/>
+      <c r="AT91" s="126"/>
+      <c r="AV91" s="131"/>
     </row>
-    <row r="92" spans="1:56" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A92" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B92" s="124" t="s">
+      <c r="B92" s="123" t="s">
         <v>343</v>
       </c>
       <c r="C92" s="38">
@@ -16843,25 +16862,17 @@
       <c r="AR92" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="AS92" s="16" t="s">
+      <c r="AS92" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="AT92" s="11"/>
-      <c r="AV92" s="133"/>
-      <c r="AW92" s="133"/>
-      <c r="AX92" s="133"/>
-      <c r="AY92" s="133"/>
-      <c r="AZ92" s="133"/>
-      <c r="BA92" s="133"/>
-      <c r="BB92" s="133"/>
-      <c r="BC92" s="133"/>
-      <c r="BD92" s="133"/>
+      <c r="AT92" s="126"/>
+      <c r="AV92" s="131"/>
     </row>
-    <row r="93" spans="1:56" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B93" s="124" t="s">
+      <c r="B93" s="123" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="38">
@@ -16993,17 +17004,17 @@
       <c r="AR93" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="AS93" s="16" t="s">
+      <c r="AS93" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="AT93" s="105"/>
+      <c r="AT93" s="141"/>
       <c r="AU93" s="32"/>
     </row>
-    <row r="94" spans="1:56" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B94" s="124" t="s">
+      <c r="B94" s="123" t="s">
         <v>350</v>
       </c>
       <c r="C94" s="38">
@@ -17135,17 +17146,17 @@
       <c r="AR94" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="AS94" s="16" t="s">
+      <c r="AS94" s="158" t="s">
         <v>338</v>
       </c>
-      <c r="AT94" s="105"/>
+      <c r="AT94" s="141"/>
       <c r="AU94" s="32"/>
     </row>
-    <row r="95" spans="1:56" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B95" s="124" t="s">
+      <c r="B95" s="123" t="s">
         <v>352</v>
       </c>
       <c r="C95" s="38">
@@ -17277,16 +17288,16 @@
       <c r="AR95" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="AS95" s="16" t="s">
+      <c r="AS95" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="AT95" s="11"/>
+      <c r="AT95" s="126"/>
     </row>
-    <row r="96" spans="1:56" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="B96" s="124" t="s">
+      <c r="B96" s="123" t="s">
         <v>354</v>
       </c>
       <c r="C96" s="38">
@@ -17418,16 +17429,16 @@
       <c r="AR96" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="AS96" s="16" t="s">
+      <c r="AS96" s="158" t="s">
         <v>338</v>
       </c>
-      <c r="AT96" s="11"/>
+      <c r="AT96" s="126"/>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="B97" s="124" t="s">
+      <c r="B97" s="123" t="s">
         <v>357</v>
       </c>
       <c r="C97" s="38">
@@ -17557,10 +17568,10 @@
       <c r="AR97" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="AS97" s="16" t="s">
+      <c r="AS97" s="158" t="s">
         <v>362</v>
       </c>
-      <c r="AT97" s="105" t="s">
+      <c r="AT97" s="141" t="s">
         <v>363</v>
       </c>
       <c r="AU97" s="46"/>
@@ -17590,7 +17601,7 @@
       <c r="H98" s="30">
         <v>354.5</v>
       </c>
-      <c r="I98" s="135"/>
+      <c r="I98" s="133"/>
       <c r="J98" s="27">
         <v>610</v>
       </c>
@@ -17604,10 +17615,10 @@
         <f t="shared" si="30"/>
         <v>34.700000000000003</v>
       </c>
-      <c r="N98" s="134">
+      <c r="N98" s="132">
         <v>1000</v>
       </c>
-      <c r="O98" s="134">
+      <c r="O98" s="132">
         <v>0.1</v>
       </c>
       <c r="P98" s="30">
@@ -17699,8 +17710,8 @@
       <c r="AP98" s="16"/>
       <c r="AQ98" s="37"/>
       <c r="AR98" s="16"/>
-      <c r="AS98" s="16"/>
-      <c r="AT98" s="105" t="s">
+      <c r="AS98" s="158"/>
+      <c r="AT98" s="141" t="s">
         <v>392</v>
       </c>
       <c r="AU98" s="32"/>
@@ -17730,7 +17741,7 @@
       <c r="H99" s="30">
         <v>354.3</v>
       </c>
-      <c r="I99" s="135"/>
+      <c r="I99" s="133"/>
       <c r="J99" s="27">
         <v>880</v>
       </c>
@@ -17744,10 +17755,10 @@
         <f t="shared" si="30"/>
         <v>56.7</v>
       </c>
-      <c r="N99" s="134">
+      <c r="N99" s="132">
         <v>1000</v>
       </c>
-      <c r="O99" s="134">
+      <c r="O99" s="132">
         <v>0.1</v>
       </c>
       <c r="P99" s="30">
@@ -17837,8 +17848,8 @@
       <c r="AP99" s="16"/>
       <c r="AQ99" s="37"/>
       <c r="AR99" s="16"/>
-      <c r="AS99" s="16"/>
-      <c r="AT99" s="105" t="s">
+      <c r="AS99" s="158"/>
+      <c r="AT99" s="141" t="s">
         <v>395</v>
       </c>
       <c r="AU99" s="32"/>
@@ -17984,10 +17995,10 @@
       <c r="AR100" s="79" t="s">
         <v>509</v>
       </c>
-      <c r="AS100" s="78" t="s">
+      <c r="AS100" s="148" t="s">
         <v>510</v>
       </c>
-      <c r="AT100" s="105"/>
+      <c r="AT100" s="141"/>
       <c r="AU100" s="108"/>
       <c r="AV100" s="95"/>
     </row>
@@ -18132,10 +18143,10 @@
       <c r="AR101" s="79" t="s">
         <v>509</v>
       </c>
-      <c r="AS101" s="78" t="s">
+      <c r="AS101" s="148" t="s">
         <v>510</v>
       </c>
-      <c r="AT101" s="11"/>
+      <c r="AT101" s="126"/>
       <c r="AU101" s="93"/>
       <c r="AV101" s="95"/>
     </row>
@@ -18280,10 +18291,10 @@
       <c r="AR102" s="79" t="s">
         <v>509</v>
       </c>
-      <c r="AS102" s="78" t="s">
+      <c r="AS102" s="148" t="s">
         <v>510</v>
       </c>
-      <c r="AT102" s="105"/>
+      <c r="AT102" s="141"/>
       <c r="AU102" s="108"/>
       <c r="AV102" s="95"/>
     </row>

</xml_diff>

<commit_message>
add more references to the pole refs column along with some age notes
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF993AC0-329A-A74B-A290-2BC5D20F0023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18AF91-8705-4B45-8454-4DE190547939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-580" yWindow="460" windowWidth="20800" windowHeight="16300" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="596">
   <si>
     <t>abs(I)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1874,6 +1874,38 @@
   </si>
   <si>
     <t>\cite{Davis1999a}</t>
+  </si>
+  <si>
+    <t>\cite{Buchan2009a}</t>
+  </si>
+  <si>
+    <t>U–Pb baddeleyite ages of 2023 ± 2 and 2027 ± 4 Ma in \cite{Buchan2009a}</t>
+  </si>
+  <si>
+    <t>U–Pb baddeleyite date of 2231 ± 2 Ma in \cite{Buchan2012a}</t>
+  </si>
+  <si>
+    <t>\cite{Buchan2012a}</t>
+  </si>
+  <si>
+    <t>\cite{Buchan2016a}</t>
+  </si>
+  <si>
+    <t>U–Pb baddeleyite date 2193 ± 2 Ma in \cite{Mitchell2014a}</t>
+  </si>
+  <si>
+    <t>U–Pb baddeleyite date of 2126 ± 3, U-Pb \cite{Buchan2016a} and unpublished abstract cited in text</t>
+  </si>
+  <si>
+    <t>\cite{Mitchell2010c}</t>
+  </si>
+  <si>
+    <t>\cite{Meert2002b}</t>
+  </si>
+  <si>
+    <t>"The St. Francois Mountains (SFM) region of Missouri is a
+1476 ± 16 Ma igneous province in central Laurentia (Figure 1;
+mean age compiled from Van Schmus et al. [1993]"</t>
   </si>
 </sst>
 </file>
@@ -3314,10 +3346,10 @@
   <dimension ref="A1:AW102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AL28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF13" sqref="AF13"/>
+      <selection pane="bottomRight" activeCell="AU32" sqref="AU32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7365,7 +7397,12 @@
       <c r="AT27" s="141" t="s">
         <v>407</v>
       </c>
-      <c r="AU27" s="32"/>
+      <c r="AU27" s="28" t="s">
+        <v>589</v>
+      </c>
+      <c r="AV27" s="31" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="28" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A28" s="47" t="s">
@@ -7515,7 +7552,7 @@
         <v>584</v>
       </c>
       <c r="AV28" s="32" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="98" x14ac:dyDescent="0.15">
@@ -7659,7 +7696,12 @@
         <v>416</v>
       </c>
       <c r="AT29" s="141"/>
-      <c r="AU29" s="105"/>
+      <c r="AU29" s="105" t="s">
+        <v>590</v>
+      </c>
+      <c r="AV29" s="31" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="30" spans="1:49" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A30" s="47" t="s">
@@ -7806,7 +7848,12 @@
         <v>423</v>
       </c>
       <c r="AT30" s="141"/>
-      <c r="AU30" s="108"/>
+      <c r="AU30" s="32" t="s">
+        <v>586</v>
+      </c>
+      <c r="AV30" s="32" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="31" spans="1:49" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A31" s="47" t="s">
@@ -8098,9 +8145,11 @@
       <c r="AT32" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="AU32" s="11"/>
+      <c r="AU32" s="105" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="33" spans="1:47" ht="56" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>396</v>
       </c>
@@ -8245,9 +8294,11 @@
         <v>438</v>
       </c>
       <c r="AT33" s="126"/>
-      <c r="AU33" s="93"/>
+      <c r="AU33" s="93" t="s">
+        <v>593</v>
+      </c>
     </row>
-    <row r="34" spans="1:47" ht="56" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A34" s="25" t="s">
         <v>396</v>
       </c>
@@ -8390,9 +8441,11 @@
         <v>438</v>
       </c>
       <c r="AT34" s="126"/>
-      <c r="AU34" s="93"/>
+      <c r="AU34" s="93" t="s">
+        <v>593</v>
+      </c>
     </row>
-    <row r="35" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A35" s="25" t="s">
         <v>396</v>
       </c>
@@ -8541,7 +8594,7 @@
       <c r="AT35" s="126"/>
       <c r="AU35" s="93"/>
     </row>
-    <row r="36" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A36" s="25" t="s">
         <v>396</v>
       </c>
@@ -8688,7 +8741,7 @@
       <c r="AT36" s="126"/>
       <c r="AU36" s="93"/>
     </row>
-    <row r="37" spans="1:47" ht="56" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A37" s="25" t="s">
         <v>396</v>
       </c>
@@ -8831,9 +8884,11 @@
         <v>438</v>
       </c>
       <c r="AT37" s="126"/>
-      <c r="AU37" s="93"/>
+      <c r="AU37" s="93" t="s">
+        <v>593</v>
+      </c>
     </row>
-    <row r="38" spans="1:47" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A38" s="47" t="s">
         <v>74</v>
       </c>
@@ -8982,7 +9037,7 @@
       </c>
       <c r="AU38" s="33"/>
     </row>
-    <row r="39" spans="1:47" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A39" s="47" t="s">
         <v>74</v>
       </c>
@@ -9129,7 +9184,7 @@
       <c r="AT39" s="143"/>
       <c r="AU39" s="33"/>
     </row>
-    <row r="40" spans="1:47" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A40" s="47" t="s">
         <v>74</v>
       </c>
@@ -9276,7 +9331,7 @@
       <c r="AT40" s="126"/>
       <c r="AU40" s="31"/>
     </row>
-    <row r="41" spans="1:47" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A41" s="47" t="s">
         <v>74</v>
       </c>
@@ -9421,9 +9476,14 @@
         <v>104</v>
       </c>
       <c r="AT41" s="143"/>
-      <c r="AU41" s="33"/>
+      <c r="AU41" s="33" t="s">
+        <v>594</v>
+      </c>
+      <c r="AV41" s="142" t="s">
+        <v>595</v>
+      </c>
     </row>
-    <row r="42" spans="1:47" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:48" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="47" t="s">
         <v>74</v>
       </c>
@@ -9572,7 +9632,7 @@
       <c r="AT42" s="126"/>
       <c r="AU42" s="31"/>
     </row>
-    <row r="43" spans="1:47" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A43" s="47" t="s">
         <v>74</v>
       </c>
@@ -9721,7 +9781,7 @@
       <c r="AT43" s="143"/>
       <c r="AU43" s="33"/>
     </row>
-    <row r="44" spans="1:47" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A44" s="47" t="s">
         <v>74</v>
       </c>
@@ -9870,7 +9930,7 @@
       <c r="AT44" s="143"/>
       <c r="AU44" s="33"/>
     </row>
-    <row r="45" spans="1:47" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A45" s="47" t="s">
         <v>74</v>
       </c>
@@ -10021,7 +10081,7 @@
       </c>
       <c r="AU45" s="33"/>
     </row>
-    <row r="46" spans="1:47" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A46" s="47" t="s">
         <v>74</v>
       </c>
@@ -10170,7 +10230,7 @@
       <c r="AT46" s="143"/>
       <c r="AU46" s="33"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A47" s="47" t="s">
         <v>74</v>
       </c>
@@ -10310,7 +10370,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
     </row>
-    <row r="48" spans="1:47" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="47" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
progress adding references to pole compilation
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E517ECE4-948F-3C49-878C-4CCAAD1A7FBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D716B0A2-5D7B-D94A-BFB7-F73BB84F2B62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29560" windowHeight="26900" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,8 @@
     <definedName name="fenno98_4" localSheetId="0">'Leirubakki-all'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Leirubakki-all'!$AI$1:$AR$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="637">
   <si>
     <t>abs(I)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -629,9 +623,6 @@
     <t>Ro,F+</t>
   </si>
   <si>
-    <t>Agate Pt rhyolite 1105.3±2.3 U-Pb, interbedded with Lower Osler R sites; Davis+Green 97, Swanson-Hysell et al., 2014 G3</t>
-  </si>
-  <si>
     <t>Upper third Osler volcanics -R</t>
   </si>
   <si>
@@ -750,9 +741,6 @@
   </si>
   <si>
     <t>(C+ from Palmer+81; F+ implicit in good grouping after tilt-correction)</t>
-  </si>
-  <si>
-    <t>1087.2±1.6 date in andesite, Kulakov et al 2013</t>
   </si>
   <si>
     <t>Kulakov, E.V., Smirnov, A.V., Diehl, J.F.</t>
@@ -1003,13 +991,7 @@
     <t>Melville Bugt diabase</t>
   </si>
   <si>
-    <t>Denyszyn, S.W., Davis, D.W., Halls, H.C.</t>
-  </si>
-  <si>
     <t>Can. J. Earth Sci.</t>
-  </si>
-  <si>
-    <t>155-167</t>
   </si>
   <si>
     <t>Victoria Fjord dolerite dykes</t>
@@ -1938,6 +1920,108 @@
   </si>
   <si>
     <t>\citep{Murthy1978a}</t>
+  </si>
+  <si>
+    <t>Biscotasing</t>
+  </si>
+  <si>
+    <t>Nipissing N1</t>
+  </si>
+  <si>
+    <t>Senneterre</t>
+  </si>
+  <si>
+    <t>\cite{Swanson-Hysell2014a}</t>
+  </si>
+  <si>
+    <t>\cite{Swanson-Hysell2014b}</t>
+  </si>
+  <si>
+    <t>Agate Pt rhyolite 1105.15 ± 0.3 U-Pb, interbedded with Osler R sites associated with this pole (Swanson-Hysell et al. 2019)</t>
+  </si>
+  <si>
+    <t>GSA Bulletin</t>
+  </si>
+  <si>
+    <t>Swanson-Hysell, N. et al</t>
+  </si>
+  <si>
+    <t>\cite{Swanson-Hysell2019a}</t>
+  </si>
+  <si>
+    <t>1085.67 ± 0.2 date in andesite, Fairchild et al. 2017</t>
+  </si>
+  <si>
+    <t>\cite{Fairchild2017a}</t>
+  </si>
+  <si>
+    <t>\cite{Donadini2011a}</t>
+  </si>
+  <si>
+    <t>\cite{Weil2003a}</t>
+  </si>
+  <si>
+    <t>\cite{Books1972a, Hnat2006a} as calculated in \cite{Swanson-Hysell2019a}</t>
+  </si>
+  <si>
+    <t>\citep{Kean1997a}</t>
+  </si>
+  <si>
+    <t>\cite{Tauxe2009a,Swanson-Hysell2019a}</t>
+  </si>
+  <si>
+    <t>Lulea Nordic workshop calculation</t>
+  </si>
+  <si>
+    <t>\cite{Ernst1993a}</t>
+  </si>
+  <si>
+    <t>\cite{Palmer1977a}</t>
+  </si>
+  <si>
+    <t>\cite{Henry1977a}</t>
+  </si>
+  <si>
+    <t>\cite{Warnock2000a}</t>
+  </si>
+  <si>
+    <t>\cite{Park1989a}</t>
+  </si>
+  <si>
+    <t>Lulea Nordic workshop calculation based on data of \cite{Harlan1993a, Harlan1997a}</t>
+  </si>
+  <si>
+    <t>\cite{Weil2006a}</t>
+  </si>
+  <si>
+    <t>\cite{Denyszyn2009a}</t>
+  </si>
+  <si>
+    <t>\cite{Murthy1992a}</t>
+  </si>
+  <si>
+    <t>\cite{McCausland2011a}</t>
+  </si>
+  <si>
+    <t>\cite{Symons1991a}</t>
+  </si>
+  <si>
+    <t>\cite{Meert1994a}</t>
+  </si>
+  <si>
+    <t>\cite{Tancyk1987a}</t>
+  </si>
+  <si>
+    <t>Halls, Hamilton and Denyszyn</t>
+  </si>
+  <si>
+    <t>Dyke Swarms: Keys for Geodynamic Interpretation</t>
+  </si>
+  <si>
+    <t>\cite{Halls2011a}</t>
+  </si>
+  <si>
+    <t>\cite{Maloof2006a}</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +2033,7 @@
     <numFmt numFmtId="165" formatCode="00.0"/>
     <numFmt numFmtId="166" formatCode="000.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -2047,6 +2131,12 @@
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2299,7 +2389,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2776,6 +2866,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="190">
     <cellStyle name="Bad" xfId="49" builtinId="27"/>
@@ -3378,10 +3469,10 @@
   <dimension ref="A1:AW102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AL43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AL64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS46" sqref="AS46"/>
+      <selection pane="bottomRight" activeCell="AN97" sqref="AN97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3413,7 +3504,7 @@
     <col min="35" max="35" width="11.1640625" style="8" customWidth="1"/>
     <col min="36" max="36" width="8.33203125" style="8" customWidth="1"/>
     <col min="37" max="37" width="8.5" style="8" customWidth="1"/>
-    <col min="38" max="38" width="20.1640625" style="41" customWidth="1"/>
+    <col min="38" max="38" width="26.6640625" style="41" customWidth="1"/>
     <col min="39" max="39" width="23.5" style="25" customWidth="1"/>
     <col min="40" max="40" width="16" style="25" customWidth="1"/>
     <col min="41" max="41" width="6.6640625" style="8" customWidth="1"/>
@@ -3546,7 +3637,7 @@
         <v>31</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="AO1" s="19" t="s">
         <v>24</v>
@@ -3564,33 +3655,33 @@
         <v>22</v>
       </c>
       <c r="AT1" s="140" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="AU1" s="19" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="AV1" s="18" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="AW1" s="24" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C2" s="38">
         <v>2629</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="E2" s="69" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F2" s="68">
         <v>0</v>
@@ -3640,7 +3731,7 @@
         <v>4.8373546489791304</v>
       </c>
       <c r="U2" s="68" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="V2" s="68">
         <v>3</v>
@@ -3699,13 +3790,13 @@
         <v>2681</v>
       </c>
       <c r="AL2" s="79" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="AM2" s="67" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="AN2" s="78" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="AO2" s="66">
         <v>1975</v>
@@ -3714,27 +3805,27 @@
         <v>94</v>
       </c>
       <c r="AQ2" s="66" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="AR2" s="79" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="AS2" s="147" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="AT2" s="141" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="AU2" s="160" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:49" s="105" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>66</v>
@@ -3847,13 +3938,13 @@
         <v>2507</v>
       </c>
       <c r="AL3" s="79" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="AM3" s="67" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AN3" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO3" s="66">
         <v>2010</v>
@@ -3865,22 +3956,22 @@
         <v>183</v>
       </c>
       <c r="AR3" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS3" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT3" s="126"/>
       <c r="AU3" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>66</v>
@@ -3993,13 +4084,13 @@
         <v>2489</v>
       </c>
       <c r="AL4" s="79" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="AM4" s="67" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="AN4" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO4" s="66">
         <v>2010</v>
@@ -4011,22 +4102,22 @@
         <v>183</v>
       </c>
       <c r="AR4" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS4" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT4" s="141"/>
       <c r="AU4" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>66</v>
@@ -4139,13 +4230,13 @@
         <v>2449</v>
       </c>
       <c r="AL5" s="79" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="AM5" s="67" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="AN5" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO5" s="66">
         <v>2010</v>
@@ -4157,25 +4248,25 @@
         <v>183</v>
       </c>
       <c r="AR5" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS5" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT5" s="126"/>
       <c r="AU5" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:49" s="108" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>473</v>
+        <v>605</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D6" s="69"/>
       <c r="E6" s="69" t="s">
@@ -4287,10 +4378,10 @@
         <v>2224</v>
       </c>
       <c r="AL6" s="79" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="AM6" s="67" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="AN6" s="78" t="s">
         <v>151</v>
@@ -4299,31 +4390,31 @@
         <v>1993</v>
       </c>
       <c r="AP6" s="78" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="AQ6" s="66">
         <v>30</v>
       </c>
       <c r="AR6" s="79" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="AS6" s="152" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="AT6" s="141"/>
       <c r="AU6" s="160" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="AW6" s="160" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>478</v>
+        <v>604</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>146</v>
@@ -4436,10 +4527,10 @@
         <v>2221</v>
       </c>
       <c r="AL7" s="79" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="AM7" s="67" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="AN7" s="78" t="s">
         <v>151</v>
@@ -4461,15 +4552,15 @@
       </c>
       <c r="AT7" s="141"/>
       <c r="AU7" s="160" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>480</v>
+        <v>603</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
@@ -4584,13 +4675,13 @@
         <v>2172</v>
       </c>
       <c r="AL8" s="79" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="AM8" s="67" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="AN8" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO8" s="66">
         <v>2010</v>
@@ -4602,22 +4693,22 @@
         <v>183</v>
       </c>
       <c r="AR8" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS8" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT8" s="141"/>
       <c r="AU8" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>66</v>
@@ -4730,13 +4821,13 @@
         <v>2070</v>
       </c>
       <c r="AL9" s="79" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="AM9" s="67" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="AN9" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO9" s="66">
         <v>2010</v>
@@ -4748,24 +4839,24 @@
         <v>183</v>
       </c>
       <c r="AR9" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS9" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT9" s="141" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="AU9" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="47" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>66</v>
@@ -4878,13 +4969,13 @@
         <v>2000</v>
       </c>
       <c r="AL10" s="79" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="AM10" s="67" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="AN10" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO10" s="66">
         <v>2010</v>
@@ -4896,27 +4987,27 @@
         <v>183</v>
       </c>
       <c r="AR10" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS10" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT10" s="126" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AU10" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="47" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
@@ -5024,13 +5115,13 @@
         <v>2126</v>
       </c>
       <c r="AL11" s="79" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="AM11" s="67" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="AN11" s="78" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="AO11" s="66">
         <v>2008</v>
@@ -5042,27 +5133,27 @@
         <v>162</v>
       </c>
       <c r="AR11" s="79" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="AS11" s="147" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="AT11" s="126" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AU11" s="161" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="12" spans="1:49" s="33" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="47" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D12" s="69"/>
       <c r="E12" s="69" t="s">
@@ -5172,13 +5263,13 @@
         <v>2106</v>
       </c>
       <c r="AL12" s="79" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="AM12" s="67" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="AN12" s="78" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="AO12" s="66">
         <v>2008</v>
@@ -5190,24 +5281,24 @@
         <v>162</v>
       </c>
       <c r="AR12" s="79" t="s">
+        <v>487</v>
+      </c>
+      <c r="AS12" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="AT12" s="126" t="s">
         <v>491</v>
       </c>
-      <c r="AS12" s="147" t="s">
-        <v>492</v>
-      </c>
-      <c r="AT12" s="126" t="s">
-        <v>495</v>
-      </c>
       <c r="AU12" s="161" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="47" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B13" s="109" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>66</v>
@@ -5320,13 +5411,13 @@
         <v>2093</v>
       </c>
       <c r="AL13" s="79" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="AM13" s="67" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="AN13" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO13" s="66">
         <v>2010</v>
@@ -5338,24 +5429,24 @@
         <v>183</v>
       </c>
       <c r="AR13" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS13" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT13" s="126" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="AU13" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="47" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>66</v>
@@ -5466,13 +5557,13 @@
         <v>2081</v>
       </c>
       <c r="AL14" s="79" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="AM14" s="67" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="AN14" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO14" s="66">
         <v>2010</v>
@@ -5484,24 +5575,24 @@
         <v>183</v>
       </c>
       <c r="AR14" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS14" s="147" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT14" s="126" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AU14" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15" spans="1:49" s="94" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5614,13 +5705,13 @@
         <v>1884</v>
       </c>
       <c r="AL15" s="79" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="AM15" s="78" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="AN15" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AO15" s="66">
         <v>2010</v>
@@ -5632,28 +5723,28 @@
         <v>183</v>
       </c>
       <c r="AR15" s="79" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AS15" s="148" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AT15" s="126"/>
       <c r="AU15" s="161" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" spans="1:49" s="94" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="25" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E16" s="79" t="s">
         <v>68</v>
@@ -5765,10 +5856,10 @@
         <v>1871</v>
       </c>
       <c r="AL16" s="79" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="AM16" s="78" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AN16" s="77" t="s">
         <v>49</v>
@@ -5785,10 +5876,10 @@
     </row>
     <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="47" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B17" s="112" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>121</v>
@@ -5900,49 +5991,49 @@
         <v>2709</v>
       </c>
       <c r="AL17" s="87" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="AM17" s="77" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="AN17" s="93" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="AO17" s="66">
         <v>2008</v>
       </c>
       <c r="AP17" s="93" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="AQ17" s="65">
         <v>9</v>
       </c>
       <c r="AR17" s="97" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="AS17" s="150" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="AT17" s="142" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="AU17" s="162" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="18" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="100" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C18" s="59" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="62"/>
       <c r="E18" s="134" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F18" s="59">
         <v>100</v>
@@ -5992,7 +6083,7 @@
         <v>7.6</v>
       </c>
       <c r="U18" s="137" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="V18" s="59">
         <v>4</v>
@@ -6049,40 +6140,40 @@
         <v>2171</v>
       </c>
       <c r="AL18" s="125" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="AM18" s="125" t="s">
+        <v>539</v>
+      </c>
+      <c r="AN18" s="126" t="s">
         <v>543</v>
-      </c>
-      <c r="AN18" s="126" t="s">
-        <v>547</v>
       </c>
       <c r="AO18" s="2">
         <v>2015</v>
       </c>
       <c r="AP18" s="11" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="AQ18" s="59">
         <v>424</v>
       </c>
       <c r="AR18" s="127" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="AS18" s="126" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="AT18" s="142"/>
       <c r="AU18" s="90" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="19" spans="1:49" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="100" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B19" s="120" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>34</v>
@@ -6138,7 +6229,7 @@
         <v>8.1</v>
       </c>
       <c r="U19" s="135" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="V19" s="64">
         <v>4</v>
@@ -6196,16 +6287,16 @@
         <v>1904</v>
       </c>
       <c r="AL19" s="125" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="AM19" s="100" t="s">
+        <v>547</v>
+      </c>
+      <c r="AN19" s="129" t="s">
+        <v>550</v>
+      </c>
+      <c r="AO19" s="130" t="s">
         <v>551</v>
-      </c>
-      <c r="AN19" s="129" t="s">
-        <v>554</v>
-      </c>
-      <c r="AO19" s="130" t="s">
-        <v>555</v>
       </c>
       <c r="AP19" s="60" t="s">
         <v>180</v>
@@ -6214,31 +6305,31 @@
         <v>44</v>
       </c>
       <c r="AR19" s="61" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="AS19" s="151" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AT19" s="142" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="AU19" s="90" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="25" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B20" s="117" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C20" s="8">
         <v>8359</v>
       </c>
       <c r="D20" s="79"/>
       <c r="E20" s="79" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F20" s="66">
         <v>0</v>
@@ -6350,37 +6441,37 @@
         <v>64</v>
       </c>
       <c r="AM20" s="78" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="AN20" s="78" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="AO20" s="66">
         <v>1999</v>
       </c>
       <c r="AP20" s="78" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="AQ20" s="66" t="s">
         <v>108</v>
       </c>
       <c r="AR20" s="79" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="AS20" s="148" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="AT20" s="126"/>
       <c r="AU20" s="161" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:49" ht="56" x14ac:dyDescent="0.15">
       <c r="A21" s="47" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B21" s="109" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C21" s="38">
         <v>8889</v>
@@ -6497,46 +6588,46 @@
         <v>64</v>
       </c>
       <c r="AM21" s="67" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="AN21" s="78" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="AO21" s="66">
         <v>2000</v>
       </c>
       <c r="AP21" s="78" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="AQ21" s="66" t="s">
         <v>60</v>
       </c>
       <c r="AR21" s="79" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="AS21" s="152" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="AT21" s="141"/>
       <c r="AU21" s="160" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="AV21" s="31" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="22" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="47" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B22" s="109" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="69" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="68">
@@ -6646,50 +6737,50 @@
         <v>1759</v>
       </c>
       <c r="AL22" s="163" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="AM22" s="67" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="AN22" s="78" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="AO22" s="66">
         <v>1995</v>
       </c>
       <c r="AP22" s="78" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="AQ22" s="66"/>
       <c r="AR22" s="79" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="AS22" s="152" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="AT22" s="142"/>
       <c r="AU22" s="162" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="AV22" s="33" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AW22" s="33" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="23" spans="1:49" s="33" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A23" s="47" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B23" s="109" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C23" s="38">
         <v>8429</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="38">
@@ -6799,13 +6890,13 @@
         <v>1924</v>
       </c>
       <c r="AL23" s="41" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="AM23" s="47" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="AN23" s="25" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AO23" s="8">
         <v>1999</v>
@@ -6814,35 +6905,35 @@
         <v>35</v>
       </c>
       <c r="AQ23" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AR23" s="42" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="AS23" s="153" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="AT23" s="126"/>
       <c r="AU23" s="31" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="AV23" s="33" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="47" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B24" s="109" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C24" s="38">
         <v>2642</v>
       </c>
       <c r="D24" s="39"/>
       <c r="E24" s="39" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F24" s="38">
         <v>0</v>
@@ -6951,13 +7042,13 @@
         <v>1831</v>
       </c>
       <c r="AL24" s="41" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="AM24" s="47" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="AN24" s="25" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AO24" s="8">
         <v>1974</v>
@@ -6966,27 +7057,27 @@
         <v>94</v>
       </c>
       <c r="AQ24" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AR24" s="42" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AS24" s="153" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AT24" s="141" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AU24" s="32" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="25" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A25" s="47" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B25" s="109" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C25" s="38">
         <v>2659</v>
@@ -7102,13 +7193,13 @@
         <v>1822</v>
       </c>
       <c r="AL25" s="41" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="AM25" s="47" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AN25" s="25" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AO25" s="8">
         <v>1973</v>
@@ -7117,27 +7208,27 @@
         <v>94</v>
       </c>
       <c r="AQ25" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AR25" s="42" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AS25" s="153" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AT25" s="141" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AU25" s="32" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="26" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="47" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B26" s="116" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>34</v>
@@ -7252,13 +7343,13 @@
         <v>2630</v>
       </c>
       <c r="AL26" s="33" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AM26" s="33" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AN26" s="33" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="AO26" s="8">
         <v>2014</v>
@@ -7270,25 +7361,25 @@
         <v>314</v>
       </c>
       <c r="AR26" s="35" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AS26" s="154" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="AT26" s="141"/>
       <c r="AU26" s="32" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="AV26" s="32" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="27" spans="1:49" s="28" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A27" s="47" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B27" s="116" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C27" s="34">
         <v>13555</v>
@@ -7403,45 +7494,45 @@
         <v>2233</v>
       </c>
       <c r="AL27" s="33" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AM27" s="33" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AN27" s="33" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="AO27" s="8">
         <v>2012</v>
       </c>
       <c r="AP27" s="33" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="AQ27" s="34">
         <v>49</v>
       </c>
       <c r="AR27" s="35" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AS27" s="146" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="AT27" s="141" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="AU27" s="28" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="AV27" s="31" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A28" s="47" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B28" s="116" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C28" s="4">
         <v>9406</v>
@@ -7556,13 +7647,13 @@
         <v>2195</v>
       </c>
       <c r="AL28" s="33" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="AM28" s="33" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="AN28" s="33" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="AO28" s="8">
         <v>2014</v>
@@ -7574,25 +7665,25 @@
         <v>314</v>
       </c>
       <c r="AR28" s="35" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AS28" s="154" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="AT28" s="141"/>
       <c r="AU28" s="32" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="AV28" s="32" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="98" x14ac:dyDescent="0.15">
       <c r="A29" s="100" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B29" s="120" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C29" s="4">
         <v>9484</v>
@@ -7704,50 +7795,50 @@
         <v>2129</v>
       </c>
       <c r="AL29" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="AM29" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AO29" s="2">
         <v>2016</v>
       </c>
       <c r="AP29" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AQ29" s="4">
         <v>275</v>
       </c>
       <c r="AR29" s="12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AS29" s="143" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AT29" s="141"/>
       <c r="AU29" s="105" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="AV29" s="31" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="30" spans="1:49" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A30" s="47" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B30" s="117" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C30" s="34">
         <v>100035</v>
       </c>
       <c r="D30" s="69"/>
       <c r="E30" s="69" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F30" s="68">
         <v>0</v>
@@ -7856,50 +7947,50 @@
         <v>2031</v>
       </c>
       <c r="AL30" s="77" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AM30" s="78" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AN30" s="78" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="AO30" s="66">
         <v>2009</v>
       </c>
       <c r="AP30" s="78" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AQ30" s="66">
         <v>46</v>
       </c>
       <c r="AR30" s="79" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AS30" s="155" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AT30" s="141"/>
       <c r="AU30" s="32" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="AV30" s="32" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="31" spans="1:49" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A31" s="47" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C31" s="38">
         <v>5915</v>
       </c>
       <c r="D31" s="69"/>
       <c r="E31" s="99" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F31" s="68">
         <v>100</v>
@@ -8008,38 +8099,38 @@
         <v>1969</v>
       </c>
       <c r="AL31" s="77" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="AM31" s="78" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="AN31" s="78" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="AO31" s="66">
         <v>1981</v>
       </c>
       <c r="AP31" s="78" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="AQ31" s="66"/>
       <c r="AR31" s="79" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="AS31" s="148" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="AT31" s="141"/>
       <c r="AU31" s="108" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="32" spans="1:49" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="60" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B32" s="139" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>34</v>
@@ -8153,42 +8244,42 @@
         <v>1892</v>
       </c>
       <c r="AL32" s="62" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="AM32" s="60" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="AN32" s="86" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AO32" s="2">
         <v>2016</v>
       </c>
       <c r="AP32" s="86" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AQ32" s="9">
         <v>275</v>
       </c>
       <c r="AR32" s="88" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AS32" s="156" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AT32" s="126" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="AU32" s="105" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="33" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -8304,13 +8395,13 @@
         <v>1890</v>
       </c>
       <c r="AL33" s="77" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="AM33" s="78" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="AN33" s="78" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="AO33" s="66">
         <v>2010</v>
@@ -8322,22 +8413,22 @@
         <v>179</v>
       </c>
       <c r="AR33" s="79" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="AS33" s="148" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="AT33" s="126"/>
       <c r="AU33" s="93" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="34" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A34" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -8451,13 +8542,13 @@
         <v>1886</v>
       </c>
       <c r="AL34" s="77" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="AM34" s="78" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="AN34" s="78" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="AO34" s="66">
         <v>2010</v>
@@ -8469,28 +8560,28 @@
         <v>179</v>
       </c>
       <c r="AR34" s="79" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="AS34" s="148" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="AT34" s="126"/>
       <c r="AU34" s="93" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="35" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A35" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B35" s="117" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C35" s="8">
         <v>16</v>
       </c>
       <c r="D35" s="79" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E35" s="79" t="s">
         <v>61</v>
@@ -8602,13 +8693,13 @@
         <v>1886</v>
       </c>
       <c r="AL35" s="77" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="AM35" s="78" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="AN35" s="78" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="AO35" s="66">
         <v>1979</v>
@@ -8620,22 +8711,22 @@
         <v>65</v>
       </c>
       <c r="AR35" s="79" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="AS35" s="148" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AT35" s="126"/>
       <c r="AU35" s="93" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A36" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B36" s="117" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C36" s="8">
         <v>18</v>
@@ -8751,13 +8842,13 @@
         <v>1886</v>
       </c>
       <c r="AL36" s="77" t="s">
+        <v>437</v>
+      </c>
+      <c r="AM36" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="AM36" s="78" t="s">
-        <v>445</v>
-      </c>
       <c r="AN36" s="78" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="AO36" s="66">
         <v>1979</v>
@@ -8769,22 +8860,22 @@
         <v>65</v>
       </c>
       <c r="AR36" s="79" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="AS36" s="148" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AT36" s="126"/>
       <c r="AU36" s="93" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A37" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -8898,13 +8989,13 @@
         <v>1874</v>
       </c>
       <c r="AL37" s="77" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="AM37" s="78" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="AN37" s="78" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="AO37" s="66">
         <v>2010</v>
@@ -8916,14 +9007,14 @@
         <v>179</v>
       </c>
       <c r="AR37" s="79" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="AS37" s="148" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="AT37" s="126"/>
       <c r="AU37" s="93" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="38" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9074,7 +9165,7 @@
         <v>82</v>
       </c>
       <c r="AU38" s="33" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -9223,7 +9314,7 @@
       </c>
       <c r="AT39" s="143"/>
       <c r="AU39" s="33" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9372,7 +9463,7 @@
       </c>
       <c r="AT40" s="126"/>
       <c r="AU40" s="31" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
@@ -9521,10 +9612,10 @@
       </c>
       <c r="AT41" s="143"/>
       <c r="AU41" s="33" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="AV41" s="142" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="42" spans="1:48" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9675,7 +9766,7 @@
       </c>
       <c r="AT42" s="126"/>
       <c r="AU42" s="31" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -9826,7 +9917,7 @@
       </c>
       <c r="AT43" s="143"/>
       <c r="AU43" s="33" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -9977,7 +10068,7 @@
       </c>
       <c r="AT44" s="143"/>
       <c r="AU44" s="33" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -10130,7 +10221,7 @@
         <v>127</v>
       </c>
       <c r="AU45" s="33" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10281,7 +10372,7 @@
       </c>
       <c r="AT46" s="143"/>
       <c r="AU46" s="33" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
@@ -10295,7 +10386,7 @@
         <v>66</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>61</v>
@@ -10424,7 +10515,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
       <c r="AU47" s="31" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -10573,7 +10664,7 @@
       </c>
       <c r="AT48" s="126"/>
       <c r="AU48" s="31" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="49" spans="1:47" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10722,7 +10813,7 @@
       </c>
       <c r="AT49" s="126"/>
       <c r="AU49" s="33" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="50" spans="1:47" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10871,7 +10962,7 @@
       </c>
       <c r="AT50" s="126"/>
       <c r="AU50" s="33" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="51" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11020,7 +11111,7 @@
       </c>
       <c r="AT51" s="143"/>
       <c r="AU51" s="33" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="52" spans="1:47" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -11170,7 +11261,9 @@
         <v>153</v>
       </c>
       <c r="AT52" s="143"/>
-      <c r="AU52" s="33"/>
+      <c r="AU52" s="33" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="53" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A53" s="47" t="s">
@@ -11319,7 +11412,9 @@
         <v>158</v>
       </c>
       <c r="AT53" s="126"/>
-      <c r="AU53" s="31"/>
+      <c r="AU53" s="31" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="54" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A54" s="47" t="s">
@@ -11466,7 +11561,9 @@
         <v>166</v>
       </c>
       <c r="AT54" s="142"/>
-      <c r="AU54" s="28"/>
+      <c r="AU54" s="28" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="55" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="47" t="s">
@@ -11581,14 +11678,13 @@
         <v>67</v>
       </c>
       <c r="AI55" s="14">
-        <f t="shared" si="21"/>
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="AJ55" s="8">
         <v>1107</v>
       </c>
       <c r="AK55" s="8">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="AL55" s="41" t="s">
         <v>170</v>
@@ -11607,7 +11703,9 @@
       <c r="AR55" s="16"/>
       <c r="AS55" s="158"/>
       <c r="AT55" s="142"/>
-      <c r="AU55" s="28"/>
+      <c r="AU55" s="28" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="56" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="47" t="s">
@@ -11722,7 +11820,7 @@
         <f t="shared" si="21"/>
         <v>1108</v>
       </c>
-      <c r="AJ56" s="37">
+      <c r="AJ56" s="135">
         <v>1105</v>
       </c>
       <c r="AK56" s="8">
@@ -11751,7 +11849,9 @@
       </c>
       <c r="AS56" s="157"/>
       <c r="AT56" s="142"/>
-      <c r="AU56" s="28"/>
+      <c r="AU56" s="28" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="57" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A57" s="47" t="s">
@@ -11863,11 +11963,10 @@
         <v>27</v>
       </c>
       <c r="AI57" s="14">
-        <f t="shared" si="21"/>
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="AJ57" s="8">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="AK57" s="8">
         <v>1111</v>
@@ -11895,7 +11994,9 @@
       </c>
       <c r="AS57" s="157"/>
       <c r="AT57" s="142"/>
-      <c r="AU57" s="28"/>
+      <c r="AU57" s="28" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="58" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A58" s="47" t="s">
@@ -12039,7 +12140,9 @@
       </c>
       <c r="AS58" s="157"/>
       <c r="AT58" s="126"/>
-      <c r="AU58" s="31"/>
+      <c r="AU58" s="28" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="59" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A59" s="47" t="s">
@@ -12088,11 +12191,11 @@
       <c r="O59" s="114">
         <v>0.1</v>
       </c>
-      <c r="P59" s="34">
-        <v>42.5</v>
-      </c>
-      <c r="Q59" s="34">
-        <v>201.6</v>
+      <c r="P59" s="4">
+        <v>42.3</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>203.4</v>
       </c>
       <c r="R59" s="34">
         <v>3.7</v>
@@ -12156,48 +12259,46 @@
         <v>1105</v>
       </c>
       <c r="AJ59" s="8">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="AK59" s="8">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="AL59" s="32" t="s">
+        <v>608</v>
+      </c>
+      <c r="AM59" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="AM59" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="AN59" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO59" s="34">
-        <v>2014</v>
-      </c>
-      <c r="AP59" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="AQ59" s="34">
-        <v>15</v>
-      </c>
-      <c r="AR59" s="35" t="s">
-        <v>176</v>
-      </c>
+      <c r="AN59" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="AO59" s="4">
+        <v>2019</v>
+      </c>
+      <c r="AP59" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="AQ59" s="34"/>
+      <c r="AR59" s="35"/>
       <c r="AT59" s="142"/>
-      <c r="AU59" s="28"/>
+      <c r="AU59" s="28" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="60" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B60" s="116" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C60" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="39"/>
       <c r="E60" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F60" s="38">
         <v>100</v>
@@ -12295,20 +12396,19 @@
         <v>27</v>
       </c>
       <c r="AI60" s="14">
-        <f t="shared" si="21"/>
         <v>1105</v>
       </c>
       <c r="AJ60" s="8">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="AK60" s="8">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AM60" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AN60" s="33" t="s">
         <v>179</v>
@@ -12327,21 +12427,23 @@
       </c>
       <c r="AS60" s="157"/>
       <c r="AT60" s="142"/>
-      <c r="AU60" s="28"/>
+      <c r="AU60" s="28" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="61" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A61" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="116" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D61" s="39"/>
       <c r="E61" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F61" s="38">
         <v>100</v>
@@ -12441,19 +12543,19 @@
       </c>
       <c r="AI61" s="14">
         <f t="shared" si="21"/>
-        <v>1100.5</v>
+        <v>1101</v>
       </c>
       <c r="AJ61" s="8">
         <v>1100</v>
       </c>
-      <c r="AK61" s="8">
-        <v>1101</v>
+      <c r="AK61" s="2">
+        <v>1102</v>
       </c>
       <c r="AL61" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AM61" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN61" s="33" t="s">
         <v>179</v>
@@ -12472,21 +12574,23 @@
       </c>
       <c r="AS61" s="157"/>
       <c r="AT61" s="126"/>
-      <c r="AU61" s="31"/>
+      <c r="AU61" s="28" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="62" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A62" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="39"/>
       <c r="E62" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F62" s="38">
         <v>100</v>
@@ -12583,21 +12687,20 @@
       <c r="AH62" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AI62" s="14">
-        <f t="shared" si="21"/>
-        <v>1098</v>
-      </c>
-      <c r="AJ62" s="8">
-        <v>1095</v>
-      </c>
-      <c r="AK62" s="8">
-        <v>1101</v>
+      <c r="AI62" s="84">
+        <v>1094</v>
+      </c>
+      <c r="AJ62" s="2">
+        <v>1090</v>
+      </c>
+      <c r="AK62" s="2">
+        <v>1100</v>
       </c>
       <c r="AL62" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AM62" s="33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AN62" s="33" t="s">
         <v>179</v>
@@ -12615,19 +12718,22 @@
         <v>181</v>
       </c>
       <c r="AT62" s="126"/>
+      <c r="AU62" s="28" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="63" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A63" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B63" s="116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>61</v>
@@ -12663,21 +12769,20 @@
       <c r="O63" s="114">
         <v>0.1</v>
       </c>
-      <c r="P63" s="34">
-        <v>34.5</v>
-      </c>
-      <c r="Q63" s="34">
-        <v>181.3</v>
-      </c>
-      <c r="R63" s="34">
-        <v>2.8</v>
-      </c>
-      <c r="S63" s="34">
-        <v>2.8</v>
-      </c>
-      <c r="T63" s="34">
-        <f t="shared" si="20"/>
-        <v>2.8</v>
+      <c r="P63" s="4">
+        <v>31.1</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>181.7</v>
+      </c>
+      <c r="R63" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="S63" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="T63" s="4">
+        <v>2.1</v>
       </c>
       <c r="U63" s="34">
         <v>0</v>
@@ -12738,13 +12843,13 @@
         <v>1100</v>
       </c>
       <c r="AL63" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="AM63" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="AN63" s="33" t="s">
         <v>200</v>
-      </c>
-      <c r="AM63" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN63" s="33" t="s">
-        <v>201</v>
       </c>
       <c r="AO63" s="37">
         <v>2009</v>
@@ -12756,16 +12861,19 @@
         <v>177</v>
       </c>
       <c r="AR63" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AT63" s="126"/>
+      <c r="AU63" s="31" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="64" spans="1:47" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A64" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C64" s="38">
         <v>8163</v>
@@ -12881,47 +12989,49 @@
         <v>1097</v>
       </c>
       <c r="AL64" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM64" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="AN64" s="25" t="s">
         <v>204</v>
-      </c>
-      <c r="AM64" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="AN64" s="25" t="s">
-        <v>205</v>
       </c>
       <c r="AO64" s="8">
         <v>1997</v>
       </c>
       <c r="AP64" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ64" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="AQ64" s="8" t="s">
+      <c r="AR64" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="AR64" s="42" t="s">
+      <c r="AS64" s="157" t="s">
         <v>208</v>
       </c>
-      <c r="AS64" s="157" t="s">
-        <v>209</v>
-      </c>
       <c r="AT64" s="142"/>
-      <c r="AU64" s="28"/>
+      <c r="AU64" s="28" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="65" spans="1:48" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C65" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D65" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E65" s="39" t="s">
         <v>211</v>
-      </c>
-      <c r="E65" s="39" t="s">
-        <v>212</v>
       </c>
       <c r="F65" s="38">
         <v>100</v>
@@ -12954,21 +13064,20 @@
       <c r="O65" s="40">
         <v>5.6</v>
       </c>
-      <c r="P65" s="110">
-        <v>26.7</v>
-      </c>
-      <c r="Q65" s="30">
-        <v>178</v>
-      </c>
-      <c r="R65" s="40">
-        <v>3.5</v>
-      </c>
-      <c r="S65" s="40">
-        <v>6.3</v>
-      </c>
-      <c r="T65" s="40">
-        <f t="shared" si="20"/>
-        <v>4.6957427527495588</v>
+      <c r="P65" s="102">
+        <v>27.5</v>
+      </c>
+      <c r="Q65" s="103">
+        <v>182.5</v>
+      </c>
+      <c r="R65" s="101">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S65" s="101">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T65" s="101">
+        <v>2.2999999999999998</v>
       </c>
       <c r="U65" s="38">
         <v>0</v>
@@ -13030,13 +13139,13 @@
         <v>1098</v>
       </c>
       <c r="AL65" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="AM65" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN65" s="25" t="s">
         <v>213</v>
-      </c>
-      <c r="AM65" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN65" s="25" t="s">
-        <v>214</v>
       </c>
       <c r="AO65" s="8">
         <v>2006</v>
@@ -13050,21 +13159,23 @@
       <c r="AR65" s="42"/>
       <c r="AS65" s="157"/>
       <c r="AT65" s="142"/>
-      <c r="AU65" s="28"/>
+      <c r="AU65" s="28" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="66" spans="1:48" ht="56" x14ac:dyDescent="0.15">
       <c r="A66" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B66" s="109" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C66" s="38">
         <v>9073</v>
       </c>
       <c r="D66" s="39"/>
       <c r="E66" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F66" s="38">
         <v>100</v>
@@ -13173,13 +13284,13 @@
         <v>1096</v>
       </c>
       <c r="AL66" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM66" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="AN66" s="25" t="s">
         <v>217</v>
-      </c>
-      <c r="AM66" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="AN66" s="25" t="s">
-        <v>218</v>
       </c>
       <c r="AO66" s="8">
         <v>2003</v>
@@ -13191,25 +13302,28 @@
         <v>12</v>
       </c>
       <c r="AR66" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="AS66" s="157" t="s">
         <v>219</v>
       </c>
-      <c r="AS66" s="157" t="s">
-        <v>220</v>
-      </c>
       <c r="AT66" s="126"/>
+      <c r="AU66" s="31" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="67" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A67" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="116" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C67" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D67" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E67" s="119"/>
       <c r="F67" s="38">
@@ -13318,42 +13432,44 @@
         <v>1099</v>
       </c>
       <c r="AL67" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AM67" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="AN67" s="33" t="s">
         <v>223</v>
-      </c>
-      <c r="AM67" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="AN67" s="33" t="s">
-        <v>224</v>
       </c>
       <c r="AO67" s="34">
         <v>2011</v>
       </c>
       <c r="AP67" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AQ67" s="34">
         <v>47</v>
       </c>
       <c r="AR67" s="35"/>
       <c r="AT67" s="142"/>
-      <c r="AU67" s="28"/>
+      <c r="AU67" s="28" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="68" spans="1:48" s="46" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B68" s="109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C68" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="E68" s="111" t="s">
         <v>227</v>
-      </c>
-      <c r="E68" s="111" t="s">
-        <v>228</v>
       </c>
       <c r="F68" s="118">
         <v>100</v>
@@ -13452,23 +13568,22 @@
         <v>67</v>
       </c>
       <c r="AI68" s="14">
-        <f t="shared" si="21"/>
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="AJ68" s="8">
         <v>1085</v>
       </c>
       <c r="AK68" s="8">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="AL68" s="41" t="s">
-        <v>229</v>
+        <v>612</v>
       </c>
       <c r="AM68" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AN68" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AO68" s="8">
         <v>2013</v>
@@ -13480,7 +13595,7 @@
         <v>50</v>
       </c>
       <c r="AR68" s="35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AS68" s="157"/>
       <c r="AT68" s="142"/>
@@ -13491,7 +13606,7 @@
         <v>74</v>
       </c>
       <c r="B69" s="120" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C69" s="64" t="s">
         <v>34</v>
@@ -13602,38 +13717,40 @@
         <v>1092</v>
       </c>
       <c r="AL69" s="62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AM69" s="100" t="s">
+        <v>230</v>
+      </c>
+      <c r="AN69" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="AN69" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="AO69" s="2">
         <v>2017</v>
       </c>
       <c r="AP69" s="60" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AQ69" s="4">
         <v>9</v>
       </c>
       <c r="AR69" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AS69" s="129" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AT69" s="142"/>
-      <c r="AU69" s="90"/>
+      <c r="AU69" s="90" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="70" spans="1:48" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A70" s="100" t="s">
         <v>74</v>
       </c>
       <c r="B70" s="120" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C70" s="64" t="s">
         <v>34</v>
@@ -13744,38 +13861,40 @@
         <v>1085</v>
       </c>
       <c r="AL70" s="62" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AM70" s="100" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AN70" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AO70" s="2">
         <v>2017</v>
       </c>
       <c r="AP70" s="60" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AQ70" s="4">
         <v>9</v>
       </c>
       <c r="AR70" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AS70" s="129" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AT70" s="142"/>
-      <c r="AU70" s="90"/>
+      <c r="AU70" s="90" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="71" spans="1:48" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C71" s="38">
         <v>2053</v>
@@ -13881,23 +14000,22 @@
         <v>71</v>
       </c>
       <c r="AI71" s="14">
-        <f t="shared" ref="AI71:AI102" si="32">AVERAGE(AJ71:AK71)</f>
-        <v>1050</v>
+        <v>1080</v>
       </c>
       <c r="AJ71" s="66">
-        <v>1020</v>
+        <v>1070</v>
       </c>
       <c r="AK71" s="66">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="AL71" s="77" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AM71" s="78" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN71" s="78" t="s">
         <v>240</v>
-      </c>
-      <c r="AN71" s="78" t="s">
-        <v>242</v>
       </c>
       <c r="AO71" s="66">
         <v>1977</v>
@@ -13909,26 +14027,28 @@
         <v>62</v>
       </c>
       <c r="AR71" s="79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AS71" s="148" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AT71" s="142"/>
-      <c r="AU71" s="87"/>
+      <c r="AU71" s="162" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="72" spans="1:48" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B72" s="109" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C72" s="38">
         <v>2051</v>
       </c>
       <c r="D72" s="69" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E72" s="69" t="s">
         <v>58</v>
@@ -14030,23 +14150,22 @@
         <v>71</v>
       </c>
       <c r="AI72" s="14">
-        <f t="shared" si="32"/>
-        <v>1050</v>
+        <v>1070</v>
       </c>
       <c r="AJ72" s="66">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="AK72" s="66">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="AL72" s="77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AM72" s="78" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AN72" s="78" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AO72" s="66">
         <v>1977</v>
@@ -14058,22 +14177,24 @@
         <v>62</v>
       </c>
       <c r="AR72" s="79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AS72" s="148" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AT72" s="142" t="s">
-        <v>248</v>
-      </c>
-      <c r="AU72" s="87"/>
+        <v>246</v>
+      </c>
+      <c r="AU72" s="162" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="73" spans="1:48" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A73" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="109" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C73" s="38">
         <v>9165</v>
@@ -14179,7 +14300,7 @@
         <v>71</v>
       </c>
       <c r="AI73" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="AI71:AI102" si="32">AVERAGE(AJ73:AK73)</f>
         <v>1015</v>
       </c>
       <c r="AJ73" s="66">
@@ -14192,10 +14313,10 @@
         <v>85</v>
       </c>
       <c r="AM73" s="78" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AN73" s="78" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AO73" s="66">
         <v>2000</v>
@@ -14204,25 +14325,27 @@
         <v>32</v>
       </c>
       <c r="AQ73" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="AR73" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="AS73" s="148" t="s">
         <v>251</v>
       </c>
-      <c r="AR73" s="79" t="s">
+      <c r="AT73" s="126" t="s">
         <v>252</v>
       </c>
-      <c r="AS73" s="148" t="s">
-        <v>253</v>
-      </c>
-      <c r="AT73" s="126" t="s">
-        <v>254</v>
-      </c>
-      <c r="AU73" s="93"/>
+      <c r="AU73" s="161" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="74" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="109" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C74" s="38">
         <v>5922</v>
@@ -14340,13 +14463,13 @@
         <v>780</v>
       </c>
       <c r="AL74" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AM74" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN74" s="25" t="s">
         <v>255</v>
-      </c>
-      <c r="AN74" s="25" t="s">
-        <v>257</v>
       </c>
       <c r="AO74" s="8">
         <v>1989</v>
@@ -14355,16 +14478,18 @@
         <v>94</v>
       </c>
       <c r="AQ74" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR74" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="AS74" s="153" t="s">
         <v>258</v>
       </c>
-      <c r="AR74" s="42" t="s">
-        <v>259</v>
-      </c>
-      <c r="AS74" s="153" t="s">
-        <v>260</v>
-      </c>
       <c r="AT74" s="142"/>
-      <c r="AU74" s="28"/>
+      <c r="AU74" s="28" t="s">
+        <v>624</v>
+      </c>
       <c r="AV74" s="131"/>
     </row>
     <row r="75" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14372,13 +14497,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="122" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C75" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D75" s="39" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E75" s="39"/>
       <c r="F75" s="38">
@@ -14487,10 +14612,10 @@
         <v>780</v>
       </c>
       <c r="AL75" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AM75" s="44" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AN75" s="16" t="s">
         <v>49</v>
@@ -14503,9 +14628,11 @@
       <c r="AR75" s="16"/>
       <c r="AS75" s="158"/>
       <c r="AT75" s="142" t="s">
-        <v>263</v>
-      </c>
-      <c r="AU75" s="28"/>
+        <v>261</v>
+      </c>
+      <c r="AU75" s="28" t="s">
+        <v>625</v>
+      </c>
       <c r="AV75" s="131"/>
     </row>
     <row r="76" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14513,7 +14640,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="112" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C76" s="23" t="s">
         <v>121</v>
@@ -14570,7 +14697,7 @@
         <v>4.684160890685348</v>
       </c>
       <c r="U76" s="23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="V76" s="23">
         <v>4</v>
@@ -14632,10 +14759,10 @@
         <v>123</v>
       </c>
       <c r="AM76" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN76" s="31" t="s">
         <v>264</v>
-      </c>
-      <c r="AN76" s="31" t="s">
-        <v>266</v>
       </c>
       <c r="AO76" s="8">
         <v>2006</v>
@@ -14647,13 +14774,16 @@
         <v>147</v>
       </c>
       <c r="AR76" s="41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AS76" s="146" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AT76" s="126" t="s">
-        <v>248</v>
+        <v>246</v>
+      </c>
+      <c r="AU76" s="31" t="s">
+        <v>626</v>
       </c>
       <c r="AV76" s="131"/>
     </row>
@@ -14662,7 +14792,7 @@
         <v>74</v>
       </c>
       <c r="B77" s="117" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>66</v>
@@ -14780,13 +14910,13 @@
         <v>727</v>
       </c>
       <c r="AL77" s="33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AM77" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="AN77" s="25" t="s">
         <v>269</v>
-      </c>
-      <c r="AN77" s="25" t="s">
-        <v>271</v>
       </c>
       <c r="AO77" s="8">
         <v>2009</v>
@@ -14798,15 +14928,17 @@
         <v>46</v>
       </c>
       <c r="AR77" s="42" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AS77" s="154" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AT77" s="126" t="s">
-        <v>248</v>
-      </c>
-      <c r="AU77" s="28"/>
+        <v>246</v>
+      </c>
+      <c r="AU77" s="28" t="s">
+        <v>627</v>
+      </c>
       <c r="AV77" s="131"/>
     </row>
     <row r="78" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14814,13 +14946,13 @@
         <v>74</v>
       </c>
       <c r="B78" s="109" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D78" s="39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E78" s="39" t="s">
         <v>28</v>
@@ -14935,10 +15067,10 @@
         <v>64</v>
       </c>
       <c r="AM78" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="AN78" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="AN78" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="AO78" s="8">
         <v>1992</v>
@@ -14947,16 +15079,18 @@
         <v>94</v>
       </c>
       <c r="AQ78" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="AR78" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="AS78" s="153" t="s">
         <v>277</v>
       </c>
-      <c r="AR78" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="AS78" s="153" t="s">
-        <v>279</v>
-      </c>
       <c r="AT78" s="142"/>
-      <c r="AU78" s="28"/>
+      <c r="AU78" s="28" t="s">
+        <v>628</v>
+      </c>
       <c r="AV78" s="131"/>
     </row>
     <row r="79" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14964,13 +15098,13 @@
         <v>74</v>
       </c>
       <c r="B79" s="109" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C79" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D79" s="39" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E79" s="39"/>
       <c r="F79" s="38">
@@ -15080,13 +15214,13 @@
         <v>585</v>
       </c>
       <c r="AL79" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="AM79" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="AN79" s="94" t="s">
         <v>282</v>
-      </c>
-      <c r="AM79" s="47" t="s">
-        <v>283</v>
-      </c>
-      <c r="AN79" s="94" t="s">
-        <v>284</v>
       </c>
       <c r="AO79" s="36">
         <v>2011</v>
@@ -15098,13 +15232,15 @@
         <v>187</v>
       </c>
       <c r="AR79" s="89" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AS79" s="153" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AT79" s="144"/>
-      <c r="AU79" s="43"/>
+      <c r="AU79" s="43" t="s">
+        <v>629</v>
+      </c>
       <c r="AV79" s="131"/>
     </row>
     <row r="80" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -15112,13 +15248,13 @@
         <v>74</v>
       </c>
       <c r="B80" s="109" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C80" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D80" s="39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E80" s="39"/>
       <c r="F80" s="38">
@@ -15228,13 +15364,13 @@
         <v>585</v>
       </c>
       <c r="AL80" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="AM80" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="AN80" s="94" t="s">
         <v>282</v>
-      </c>
-      <c r="AM80" s="47" t="s">
-        <v>288</v>
-      </c>
-      <c r="AN80" s="94" t="s">
-        <v>284</v>
       </c>
       <c r="AO80" s="36">
         <v>2011</v>
@@ -15246,15 +15382,17 @@
         <v>187</v>
       </c>
       <c r="AR80" s="89" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AS80" s="153" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AT80" s="141" t="s">
-        <v>289</v>
-      </c>
-      <c r="AU80" s="32"/>
+        <v>287</v>
+      </c>
+      <c r="AU80" s="43" t="s">
+        <v>629</v>
+      </c>
       <c r="AV80" s="131"/>
     </row>
     <row r="81" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -15262,7 +15400,7 @@
         <v>74</v>
       </c>
       <c r="B81" s="109" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C81" s="38">
         <v>6458</v>
@@ -15381,10 +15519,10 @@
         <v>64</v>
       </c>
       <c r="AM81" s="47" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AN81" s="25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AO81" s="8">
         <v>1991</v>
@@ -15393,16 +15531,18 @@
         <v>94</v>
       </c>
       <c r="AQ81" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="AR81" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="AS81" s="153" t="s">
         <v>292</v>
       </c>
-      <c r="AR81" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="AS81" s="153" t="s">
-        <v>294</v>
-      </c>
       <c r="AT81" s="141"/>
-      <c r="AU81" s="32"/>
+      <c r="AU81" s="32" t="s">
+        <v>630</v>
+      </c>
       <c r="AV81" s="131"/>
     </row>
     <row r="82" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -15410,7 +15550,7 @@
         <v>74</v>
       </c>
       <c r="B82" s="109" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C82" s="38">
         <v>7474</v>
@@ -15419,7 +15559,7 @@
         <v>56</v>
       </c>
       <c r="E82" s="39" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F82" s="38">
         <v>100</v>
@@ -15528,13 +15668,13 @@
         <v>577</v>
       </c>
       <c r="AL82" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AM82" s="47" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AN82" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AO82" s="8">
         <v>1994</v>
@@ -15543,16 +15683,18 @@
         <v>32</v>
       </c>
       <c r="AQ82" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="AR82" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="AS82" s="153" t="s">
         <v>299</v>
       </c>
-      <c r="AR82" s="42" t="s">
-        <v>300</v>
-      </c>
-      <c r="AS82" s="153" t="s">
-        <v>301</v>
-      </c>
       <c r="AT82" s="141"/>
-      <c r="AU82" s="32"/>
+      <c r="AU82" s="32" t="s">
+        <v>631</v>
+      </c>
       <c r="AV82" s="131"/>
     </row>
     <row r="83" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -15560,7 +15702,7 @@
         <v>74</v>
       </c>
       <c r="B83" s="109" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C83" s="38">
         <v>1752</v>
@@ -15681,10 +15823,10 @@
         <v>64</v>
       </c>
       <c r="AM83" s="47" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AN83" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AO83" s="8">
         <v>1987</v>
@@ -15693,26 +15835,28 @@
         <v>94</v>
       </c>
       <c r="AQ83" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AR83" s="42" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AS83" s="153" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AT83" s="141" t="s">
-        <v>289</v>
-      </c>
-      <c r="AU83" s="32"/>
+        <v>287</v>
+      </c>
+      <c r="AU83" s="32" t="s">
+        <v>632</v>
+      </c>
       <c r="AV83" s="131"/>
     </row>
     <row r="84" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B84" s="116" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C84" s="34">
         <v>100377</v>
@@ -15768,7 +15912,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="U84" s="29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="V84" s="29"/>
       <c r="W84" s="6">
@@ -15824,37 +15968,35 @@
         <v>1638</v>
       </c>
       <c r="AL84" s="28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AM84" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="AN84" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="AO84" s="34">
-        <v>2009</v>
-      </c>
-      <c r="AP84" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="AQ84" s="34">
-        <v>46</v>
-      </c>
-      <c r="AR84" s="35" t="s">
-        <v>313</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="AN84" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="AO84" s="4">
+        <v>2011</v>
+      </c>
+      <c r="AP84" s="164" t="s">
+        <v>634</v>
+      </c>
+      <c r="AQ84" s="4"/>
+      <c r="AR84" s="12"/>
       <c r="AS84" s="159"/>
       <c r="AT84" s="141"/>
-      <c r="AU84" s="32"/>
+      <c r="AU84" s="32" t="s">
+        <v>635</v>
+      </c>
       <c r="AV84" s="131"/>
     </row>
     <row r="85" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B85" s="123" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C85" s="38">
         <v>489</v>
@@ -15967,28 +16109,28 @@
         <v>1384</v>
       </c>
       <c r="AL85" s="39" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AM85" s="39" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AN85" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AO85" s="37">
         <v>1987</v>
       </c>
       <c r="AP85" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AQ85" s="37">
         <v>91</v>
       </c>
       <c r="AR85" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AS85" s="158" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="AT85" s="141"/>
       <c r="AU85" s="32"/>
@@ -15996,10 +16138,10 @@
     </row>
     <row r="86" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B86" s="123" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C86" s="38">
         <v>99</v>
@@ -16111,28 +16253,28 @@
         <v>1384</v>
       </c>
       <c r="AL86" s="39" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="AM86" s="39" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AN86" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AO86" s="37">
         <v>1983</v>
       </c>
       <c r="AP86" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AQ86" s="37">
         <v>73</v>
       </c>
       <c r="AR86" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="AS86" s="158" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AT86" s="141"/>
       <c r="AU86" s="32"/>
@@ -16140,10 +16282,10 @@
     </row>
     <row r="87" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B87" s="123" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C87" s="38">
         <v>98</v>
@@ -16254,28 +16396,28 @@
         <v>1384</v>
       </c>
       <c r="AL87" s="39" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AM87" s="39" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="AN87" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AO87" s="37">
         <v>1983</v>
       </c>
       <c r="AP87" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AQ87" s="37">
         <v>73</v>
       </c>
       <c r="AR87" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="AS87" s="158" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AT87" s="141"/>
       <c r="AU87" s="32"/>
@@ -16283,10 +16425,10 @@
     </row>
     <row r="88" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B88" s="123" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C88" s="38">
         <v>2107</v>
@@ -16397,38 +16539,38 @@
         <v>1277</v>
       </c>
       <c r="AL88" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="AM88" s="39" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="AN88" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AO88" s="37">
         <v>1977</v>
       </c>
       <c r="AP88" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AQ88" s="37">
         <v>14</v>
       </c>
       <c r="AR88" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AS88" s="158" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="AT88" s="126"/>
       <c r="AV88" s="131"/>
     </row>
     <row r="89" spans="1:48" ht="56" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B89" s="123" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C89" s="38">
         <v>6607</v>
@@ -16539,13 +16681,13 @@
         <v>1276</v>
       </c>
       <c r="AL89" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AM89" s="39" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AN89" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO89" s="37">
         <v>1992</v>
@@ -16557,10 +16699,10 @@
         <v>54</v>
       </c>
       <c r="AR89" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AS89" s="158" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AT89" s="145"/>
       <c r="AU89" s="46"/>
@@ -16568,10 +16710,10 @@
     </row>
     <row r="90" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A90" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C90" s="38">
         <v>2106</v>
@@ -16682,28 +16824,28 @@
         <v>1251</v>
       </c>
       <c r="AL90" s="39" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="AM90" s="39" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="AN90" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AO90" s="37">
         <v>1977</v>
       </c>
       <c r="AP90" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AQ90" s="37">
         <v>14</v>
       </c>
       <c r="AR90" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AS90" s="158" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="AT90" s="141"/>
       <c r="AU90" s="32"/>
@@ -16711,10 +16853,10 @@
     </row>
     <row r="91" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A91" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B91" s="123" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C91" s="38">
         <v>2108</v>
@@ -16825,38 +16967,38 @@
         <v>1249</v>
       </c>
       <c r="AL91" s="39" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="AM91" s="39" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="AN91" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AO91" s="37">
         <v>1977</v>
       </c>
       <c r="AP91" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AQ91" s="37">
         <v>14</v>
       </c>
       <c r="AR91" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AS91" s="158" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="AT91" s="126"/>
       <c r="AV91" s="131"/>
     </row>
     <row r="92" spans="1:48" ht="42" x14ac:dyDescent="0.2">
       <c r="A92" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B92" s="123" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C92" s="38">
         <v>2132</v>
@@ -16967,38 +17109,38 @@
         <v>1189</v>
       </c>
       <c r="AL92" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="AM92" s="39" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="AN92" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO92" s="37">
         <v>1977</v>
       </c>
       <c r="AP92" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="AQ92" s="37">
         <v>26</v>
       </c>
       <c r="AR92" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="AS92" s="158" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="AT92" s="126"/>
       <c r="AV92" s="131"/>
     </row>
     <row r="93" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B93" s="123" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C93" s="38">
         <v>2133</v>
@@ -17109,38 +17251,38 @@
         <v>1189</v>
       </c>
       <c r="AL93" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="AM93" s="39" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="AN93" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO93" s="37">
         <v>1977</v>
       </c>
       <c r="AP93" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="AQ93" s="37">
         <v>26</v>
       </c>
       <c r="AR93" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="AS93" s="158" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="AT93" s="141"/>
       <c r="AU93" s="32"/>
     </row>
     <row r="94" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B94" s="123" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C94" s="38">
         <v>6610</v>
@@ -17251,13 +17393,13 @@
         <v>1165</v>
       </c>
       <c r="AL94" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="AM94" s="39" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="AN94" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO94" s="37">
         <v>1992</v>
@@ -17269,20 +17411,20 @@
         <v>54</v>
       </c>
       <c r="AR94" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AS94" s="158" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AT94" s="141"/>
       <c r="AU94" s="32"/>
     </row>
     <row r="95" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B95" s="123" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C95" s="38">
         <v>2131</v>
@@ -17393,37 +17535,37 @@
         <v>1165</v>
       </c>
       <c r="AL95" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="AM95" s="39" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="AN95" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO95" s="37">
         <v>1977</v>
       </c>
       <c r="AP95" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="AQ95" s="37">
         <v>26</v>
       </c>
       <c r="AR95" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="AS95" s="158" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="AT95" s="126"/>
     </row>
     <row r="96" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B96" s="123" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C96" s="38">
         <v>6609</v>
@@ -17534,13 +17676,13 @@
         <v>1165</v>
       </c>
       <c r="AL96" s="39" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AM96" s="39" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="AN96" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AO96" s="37">
         <v>1992</v>
@@ -17552,19 +17694,19 @@
         <v>54</v>
       </c>
       <c r="AR96" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AS96" s="158" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AT96" s="126"/>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="28" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B97" s="123" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C97" s="38">
         <v>3222</v>
@@ -17675,47 +17817,47 @@
         <v>2054</v>
       </c>
       <c r="AL97" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AM97" s="39" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AN97" s="16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AO97" s="37">
         <v>1976</v>
       </c>
       <c r="AP97" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AQ97" s="37"/>
       <c r="AR97" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="AS97" s="158" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AT97" s="141" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="AU97" s="46"/>
     </row>
     <row r="98" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="B98" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="E98" s="26" t="s">
         <v>385</v>
-      </c>
-      <c r="B98" s="122" t="s">
-        <v>386</v>
-      </c>
-      <c r="C98" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="E98" s="26" t="s">
-        <v>389</v>
       </c>
       <c r="F98" s="27">
         <v>100</v>
@@ -17821,10 +17963,10 @@
         <v>1269</v>
       </c>
       <c r="AL98" s="26" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="AM98" s="44" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AN98" s="16" t="s">
         <v>49</v>
@@ -17837,25 +17979,27 @@
       <c r="AR98" s="16"/>
       <c r="AS98" s="158"/>
       <c r="AT98" s="141" t="s">
-        <v>391</v>
-      </c>
-      <c r="AU98" s="32"/>
+        <v>387</v>
+      </c>
+      <c r="AU98" s="28" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="99" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="B99" s="122" t="s">
+        <v>388</v>
+      </c>
+      <c r="C99" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="E99" s="26" t="s">
         <v>385</v>
-      </c>
-      <c r="B99" s="122" t="s">
-        <v>392</v>
-      </c>
-      <c r="C99" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="E99" s="26" t="s">
-        <v>389</v>
       </c>
       <c r="F99" s="27">
         <v>100</v>
@@ -17962,7 +18106,7 @@
       </c>
       <c r="AL99" s="26"/>
       <c r="AM99" s="44" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="AN99" s="16" t="s">
         <v>49</v>
@@ -17975,23 +18119,25 @@
       <c r="AR99" s="16"/>
       <c r="AS99" s="158"/>
       <c r="AT99" s="141" t="s">
-        <v>394</v>
-      </c>
-      <c r="AU99" s="32"/>
+        <v>390</v>
+      </c>
+      <c r="AU99" s="28" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="100" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="33" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B100" s="117" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C100" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D100" s="69"/>
       <c r="E100" s="69" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="F100" s="68">
         <v>100</v>
@@ -18100,46 +18246,48 @@
         <v>850</v>
       </c>
       <c r="AL100" s="77" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="AM100" s="78" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="AN100" s="78" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="AO100" s="66">
         <v>2006</v>
       </c>
       <c r="AP100" s="78" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="AQ100" s="66">
         <v>118</v>
       </c>
       <c r="AR100" s="79" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="AS100" s="148" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="AT100" s="141"/>
-      <c r="AU100" s="108"/>
+      <c r="AU100" s="160" t="s">
+        <v>636</v>
+      </c>
       <c r="AV100" s="95"/>
     </row>
     <row r="101" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="33" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B101" s="117" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D101" s="69"/>
       <c r="E101" s="69" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="F101" s="68">
         <v>100</v>
@@ -18248,46 +18396,48 @@
         <v>811</v>
       </c>
       <c r="AL101" s="77" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="AM101" s="78" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="AN101" s="78" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="AO101" s="66">
         <v>2006</v>
       </c>
       <c r="AP101" s="78" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="AQ101" s="66">
         <v>118</v>
       </c>
       <c r="AR101" s="79" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="AS101" s="148" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="AT101" s="126"/>
-      <c r="AU101" s="93"/>
+      <c r="AU101" s="160" t="s">
+        <v>636</v>
+      </c>
       <c r="AV101" s="95"/>
     </row>
     <row r="102" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="33" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B102" s="117" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C102" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D102" s="69"/>
       <c r="E102" s="69" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F102" s="68">
         <v>100</v>
@@ -18396,31 +18546,33 @@
         <v>789</v>
       </c>
       <c r="AL102" s="77" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="AM102" s="78" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="AN102" s="78" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="AO102" s="66">
         <v>2006</v>
       </c>
       <c r="AP102" s="78" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="AQ102" s="66">
         <v>118</v>
       </c>
       <c r="AR102" s="79" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="AS102" s="148" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="AT102" s="141"/>
-      <c r="AU102" s="108"/>
+      <c r="AU102" s="160" t="s">
+        <v>636</v>
+      </c>
       <c r="AV102" s="95"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update names to make more consistent
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81913D17-F499-6844-8FAD-9AC4A8248774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748350E7-E04E-274E-989C-842B35E391A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="27820" windowHeight="16340" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1620" windowWidth="27820" windowHeight="16340" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,8 @@
     <definedName name="fenno98_4" localSheetId="0">'Leirubakki-all'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Leirubakki-all'!$AI$1:$AR$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="681">
   <si>
     <t>abs(I)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1460,9 +1454,6 @@
   </si>
   <si>
     <t>Overlaps with Cenozoic</t>
-  </si>
-  <si>
-    <t>PTARMIGAN MEAN</t>
   </si>
   <si>
     <t xml:space="preserve">2505±2, </t>
@@ -1921,15 +1912,6 @@
     <t>\citep{Murthy1978a}</t>
   </si>
   <si>
-    <t>Biscotasing</t>
-  </si>
-  <si>
-    <t>Nipissing N1</t>
-  </si>
-  <si>
-    <t>Senneterre</t>
-  </si>
-  <si>
     <t>\cite{Swanson-Hysell2014a}</t>
   </si>
   <si>
@@ -2032,15 +2014,6 @@
     <t>Mean Kahochella, Peacock Hills</t>
   </si>
   <si>
-    <t>Mean Pearson A/Peninsular sill/Kilohigok basin sill</t>
-  </si>
-  <si>
-    <t>Mean Rocky Mountain intrusions</t>
-  </si>
-  <si>
-    <t>Mean Nipigon sills and lavas</t>
-  </si>
-  <si>
     <t>Torridon Group</t>
   </si>
   <si>
@@ -2108,6 +2081,78 @@
   </si>
   <si>
     <t>\cite{Abrahamsen1987a}</t>
+  </si>
+  <si>
+    <t>Matachewan dykes R</t>
+  </si>
+  <si>
+    <t>Matachewan dykes N</t>
+  </si>
+  <si>
+    <t>Senneterre dykes</t>
+  </si>
+  <si>
+    <t>Otto Stock dykes and aureole</t>
+  </si>
+  <si>
+    <t>Nipissing N1 sills</t>
+  </si>
+  <si>
+    <t>Biscotasing dykes</t>
+  </si>
+  <si>
+    <t>Lac Esprit dykes</t>
+  </si>
+  <si>
+    <t>Minto dykes</t>
+  </si>
+  <si>
+    <t>Marathon dykes N</t>
+  </si>
+  <si>
+    <t>Marathon dykes R</t>
+  </si>
+  <si>
+    <t>Fort Frances dykes</t>
+  </si>
+  <si>
+    <t>Molson (B+C2) dykes</t>
+  </si>
+  <si>
+    <t>Ptarmigan-Mistassini dykes</t>
+  </si>
+  <si>
+    <t>Cauchon Lake dykes</t>
+  </si>
+  <si>
+    <t>Rifle Formation</t>
+  </si>
+  <si>
+    <t>Pearson A/Peninsular/Kilohigok sills</t>
+  </si>
+  <si>
+    <t>Michikamau Intrusion</t>
+  </si>
+  <si>
+    <t>Tobacco Root dykes</t>
+  </si>
+  <si>
+    <t>Rocky Mountain intrusions</t>
+  </si>
+  <si>
+    <t>Nipigon sills and lavas</t>
+  </si>
+  <si>
+    <t>Tsezotene Sills</t>
+  </si>
+  <si>
+    <t>Sept-Iles layered intrusion</t>
+  </si>
+  <si>
+    <t>North Qoroq intrusives</t>
+  </si>
+  <si>
+    <t>NE-SW Trending dykes</t>
   </si>
 </sst>
 </file>
@@ -3555,10 +3600,10 @@
   <dimension ref="A1:AW103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AM90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU87" sqref="AU87"/>
+      <selection pane="bottomRight" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3723,7 +3768,7 @@
         <v>31</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AO1" s="19" t="s">
         <v>24</v>
@@ -3741,16 +3786,16 @@
         <v>22</v>
       </c>
       <c r="AT1" s="140" t="s">
+        <v>554</v>
+      </c>
+      <c r="AU1" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AV1" s="18" t="s">
         <v>556</v>
       </c>
-      <c r="AV1" s="18" t="s">
-        <v>557</v>
-      </c>
       <c r="AW1" s="24" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="2" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -3758,7 +3803,7 @@
         <v>447</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>448</v>
+        <v>660</v>
       </c>
       <c r="C2" s="38">
         <v>2629</v>
@@ -3903,7 +3948,7 @@
         <v>457</v>
       </c>
       <c r="AU2" s="160" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:49" s="105" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -3911,7 +3956,7 @@
         <v>447</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>458</v>
+        <v>669</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>66</v>
@@ -4024,13 +4069,13 @@
         <v>2507</v>
       </c>
       <c r="AL3" s="79" t="s">
+        <v>458</v>
+      </c>
+      <c r="AM3" s="67" t="s">
         <v>459</v>
       </c>
-      <c r="AM3" s="67" t="s">
+      <c r="AN3" s="78" t="s">
         <v>460</v>
-      </c>
-      <c r="AN3" s="78" t="s">
-        <v>461</v>
       </c>
       <c r="AO3" s="66">
         <v>2010</v>
@@ -4042,14 +4087,14 @@
         <v>183</v>
       </c>
       <c r="AR3" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS3" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS3" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT3" s="126"/>
       <c r="AU3" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4057,7 +4102,7 @@
         <v>447</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>464</v>
+        <v>657</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>66</v>
@@ -4170,13 +4215,13 @@
         <v>2489</v>
       </c>
       <c r="AL4" s="79" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AM4" s="67" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AN4" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO4" s="66">
         <v>2010</v>
@@ -4188,14 +4233,14 @@
         <v>183</v>
       </c>
       <c r="AR4" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS4" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS4" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT4" s="141"/>
       <c r="AU4" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4203,7 +4248,7 @@
         <v>447</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>466</v>
+        <v>658</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>66</v>
@@ -4316,13 +4361,13 @@
         <v>2449</v>
       </c>
       <c r="AL5" s="79" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AM5" s="67" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AN5" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO5" s="66">
         <v>2010</v>
@@ -4334,14 +4379,14 @@
         <v>183</v>
       </c>
       <c r="AR5" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS5" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS5" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT5" s="126"/>
       <c r="AU5" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="6" spans="1:49" s="108" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -4349,10 +4394,10 @@
         <v>447</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>603</v>
+        <v>659</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D6" s="69"/>
       <c r="E6" s="69" t="s">
@@ -4464,10 +4509,10 @@
         <v>2224</v>
       </c>
       <c r="AL6" s="79" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AM6" s="67" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AN6" s="78" t="s">
         <v>151</v>
@@ -4482,17 +4527,17 @@
         <v>30</v>
       </c>
       <c r="AR6" s="79" t="s">
+        <v>470</v>
+      </c>
+      <c r="AS6" s="152" t="s">
         <v>471</v>
-      </c>
-      <c r="AS6" s="152" t="s">
-        <v>472</v>
       </c>
       <c r="AT6" s="141"/>
       <c r="AU6" s="160" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AW6" s="160" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="7" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -4500,7 +4545,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>602</v>
+        <v>661</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>146</v>
@@ -4613,10 +4658,10 @@
         <v>2221</v>
       </c>
       <c r="AL7" s="79" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AM7" s="67" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AN7" s="78" t="s">
         <v>151</v>
@@ -4638,7 +4683,7 @@
       </c>
       <c r="AT7" s="141"/>
       <c r="AU7" s="160" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4646,7 +4691,7 @@
         <v>447</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>601</v>
+        <v>662</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
@@ -4761,13 +4806,13 @@
         <v>2172</v>
       </c>
       <c r="AL8" s="79" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AM8" s="67" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AN8" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO8" s="66">
         <v>2010</v>
@@ -4779,14 +4824,14 @@
         <v>183</v>
       </c>
       <c r="AR8" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS8" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS8" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT8" s="141"/>
       <c r="AU8" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4794,7 +4839,7 @@
         <v>447</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>477</v>
+        <v>663</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>66</v>
@@ -4907,13 +4952,13 @@
         <v>2070</v>
       </c>
       <c r="AL9" s="79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AM9" s="67" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AN9" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO9" s="66">
         <v>2010</v>
@@ -4925,16 +4970,16 @@
         <v>183</v>
       </c>
       <c r="AR9" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS9" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS9" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT9" s="141" t="s">
         <v>457</v>
       </c>
       <c r="AU9" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4942,7 +4987,7 @@
         <v>447</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>479</v>
+        <v>664</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>66</v>
@@ -5055,13 +5100,13 @@
         <v>2000</v>
       </c>
       <c r="AL10" s="79" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AM10" s="67" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AN10" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO10" s="66">
         <v>2010</v>
@@ -5073,27 +5118,27 @@
         <v>183</v>
       </c>
       <c r="AR10" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS10" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS10" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT10" s="126" t="s">
         <v>386</v>
       </c>
       <c r="AU10" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="47" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B11" s="109" t="s">
+        <v>665</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>482</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>483</v>
       </c>
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
@@ -5201,13 +5246,13 @@
         <v>2126</v>
       </c>
       <c r="AL11" s="79" t="s">
+        <v>483</v>
+      </c>
+      <c r="AM11" s="67" t="s">
+        <v>481</v>
+      </c>
+      <c r="AN11" s="78" t="s">
         <v>484</v>
-      </c>
-      <c r="AM11" s="67" t="s">
-        <v>482</v>
-      </c>
-      <c r="AN11" s="78" t="s">
-        <v>485</v>
       </c>
       <c r="AO11" s="66">
         <v>2008</v>
@@ -5219,27 +5264,27 @@
         <v>162</v>
       </c>
       <c r="AR11" s="79" t="s">
+        <v>485</v>
+      </c>
+      <c r="AS11" s="147" t="s">
         <v>486</v>
-      </c>
-      <c r="AS11" s="147" t="s">
-        <v>487</v>
       </c>
       <c r="AT11" s="126" t="s">
         <v>386</v>
       </c>
       <c r="AU11" s="161" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:49" s="33" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="47" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>488</v>
+        <v>666</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D12" s="69"/>
       <c r="E12" s="69" t="s">
@@ -5349,13 +5394,13 @@
         <v>2106</v>
       </c>
       <c r="AL12" s="79" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AM12" s="67" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AN12" s="78" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AO12" s="66">
         <v>2008</v>
@@ -5367,24 +5412,24 @@
         <v>162</v>
       </c>
       <c r="AR12" s="79" t="s">
+        <v>485</v>
+      </c>
+      <c r="AS12" s="147" t="s">
         <v>486</v>
       </c>
-      <c r="AS12" s="147" t="s">
-        <v>487</v>
-      </c>
       <c r="AT12" s="126" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AU12" s="161" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="47" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B13" s="109" t="s">
-        <v>491</v>
+        <v>670</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>66</v>
@@ -5497,13 +5542,13 @@
         <v>2093</v>
       </c>
       <c r="AL13" s="79" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AM13" s="67" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AN13" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO13" s="66">
         <v>2010</v>
@@ -5515,24 +5560,24 @@
         <v>183</v>
       </c>
       <c r="AR13" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS13" s="147" t="s">
         <v>462</v>
       </c>
-      <c r="AS13" s="147" t="s">
-        <v>463</v>
-      </c>
       <c r="AT13" s="126" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AU13" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="47" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>493</v>
+        <v>667</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>66</v>
@@ -5643,13 +5688,13 @@
         <v>2081</v>
       </c>
       <c r="AL14" s="79" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AM14" s="67" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AN14" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO14" s="66">
         <v>2010</v>
@@ -5661,24 +5706,24 @@
         <v>183</v>
       </c>
       <c r="AR14" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS14" s="147" t="s">
         <v>462</v>
-      </c>
-      <c r="AS14" s="147" t="s">
-        <v>463</v>
       </c>
       <c r="AT14" s="126" t="s">
         <v>386</v>
       </c>
       <c r="AU14" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:49" s="94" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>495</v>
+        <v>668</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5791,13 +5836,13 @@
         <v>1884</v>
       </c>
       <c r="AL15" s="79" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AM15" s="78" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AN15" s="78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AO15" s="66">
         <v>2010</v>
@@ -5809,14 +5854,14 @@
         <v>183</v>
       </c>
       <c r="AR15" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="AS15" s="148" t="s">
         <v>462</v>
-      </c>
-      <c r="AS15" s="148" t="s">
-        <v>463</v>
       </c>
       <c r="AT15" s="126"/>
       <c r="AU15" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="1:49" s="94" customFormat="1" x14ac:dyDescent="0.15">
@@ -5824,7 +5869,7 @@
         <v>443</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
@@ -5959,15 +6004,15 @@
       <c r="AS16" s="149"/>
       <c r="AT16" s="126"/>
       <c r="AU16" s="31" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B17" s="112" t="s">
         <v>530</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>531</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>121</v>
@@ -6079,49 +6124,49 @@
         <v>2709</v>
       </c>
       <c r="AL17" s="87" t="s">
+        <v>531</v>
+      </c>
+      <c r="AM17" s="77" t="s">
+        <v>530</v>
+      </c>
+      <c r="AN17" s="93" t="s">
         <v>532</v>
-      </c>
-      <c r="AM17" s="77" t="s">
-        <v>531</v>
-      </c>
-      <c r="AN17" s="93" t="s">
-        <v>533</v>
       </c>
       <c r="AO17" s="66">
         <v>2008</v>
       </c>
       <c r="AP17" s="93" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AQ17" s="65">
         <v>9</v>
       </c>
       <c r="AR17" s="97" t="s">
+        <v>534</v>
+      </c>
+      <c r="AS17" s="150" t="s">
         <v>535</v>
       </c>
-      <c r="AS17" s="150" t="s">
+      <c r="AT17" s="142" t="s">
         <v>536</v>
       </c>
-      <c r="AT17" s="142" t="s">
-        <v>537</v>
-      </c>
       <c r="AU17" s="162" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="18" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="100" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C18" s="59" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="62"/>
       <c r="E18" s="134" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F18" s="59">
         <v>100</v>
@@ -6171,7 +6216,7 @@
         <v>7.6</v>
       </c>
       <c r="U18" s="137" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V18" s="59">
         <v>4</v>
@@ -6228,40 +6273,40 @@
         <v>2171</v>
       </c>
       <c r="AL18" s="125" t="s">
+        <v>540</v>
+      </c>
+      <c r="AM18" s="125" t="s">
+        <v>537</v>
+      </c>
+      <c r="AN18" s="126" t="s">
         <v>541</v>
-      </c>
-      <c r="AM18" s="125" t="s">
-        <v>538</v>
-      </c>
-      <c r="AN18" s="126" t="s">
-        <v>542</v>
       </c>
       <c r="AO18" s="2">
         <v>2015</v>
       </c>
       <c r="AP18" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="AQ18" s="59">
         <v>424</v>
       </c>
       <c r="AR18" s="127" t="s">
+        <v>543</v>
+      </c>
+      <c r="AS18" s="126" t="s">
         <v>544</v>
-      </c>
-      <c r="AS18" s="126" t="s">
-        <v>545</v>
       </c>
       <c r="AT18" s="142"/>
       <c r="AU18" s="90" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:49" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="100" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B19" s="120" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>34</v>
@@ -6317,7 +6362,7 @@
         <v>8.1</v>
       </c>
       <c r="U19" s="135" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="V19" s="64">
         <v>4</v>
@@ -6375,16 +6420,16 @@
         <v>1904</v>
       </c>
       <c r="AL19" s="125" t="s">
+        <v>547</v>
+      </c>
+      <c r="AM19" s="100" t="s">
+        <v>545</v>
+      </c>
+      <c r="AN19" s="129" t="s">
         <v>548</v>
       </c>
-      <c r="AM19" s="100" t="s">
-        <v>546</v>
-      </c>
-      <c r="AN19" s="129" t="s">
+      <c r="AO19" s="130" t="s">
         <v>549</v>
-      </c>
-      <c r="AO19" s="130" t="s">
-        <v>550</v>
       </c>
       <c r="AP19" s="60" t="s">
         <v>179</v>
@@ -6393,31 +6438,31 @@
         <v>44</v>
       </c>
       <c r="AR19" s="61" t="s">
+        <v>550</v>
+      </c>
+      <c r="AS19" s="151" t="s">
         <v>551</v>
       </c>
-      <c r="AS19" s="151" t="s">
+      <c r="AT19" s="142" t="s">
         <v>552</v>
       </c>
-      <c r="AT19" s="142" t="s">
-        <v>553</v>
-      </c>
       <c r="AU19" s="90" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:49" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="B20" s="117" t="s">
         <v>511</v>
-      </c>
-      <c r="B20" s="117" t="s">
-        <v>512</v>
       </c>
       <c r="C20" s="8">
         <v>8359</v>
       </c>
       <c r="D20" s="79"/>
       <c r="E20" s="79" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F20" s="66">
         <v>0</v>
@@ -6529,37 +6574,37 @@
         <v>64</v>
       </c>
       <c r="AM20" s="78" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AN20" s="78" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AO20" s="66">
         <v>1999</v>
       </c>
       <c r="AP20" s="78" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AQ20" s="66" t="s">
         <v>108</v>
       </c>
       <c r="AR20" s="79" t="s">
+        <v>515</v>
+      </c>
+      <c r="AS20" s="148" t="s">
         <v>516</v>
-      </c>
-      <c r="AS20" s="148" t="s">
-        <v>517</v>
       </c>
       <c r="AT20" s="126"/>
       <c r="AU20" s="161" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="21" spans="1:49" ht="56" x14ac:dyDescent="0.15">
       <c r="A21" s="47" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B21" s="109" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C21" s="38">
         <v>8889</v>
@@ -6676,46 +6721,46 @@
         <v>64</v>
       </c>
       <c r="AM21" s="67" t="s">
+        <v>517</v>
+      </c>
+      <c r="AN21" s="78" t="s">
         <v>518</v>
-      </c>
-      <c r="AN21" s="78" t="s">
-        <v>519</v>
       </c>
       <c r="AO21" s="66">
         <v>2000</v>
       </c>
       <c r="AP21" s="78" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AQ21" s="66" t="s">
         <v>60</v>
       </c>
       <c r="AR21" s="79" t="s">
+        <v>520</v>
+      </c>
+      <c r="AS21" s="152" t="s">
         <v>521</v>
-      </c>
-      <c r="AS21" s="152" t="s">
-        <v>522</v>
       </c>
       <c r="AT21" s="141"/>
       <c r="AU21" s="160" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AV21" s="31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="22" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="47" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B22" s="109" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="69" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="68">
@@ -6825,36 +6870,36 @@
         <v>1759</v>
       </c>
       <c r="AL22" s="163" t="s">
+        <v>524</v>
+      </c>
+      <c r="AM22" s="67" t="s">
+        <v>522</v>
+      </c>
+      <c r="AN22" s="78" t="s">
         <v>525</v>
-      </c>
-      <c r="AM22" s="67" t="s">
-        <v>523</v>
-      </c>
-      <c r="AN22" s="78" t="s">
-        <v>526</v>
       </c>
       <c r="AO22" s="66">
         <v>1995</v>
       </c>
       <c r="AP22" s="78" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AQ22" s="66"/>
       <c r="AR22" s="79" t="s">
+        <v>527</v>
+      </c>
+      <c r="AS22" s="152" t="s">
         <v>528</v>
-      </c>
-      <c r="AS22" s="152" t="s">
-        <v>529</v>
       </c>
       <c r="AT22" s="142"/>
       <c r="AU22" s="162" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AV22" s="33" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AW22" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="1:49" s="33" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -7003,10 +7048,10 @@
       </c>
       <c r="AT23" s="126"/>
       <c r="AU23" s="31" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AV23" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="42" x14ac:dyDescent="0.15">
@@ -7157,7 +7202,7 @@
         <v>373</v>
       </c>
       <c r="AU24" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="25" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7308,7 +7353,7 @@
         <v>373</v>
       </c>
       <c r="AU25" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7456,10 +7501,10 @@
       </c>
       <c r="AT26" s="141"/>
       <c r="AU26" s="32" t="s">
+        <v>577</v>
+      </c>
+      <c r="AV26" s="32" t="s">
         <v>578</v>
-      </c>
-      <c r="AV26" s="32" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="27" spans="1:49" s="28" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -7609,10 +7654,10 @@
         <v>401</v>
       </c>
       <c r="AU27" s="28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AV27" s="31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7760,10 +7805,10 @@
       </c>
       <c r="AT28" s="141"/>
       <c r="AU28" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AV28" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="98" x14ac:dyDescent="0.15">
@@ -7908,10 +7953,10 @@
       </c>
       <c r="AT29" s="141"/>
       <c r="AU29" s="105" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AV29" s="31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="30" spans="1:49" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -8060,10 +8105,10 @@
       </c>
       <c r="AT30" s="141"/>
       <c r="AU30" s="32" t="s">
+        <v>579</v>
+      </c>
+      <c r="AV30" s="32" t="s">
         <v>580</v>
-      </c>
-      <c r="AV30" s="32" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:49" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -8071,7 +8116,7 @@
         <v>390</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>418</v>
+        <v>671</v>
       </c>
       <c r="C31" s="38">
         <v>5915</v>
@@ -8210,7 +8255,7 @@
       </c>
       <c r="AT31" s="141"/>
       <c r="AU31" s="108" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="32" spans="1:49" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -8359,7 +8404,7 @@
         <v>427</v>
       </c>
       <c r="AU32" s="105" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -8367,7 +8412,7 @@
         <v>390</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -8508,7 +8553,7 @@
       </c>
       <c r="AT33" s="126"/>
       <c r="AU33" s="93" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="34" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -8516,7 +8561,7 @@
         <v>390</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -8655,7 +8700,7 @@
       </c>
       <c r="AT34" s="126"/>
       <c r="AU34" s="93" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="35" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -8806,7 +8851,7 @@
       </c>
       <c r="AT35" s="126"/>
       <c r="AU35" s="93" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -8955,7 +9000,7 @@
       </c>
       <c r="AT36" s="126"/>
       <c r="AU36" s="93" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -8963,7 +9008,7 @@
         <v>390</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -9102,7 +9147,7 @@
       </c>
       <c r="AT37" s="126"/>
       <c r="AU37" s="93" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="38" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9253,7 +9298,7 @@
         <v>82</v>
       </c>
       <c r="AU38" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -9402,7 +9447,7 @@
       </c>
       <c r="AT39" s="143"/>
       <c r="AU39" s="33" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9551,7 +9596,7 @@
       </c>
       <c r="AT40" s="126"/>
       <c r="AU40" s="31" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
@@ -9700,10 +9745,10 @@
       </c>
       <c r="AT41" s="143"/>
       <c r="AU41" s="33" t="s">
+        <v>587</v>
+      </c>
+      <c r="AV41" s="142" t="s">
         <v>588</v>
-      </c>
-      <c r="AV41" s="142" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="42" spans="1:48" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9711,7 +9756,7 @@
         <v>74</v>
       </c>
       <c r="B42" s="109" t="s">
-        <v>105</v>
+        <v>673</v>
       </c>
       <c r="C42" s="38">
         <v>2274</v>
@@ -9854,7 +9899,7 @@
       </c>
       <c r="AT42" s="126"/>
       <c r="AU42" s="31" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10005,7 +10050,7 @@
       </c>
       <c r="AT43" s="143"/>
       <c r="AU43" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10156,7 +10201,7 @@
       </c>
       <c r="AT44" s="143"/>
       <c r="AU44" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -10164,7 +10209,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>120</v>
+        <v>674</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>121</v>
@@ -10309,7 +10354,7 @@
         <v>127</v>
       </c>
       <c r="AU45" s="33" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10460,7 +10505,7 @@
       </c>
       <c r="AT46" s="143"/>
       <c r="AU46" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
@@ -10468,13 +10513,13 @@
         <v>74</v>
       </c>
       <c r="B47" s="113" t="s">
-        <v>639</v>
+        <v>675</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>61</v>
@@ -10603,7 +10648,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
       <c r="AU47" s="31" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
     </row>
     <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -10752,7 +10797,7 @@
       </c>
       <c r="AT48" s="126"/>
       <c r="AU48" s="31" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="49" spans="1:49" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10901,7 +10946,7 @@
       </c>
       <c r="AT49" s="126"/>
       <c r="AU49" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="50" spans="1:49" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -11050,7 +11095,7 @@
       </c>
       <c r="AT50" s="126"/>
       <c r="AU50" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="51" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11199,7 +11244,7 @@
       </c>
       <c r="AT51" s="143"/>
       <c r="AU51" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="52" spans="1:49" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -11350,7 +11395,7 @@
       </c>
       <c r="AT52" s="143"/>
       <c r="AU52" s="33" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="53" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11501,7 +11546,7 @@
       </c>
       <c r="AT53" s="126"/>
       <c r="AU53" s="31" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11509,14 +11554,14 @@
         <v>74</v>
       </c>
       <c r="B54" s="109" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="39" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="F54" s="38">
         <v>0</v>
@@ -11623,13 +11668,13 @@
         <v>1153</v>
       </c>
       <c r="AL54" s="41" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="AM54" s="109" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="AN54" s="25" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="AO54" s="8">
         <v>2018</v>
@@ -11640,10 +11685,10 @@
       <c r="AS54" s="157"/>
       <c r="AT54" s="126"/>
       <c r="AU54" s="31" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="AW54" s="32" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
     </row>
     <row r="55" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11792,7 +11837,7 @@
       </c>
       <c r="AT55" s="142"/>
       <c r="AU55" s="28" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="56" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11800,13 +11845,13 @@
         <v>74</v>
       </c>
       <c r="B56" s="113" t="s">
-        <v>640</v>
+        <v>676</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="E56" s="39" t="s">
         <v>168</v>
@@ -11934,7 +11979,7 @@
       <c r="AS56" s="158"/>
       <c r="AT56" s="142"/>
       <c r="AU56" s="28" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
     </row>
     <row r="57" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12080,7 +12125,7 @@
       <c r="AS57" s="157"/>
       <c r="AT57" s="142"/>
       <c r="AU57" s="28" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="58" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12225,7 +12270,7 @@
       <c r="AS58" s="157"/>
       <c r="AT58" s="142"/>
       <c r="AU58" s="28" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="59" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12371,7 +12416,7 @@
       <c r="AS59" s="157"/>
       <c r="AT59" s="126"/>
       <c r="AU59" s="28" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.15">
@@ -12495,28 +12540,28 @@
         <v>1106</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="AM60" s="33" t="s">
         <v>187</v>
       </c>
       <c r="AN60" s="3" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="AO60" s="4">
         <v>2019</v>
       </c>
       <c r="AP60" s="3" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="AQ60" s="34"/>
       <c r="AR60" s="35"/>
       <c r="AT60" s="142"/>
       <c r="AU60" s="28" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="AW60" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="61" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -12661,7 +12706,7 @@
       <c r="AS61" s="157"/>
       <c r="AT61" s="142"/>
       <c r="AU61" s="28" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="62" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12808,7 +12853,7 @@
       <c r="AS62" s="157"/>
       <c r="AT62" s="126"/>
       <c r="AU62" s="28" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.15">
@@ -12952,10 +12997,10 @@
       </c>
       <c r="AT63" s="126"/>
       <c r="AU63" s="28" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="AW63" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.15">
@@ -13101,10 +13146,10 @@
       </c>
       <c r="AT64" s="126"/>
       <c r="AU64" s="31" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="AW64" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -13253,7 +13298,7 @@
       </c>
       <c r="AT65" s="142"/>
       <c r="AU65" s="28" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="66" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -13399,10 +13444,10 @@
       <c r="AS66" s="157"/>
       <c r="AT66" s="142"/>
       <c r="AU66" s="28" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="AW66" s="32" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="67" spans="1:49" ht="56" x14ac:dyDescent="0.15">
@@ -13551,7 +13596,7 @@
       </c>
       <c r="AT67" s="126"/>
       <c r="AU67" s="31" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.15">
@@ -13694,7 +13739,7 @@
       <c r="AR68" s="35"/>
       <c r="AT68" s="142"/>
       <c r="AU68" s="28" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="69" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -13819,7 +13864,7 @@
         <v>1087</v>
       </c>
       <c r="AL69" s="41" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="AM69" s="25" t="s">
         <v>224</v>
@@ -13843,7 +13888,7 @@
       <c r="AT69" s="142"/>
       <c r="AU69" s="28"/>
       <c r="AW69" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="70" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -13987,7 +14032,7 @@
       </c>
       <c r="AT70" s="142"/>
       <c r="AU70" s="90" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="71" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14131,7 +14176,7 @@
       </c>
       <c r="AT71" s="142"/>
       <c r="AU71" s="90" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="72" spans="1:49" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -14279,10 +14324,10 @@
       </c>
       <c r="AT72" s="142"/>
       <c r="AU72" s="162" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AW72" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="73" spans="1:49" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -14434,10 +14479,10 @@
         <v>245</v>
       </c>
       <c r="AU73" s="162" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AW73" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="74" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -14588,7 +14633,7 @@
         <v>251</v>
       </c>
       <c r="AU74" s="161" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="75" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14596,7 +14641,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>252</v>
+        <v>677</v>
       </c>
       <c r="C75" s="38">
         <v>5922</v>
@@ -14739,7 +14784,7 @@
       </c>
       <c r="AT75" s="142"/>
       <c r="AU75" s="28" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AV75" s="131"/>
     </row>
@@ -14748,7 +14793,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="122" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="C76" s="38" t="s">
         <v>66</v>
@@ -14882,7 +14927,7 @@
         <v>260</v>
       </c>
       <c r="AU76" s="28" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="AV76" s="131"/>
     </row>
@@ -15034,7 +15079,7 @@
         <v>245</v>
       </c>
       <c r="AU77" s="31" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AV77" s="131"/>
     </row>
@@ -15188,7 +15233,7 @@
         <v>245</v>
       </c>
       <c r="AU78" s="28" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AV78" s="131"/>
     </row>
@@ -15340,7 +15385,7 @@
       </c>
       <c r="AT79" s="142"/>
       <c r="AU79" s="28" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AV79" s="131"/>
     </row>
@@ -15490,7 +15535,7 @@
       </c>
       <c r="AT80" s="144"/>
       <c r="AU80" s="43" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="AV80" s="131"/>
     </row>
@@ -15642,7 +15687,7 @@
         <v>286</v>
       </c>
       <c r="AU81" s="43" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="AV81" s="131"/>
     </row>
@@ -15792,7 +15837,7 @@
       </c>
       <c r="AT82" s="141"/>
       <c r="AU82" s="32" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="AV82" s="131"/>
     </row>
@@ -15944,7 +15989,7 @@
       </c>
       <c r="AT83" s="141"/>
       <c r="AU83" s="32" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AV83" s="131"/>
     </row>
@@ -15953,7 +15998,7 @@
         <v>74</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>299</v>
+        <v>678</v>
       </c>
       <c r="C84" s="38">
         <v>1752</v>
@@ -16098,7 +16143,7 @@
         <v>286</v>
       </c>
       <c r="AU84" s="32" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AV84" s="131"/>
     </row>
@@ -16225,24 +16270,24 @@
         <v>307</v>
       </c>
       <c r="AN85" s="3" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="AO85" s="4">
         <v>2011</v>
       </c>
       <c r="AP85" s="164" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="AQ85" s="4"/>
       <c r="AR85" s="12"/>
       <c r="AS85" s="159"/>
       <c r="AT85" s="141"/>
       <c r="AU85" s="32" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="AV85" s="131"/>
       <c r="AW85" s="31" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="86" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -16388,7 +16433,7 @@
       </c>
       <c r="AT86" s="141"/>
       <c r="AU86" s="32" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="AV86" s="131"/>
     </row>
@@ -16534,7 +16579,7 @@
       </c>
       <c r="AT87" s="141"/>
       <c r="AU87" s="32" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="AV87" s="131"/>
     </row>
@@ -16679,7 +16724,7 @@
       </c>
       <c r="AT88" s="141"/>
       <c r="AU88" s="32" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="AV88" s="131"/>
     </row>
@@ -16824,7 +16869,7 @@
       </c>
       <c r="AT89" s="126"/>
       <c r="AU89" s="31" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="AV89" s="131"/>
     </row>
@@ -16833,7 +16878,7 @@
         <v>303</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>328</v>
+        <v>679</v>
       </c>
       <c r="C90" s="38">
         <v>6607</v>
@@ -16969,7 +17014,7 @@
       </c>
       <c r="AT90" s="145"/>
       <c r="AU90" s="32" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="AV90" s="131"/>
     </row>
@@ -17114,7 +17159,7 @@
       </c>
       <c r="AT91" s="141"/>
       <c r="AU91" s="31" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="AV91" s="131"/>
     </row>
@@ -17259,7 +17304,7 @@
       </c>
       <c r="AT92" s="126"/>
       <c r="AU92" s="31" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="AV92" s="131"/>
     </row>
@@ -17404,7 +17449,7 @@
       </c>
       <c r="AT93" s="126"/>
       <c r="AU93" s="31" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="AV93" s="131"/>
     </row>
@@ -17549,7 +17594,7 @@
       </c>
       <c r="AT94" s="141"/>
       <c r="AU94" s="31" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="95" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17693,7 +17738,7 @@
       </c>
       <c r="AT95" s="141"/>
       <c r="AU95" s="32" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="96" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17837,7 +17882,7 @@
       </c>
       <c r="AT96" s="126"/>
       <c r="AU96" s="31" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17845,7 +17890,7 @@
         <v>303</v>
       </c>
       <c r="B97" s="123" t="s">
-        <v>348</v>
+        <v>680</v>
       </c>
       <c r="C97" s="38">
         <v>6609</v>
@@ -17981,7 +18026,7 @@
       </c>
       <c r="AT97" s="126"/>
       <c r="AU97" s="32" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="98" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18125,7 +18170,7 @@
         <v>357</v>
       </c>
       <c r="AU98" s="32" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="99" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18133,7 +18178,7 @@
         <v>380</v>
       </c>
       <c r="B99" s="122" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>382</v>
@@ -18267,7 +18312,7 @@
         <v>386</v>
       </c>
       <c r="AU99" s="28" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="100" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18275,7 +18320,7 @@
         <v>380</v>
       </c>
       <c r="B100" s="122" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>382</v>
@@ -18407,22 +18452,22 @@
         <v>389</v>
       </c>
       <c r="AU100" s="28" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="B101" s="117" t="s">
         <v>497</v>
-      </c>
-      <c r="B101" s="117" t="s">
-        <v>498</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D101" s="69"/>
       <c r="E101" s="69" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F101" s="68">
         <v>100</v>
@@ -18531,48 +18576,48 @@
         <v>850</v>
       </c>
       <c r="AL101" s="77" t="s">
+        <v>499</v>
+      </c>
+      <c r="AM101" s="78" t="s">
+        <v>497</v>
+      </c>
+      <c r="AN101" s="78" t="s">
         <v>500</v>
-      </c>
-      <c r="AM101" s="78" t="s">
-        <v>498</v>
-      </c>
-      <c r="AN101" s="78" t="s">
-        <v>501</v>
       </c>
       <c r="AO101" s="66">
         <v>2006</v>
       </c>
       <c r="AP101" s="78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AQ101" s="66">
         <v>118</v>
       </c>
       <c r="AR101" s="79" t="s">
+        <v>502</v>
+      </c>
+      <c r="AS101" s="148" t="s">
         <v>503</v>
-      </c>
-      <c r="AS101" s="148" t="s">
-        <v>504</v>
       </c>
       <c r="AT101" s="141"/>
       <c r="AU101" s="160" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="AV101" s="95"/>
     </row>
     <row r="102" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B102" s="117" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C102" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D102" s="69"/>
       <c r="E102" s="69" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F102" s="68">
         <v>100</v>
@@ -18681,48 +18726,48 @@
         <v>811</v>
       </c>
       <c r="AL102" s="77" t="s">
+        <v>505</v>
+      </c>
+      <c r="AM102" s="78" t="s">
         <v>506</v>
       </c>
-      <c r="AM102" s="78" t="s">
-        <v>507</v>
-      </c>
       <c r="AN102" s="78" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AO102" s="66">
         <v>2006</v>
       </c>
       <c r="AP102" s="78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AQ102" s="66">
         <v>118</v>
       </c>
       <c r="AR102" s="79" t="s">
+        <v>502</v>
+      </c>
+      <c r="AS102" s="148" t="s">
         <v>503</v>
-      </c>
-      <c r="AS102" s="148" t="s">
-        <v>504</v>
       </c>
       <c r="AT102" s="126"/>
       <c r="AU102" s="160" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="AV102" s="95"/>
     </row>
     <row r="103" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B103" s="117" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C103" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D103" s="69"/>
       <c r="E103" s="69" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F103" s="68">
         <v>100</v>
@@ -18831,32 +18876,32 @@
         <v>789</v>
       </c>
       <c r="AL103" s="77" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AM103" s="78" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="AN103" s="78" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AO103" s="66">
         <v>2006</v>
       </c>
       <c r="AP103" s="78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AQ103" s="66">
         <v>118</v>
       </c>
       <c r="AR103" s="79" t="s">
+        <v>502</v>
+      </c>
+      <c r="AS103" s="148" t="s">
         <v>503</v>
-      </c>
-      <c r="AS103" s="148" t="s">
-        <v>504</v>
       </c>
       <c r="AT103" s="141"/>
       <c r="AU103" s="160" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="AV103" s="95"/>
     </row>

</xml_diff>

<commit_message>
clean up pole table
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748350E7-E04E-274E-989C-842B35E391A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF07483-A578-0648-8ABE-7415948F992F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1620" windowWidth="27820" windowHeight="16340" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="682">
   <si>
     <t>abs(I)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1882,9 +1882,6 @@
     <t>\cite{Evans1981a}</t>
   </si>
   <si>
-    <t>\citep{Irving1979a}</t>
-  </si>
-  <si>
     <t>\cite{Park1973}</t>
   </si>
   <si>
@@ -1897,9 +1894,6 @@
     <t>\cite{Emslie1976a}</t>
   </si>
   <si>
-    <t>\cite{Elston2002}</t>
-  </si>
-  <si>
     <t>\cite{Harlan2008a}</t>
   </si>
   <si>
@@ -1909,9 +1903,6 @@
     <t>\cite{Fahrig1976a}</t>
   </si>
   <si>
-    <t>\citep{Murthy1978a}</t>
-  </si>
-  <si>
     <t>\cite{Swanson-Hysell2014a}</t>
   </si>
   <si>
@@ -1942,9 +1933,6 @@
     <t>\cite{Books1972a, Hnat2006a} as calculated in \cite{Swanson-Hysell2019a}</t>
   </si>
   <si>
-    <t>\citep{Kean1997a}</t>
-  </si>
-  <si>
     <t>\cite{Tauxe2009a,Swanson-Hysell2019a}</t>
   </si>
   <si>
@@ -1981,9 +1969,6 @@
     <t>\cite{Meert1994a}</t>
   </si>
   <si>
-    <t>\cite{Tancyk1987a}</t>
-  </si>
-  <si>
     <t>Halls, Hamilton and Denyszyn</t>
   </si>
   <si>
@@ -2153,6 +2138,24 @@
   </si>
   <si>
     <t>NE-SW Trending dykes</t>
+  </si>
+  <si>
+    <t>\cite{Tanczyk1987a}</t>
+  </si>
+  <si>
+    <t>\cite{Kulakov2013a}</t>
+  </si>
+  <si>
+    <t>\cite{Irving1979a}</t>
+  </si>
+  <si>
+    <t>\cite{Murthy1978a}</t>
+  </si>
+  <si>
+    <t>\cite{Kean1997a}</t>
+  </si>
+  <si>
+    <t>\cite{Elston2002a}</t>
   </si>
 </sst>
 </file>
@@ -3600,10 +3603,10 @@
   <dimension ref="A1:AW103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AM12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B98" sqref="B98"/>
+      <selection pane="bottomRight" activeCell="AU16" sqref="AU16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3803,7 +3806,7 @@
         <v>447</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="C2" s="38">
         <v>2629</v>
@@ -3956,7 +3959,7 @@
         <v>447</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>66</v>
@@ -4102,7 +4105,7 @@
         <v>447</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>66</v>
@@ -4248,7 +4251,7 @@
         <v>447</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>66</v>
@@ -4394,7 +4397,7 @@
         <v>447</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>468</v>
@@ -4545,7 +4548,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>146</v>
@@ -4691,7 +4694,7 @@
         <v>447</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
@@ -4839,7 +4842,7 @@
         <v>447</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>66</v>
@@ -4987,7 +4990,7 @@
         <v>447</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>66</v>
@@ -5135,7 +5138,7 @@
         <v>480</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>482</v>
@@ -5281,7 +5284,7 @@
         <v>480</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>482</v>
@@ -5429,7 +5432,7 @@
         <v>480</v>
       </c>
       <c r="B13" s="109" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>66</v>
@@ -5577,7 +5580,7 @@
         <v>480</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>66</v>
@@ -5723,7 +5726,7 @@
         <v>480</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5869,7 +5872,7 @@
         <v>443</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
@@ -6004,7 +6007,7 @@
       <c r="AS16" s="149"/>
       <c r="AT16" s="126"/>
       <c r="AU16" s="31" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
     </row>
     <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -8116,7 +8119,7 @@
         <v>390</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="C31" s="38">
         <v>5915</v>
@@ -8412,7 +8415,7 @@
         <v>390</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -8561,7 +8564,7 @@
         <v>390</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -8851,7 +8854,7 @@
       </c>
       <c r="AT35" s="126"/>
       <c r="AU35" s="93" t="s">
-        <v>590</v>
+        <v>678</v>
       </c>
     </row>
     <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9000,7 +9003,7 @@
       </c>
       <c r="AT36" s="126"/>
       <c r="AU36" s="93" t="s">
-        <v>590</v>
+        <v>678</v>
       </c>
     </row>
     <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -9008,7 +9011,7 @@
         <v>390</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -9298,7 +9301,7 @@
         <v>82</v>
       </c>
       <c r="AU38" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -9447,7 +9450,7 @@
       </c>
       <c r="AT39" s="143"/>
       <c r="AU39" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9596,7 +9599,7 @@
       </c>
       <c r="AT40" s="126"/>
       <c r="AU40" s="31" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
@@ -9756,7 +9759,7 @@
         <v>74</v>
       </c>
       <c r="B42" s="109" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="C42" s="38">
         <v>2274</v>
@@ -9899,7 +9902,7 @@
       </c>
       <c r="AT42" s="126"/>
       <c r="AU42" s="31" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10050,7 +10053,7 @@
       </c>
       <c r="AT43" s="143"/>
       <c r="AU43" s="33" t="s">
-        <v>595</v>
+        <v>681</v>
       </c>
     </row>
     <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10201,7 +10204,7 @@
       </c>
       <c r="AT44" s="143"/>
       <c r="AU44" s="33" t="s">
-        <v>595</v>
+        <v>681</v>
       </c>
     </row>
     <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -10209,7 +10212,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>121</v>
@@ -10354,7 +10357,7 @@
         <v>127</v>
       </c>
       <c r="AU45" s="33" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10505,7 +10508,7 @@
       </c>
       <c r="AT46" s="143"/>
       <c r="AU46" s="33" t="s">
-        <v>595</v>
+        <v>681</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
@@ -10513,13 +10516,13 @@
         <v>74</v>
       </c>
       <c r="B47" s="113" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>61</v>
@@ -10648,7 +10651,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
       <c r="AU47" s="31" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
     </row>
     <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -10797,7 +10800,7 @@
       </c>
       <c r="AT48" s="126"/>
       <c r="AU48" s="31" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="49" spans="1:49" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10946,7 +10949,7 @@
       </c>
       <c r="AT49" s="126"/>
       <c r="AU49" s="33" t="s">
-        <v>595</v>
+        <v>681</v>
       </c>
     </row>
     <row r="50" spans="1:49" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -11095,7 +11098,7 @@
       </c>
       <c r="AT50" s="126"/>
       <c r="AU50" s="33" t="s">
-        <v>595</v>
+        <v>681</v>
       </c>
     </row>
     <row r="51" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11244,7 +11247,7 @@
       </c>
       <c r="AT51" s="143"/>
       <c r="AU51" s="33" t="s">
-        <v>599</v>
+        <v>679</v>
       </c>
     </row>
     <row r="52" spans="1:49" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -11546,7 +11549,7 @@
       </c>
       <c r="AT53" s="126"/>
       <c r="AU53" s="31" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="54" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11554,14 +11557,14 @@
         <v>74</v>
       </c>
       <c r="B54" s="109" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="39" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="F54" s="38">
         <v>0</v>
@@ -11668,13 +11671,13 @@
         <v>1153</v>
       </c>
       <c r="AL54" s="41" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="AM54" s="109" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="AN54" s="25" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="AO54" s="8">
         <v>2018</v>
@@ -11685,10 +11688,10 @@
       <c r="AS54" s="157"/>
       <c r="AT54" s="126"/>
       <c r="AU54" s="31" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="AW54" s="32" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
     </row>
     <row r="55" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11837,7 +11840,7 @@
       </c>
       <c r="AT55" s="142"/>
       <c r="AU55" s="28" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="56" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11845,13 +11848,13 @@
         <v>74</v>
       </c>
       <c r="B56" s="113" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E56" s="39" t="s">
         <v>168</v>
@@ -11979,7 +11982,7 @@
       <c r="AS56" s="158"/>
       <c r="AT56" s="142"/>
       <c r="AU56" s="28" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="57" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12125,7 +12128,7 @@
       <c r="AS57" s="157"/>
       <c r="AT57" s="142"/>
       <c r="AU57" s="28" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="58" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12270,7 +12273,7 @@
       <c r="AS58" s="157"/>
       <c r="AT58" s="142"/>
       <c r="AU58" s="28" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="59" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12416,7 +12419,7 @@
       <c r="AS59" s="157"/>
       <c r="AT59" s="126"/>
       <c r="AU59" s="28" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.15">
@@ -12540,28 +12543,28 @@
         <v>1106</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AM60" s="33" t="s">
         <v>187</v>
       </c>
       <c r="AN60" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AO60" s="4">
         <v>2019</v>
       </c>
       <c r="AP60" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="AQ60" s="34"/>
       <c r="AR60" s="35"/>
       <c r="AT60" s="142"/>
       <c r="AU60" s="28" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="AW60" s="31" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="61" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -12706,7 +12709,7 @@
       <c r="AS61" s="157"/>
       <c r="AT61" s="142"/>
       <c r="AU61" s="28" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="62" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12853,7 +12856,7 @@
       <c r="AS62" s="157"/>
       <c r="AT62" s="126"/>
       <c r="AU62" s="28" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.15">
@@ -12997,10 +13000,10 @@
       </c>
       <c r="AT63" s="126"/>
       <c r="AU63" s="28" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AW63" s="31" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.15">
@@ -13146,10 +13149,10 @@
       </c>
       <c r="AT64" s="126"/>
       <c r="AU64" s="31" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="AW64" s="31" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -13298,7 +13301,7 @@
       </c>
       <c r="AT65" s="142"/>
       <c r="AU65" s="28" t="s">
-        <v>610</v>
+        <v>680</v>
       </c>
     </row>
     <row r="66" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -13444,10 +13447,10 @@
       <c r="AS66" s="157"/>
       <c r="AT66" s="142"/>
       <c r="AU66" s="28" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="AW66" s="32" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="67" spans="1:49" ht="56" x14ac:dyDescent="0.15">
@@ -13596,7 +13599,7 @@
       </c>
       <c r="AT67" s="126"/>
       <c r="AU67" s="31" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.15">
@@ -13739,7 +13742,7 @@
       <c r="AR68" s="35"/>
       <c r="AT68" s="142"/>
       <c r="AU68" s="28" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="69" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -13864,7 +13867,7 @@
         <v>1087</v>
       </c>
       <c r="AL69" s="41" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="AM69" s="25" t="s">
         <v>224</v>
@@ -13886,9 +13889,11 @@
       </c>
       <c r="AS69" s="157"/>
       <c r="AT69" s="142"/>
-      <c r="AU69" s="28"/>
+      <c r="AU69" s="28" t="s">
+        <v>677</v>
+      </c>
       <c r="AW69" s="31" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="70" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14032,7 +14037,7 @@
       </c>
       <c r="AT70" s="142"/>
       <c r="AU70" s="90" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="71" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14176,7 +14181,7 @@
       </c>
       <c r="AT71" s="142"/>
       <c r="AU71" s="90" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="72" spans="1:49" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -14324,10 +14329,10 @@
       </c>
       <c r="AT72" s="142"/>
       <c r="AU72" s="162" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="AW72" s="31" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="73" spans="1:49" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -14479,10 +14484,10 @@
         <v>245</v>
       </c>
       <c r="AU73" s="162" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="AW73" s="31" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="74" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -14633,7 +14638,7 @@
         <v>251</v>
       </c>
       <c r="AU74" s="161" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="75" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14641,7 +14646,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="C75" s="38">
         <v>5922</v>
@@ -14784,7 +14789,7 @@
       </c>
       <c r="AT75" s="142"/>
       <c r="AU75" s="28" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="AV75" s="131"/>
     </row>
@@ -14793,7 +14798,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="122" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="C76" s="38" t="s">
         <v>66</v>
@@ -14927,7 +14932,7 @@
         <v>260</v>
       </c>
       <c r="AU76" s="28" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AV76" s="131"/>
     </row>
@@ -15079,7 +15084,7 @@
         <v>245</v>
       </c>
       <c r="AU77" s="31" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="AV77" s="131"/>
     </row>
@@ -15233,7 +15238,7 @@
         <v>245</v>
       </c>
       <c r="AU78" s="28" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AV78" s="131"/>
     </row>
@@ -15385,7 +15390,7 @@
       </c>
       <c r="AT79" s="142"/>
       <c r="AU79" s="28" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AV79" s="131"/>
     </row>
@@ -15535,7 +15540,7 @@
       </c>
       <c r="AT80" s="144"/>
       <c r="AU80" s="43" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AV80" s="131"/>
     </row>
@@ -15687,7 +15692,7 @@
         <v>286</v>
       </c>
       <c r="AU81" s="43" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AV81" s="131"/>
     </row>
@@ -15837,7 +15842,7 @@
       </c>
       <c r="AT82" s="141"/>
       <c r="AU82" s="32" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AV82" s="131"/>
     </row>
@@ -15989,7 +15994,7 @@
       </c>
       <c r="AT83" s="141"/>
       <c r="AU83" s="32" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AV83" s="131"/>
     </row>
@@ -15998,7 +16003,7 @@
         <v>74</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="C84" s="38">
         <v>1752</v>
@@ -16143,7 +16148,7 @@
         <v>286</v>
       </c>
       <c r="AU84" s="32" t="s">
-        <v>623</v>
+        <v>676</v>
       </c>
       <c r="AV84" s="131"/>
     </row>
@@ -16270,24 +16275,24 @@
         <v>307</v>
       </c>
       <c r="AN85" s="3" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="AO85" s="4">
         <v>2011</v>
       </c>
       <c r="AP85" s="164" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="AQ85" s="4"/>
       <c r="AR85" s="12"/>
       <c r="AS85" s="159"/>
       <c r="AT85" s="141"/>
       <c r="AU85" s="32" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="AV85" s="131"/>
       <c r="AW85" s="31" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="86" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -16433,7 +16438,7 @@
       </c>
       <c r="AT86" s="141"/>
       <c r="AU86" s="32" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="AV86" s="131"/>
     </row>
@@ -16579,7 +16584,7 @@
       </c>
       <c r="AT87" s="141"/>
       <c r="AU87" s="32" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="AV87" s="131"/>
     </row>
@@ -16724,7 +16729,7 @@
       </c>
       <c r="AT88" s="141"/>
       <c r="AU88" s="32" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="AV88" s="131"/>
     </row>
@@ -16869,7 +16874,7 @@
       </c>
       <c r="AT89" s="126"/>
       <c r="AU89" s="31" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="AV89" s="131"/>
     </row>
@@ -16878,7 +16883,7 @@
         <v>303</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="C90" s="38">
         <v>6607</v>
@@ -17014,7 +17019,7 @@
       </c>
       <c r="AT90" s="145"/>
       <c r="AU90" s="32" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="AV90" s="131"/>
     </row>
@@ -17159,7 +17164,7 @@
       </c>
       <c r="AT91" s="141"/>
       <c r="AU91" s="31" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="AV91" s="131"/>
     </row>
@@ -17304,7 +17309,7 @@
       </c>
       <c r="AT92" s="126"/>
       <c r="AU92" s="31" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="AV92" s="131"/>
     </row>
@@ -17449,7 +17454,7 @@
       </c>
       <c r="AT93" s="126"/>
       <c r="AU93" s="31" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="AV93" s="131"/>
     </row>
@@ -17594,7 +17599,7 @@
       </c>
       <c r="AT94" s="141"/>
       <c r="AU94" s="31" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="95" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17738,7 +17743,7 @@
       </c>
       <c r="AT95" s="141"/>
       <c r="AU95" s="32" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
     </row>
     <row r="96" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17882,7 +17887,7 @@
       </c>
       <c r="AT96" s="126"/>
       <c r="AU96" s="31" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17890,7 +17895,7 @@
         <v>303</v>
       </c>
       <c r="B97" s="123" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="C97" s="38">
         <v>6609</v>
@@ -18026,7 +18031,7 @@
       </c>
       <c r="AT97" s="126"/>
       <c r="AU97" s="32" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
     </row>
     <row r="98" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18170,7 +18175,7 @@
         <v>357</v>
       </c>
       <c r="AU98" s="32" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
     <row r="99" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18178,7 +18183,7 @@
         <v>380</v>
       </c>
       <c r="B99" s="122" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>382</v>
@@ -18312,7 +18317,7 @@
         <v>386</v>
       </c>
       <c r="AU99" s="28" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="100" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18320,7 +18325,7 @@
         <v>380</v>
       </c>
       <c r="B100" s="122" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>382</v>
@@ -18452,7 +18457,7 @@
         <v>389</v>
       </c>
       <c r="AU100" s="28" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="101" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18601,7 +18606,7 @@
       </c>
       <c r="AT101" s="141"/>
       <c r="AU101" s="160" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AV101" s="95"/>
     </row>
@@ -18751,7 +18756,7 @@
       </c>
       <c r="AT102" s="126"/>
       <c r="AU102" s="160" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AV102" s="95"/>
     </row>
@@ -18901,7 +18906,7 @@
       </c>
       <c r="AT103" s="141"/>
       <c r="AU103" s="160" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AV103" s="95"/>
     </row>

</xml_diff>

<commit_message>
fix a few table references
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/Laurentia_Paleogeography/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF07483-A578-0648-8ABE-7415948F992F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73897524-68F6-B640-814A-1BC3B032684B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1620" windowWidth="27820" windowHeight="16340" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-600" yWindow="460" windowWidth="27820" windowHeight="16280" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,14 @@
     <definedName name="fenno98_4" localSheetId="0">'Leirubakki-all'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Leirubakki-all'!$AI$1:$AR$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1882,15 +1888,6 @@
     <t>\cite{Evans1981a}</t>
   </si>
   <si>
-    <t>\cite{Park1973}</t>
-  </si>
-  <si>
-    <t>\cite{Irving2004}</t>
-  </si>
-  <si>
-    <t>\cite{Irving1972}</t>
-  </si>
-  <si>
     <t>\cite{Emslie1976a}</t>
   </si>
   <si>
@@ -2156,6 +2153,15 @@
   </si>
   <si>
     <t>\cite{Elston2002a}</t>
+  </si>
+  <si>
+    <t>\cite{Irving2004a}</t>
+  </si>
+  <si>
+    <t>\cite{Irving1972a}</t>
+  </si>
+  <si>
+    <t>\cite{Park1973a}</t>
   </si>
 </sst>
 </file>
@@ -3603,10 +3609,10 @@
   <dimension ref="A1:AW103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AM12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AL32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU16" sqref="AU16"/>
+      <selection pane="bottomRight" activeCell="AU38" sqref="AU38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3806,7 +3812,7 @@
         <v>447</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C2" s="38">
         <v>2629</v>
@@ -3959,7 +3965,7 @@
         <v>447</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>66</v>
@@ -4105,7 +4111,7 @@
         <v>447</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>66</v>
@@ -4251,7 +4257,7 @@
         <v>447</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>66</v>
@@ -4397,7 +4403,7 @@
         <v>447</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>468</v>
@@ -4548,7 +4554,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>146</v>
@@ -4694,7 +4700,7 @@
         <v>447</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
@@ -4842,7 +4848,7 @@
         <v>447</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>66</v>
@@ -4990,7 +4996,7 @@
         <v>447</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>66</v>
@@ -5138,7 +5144,7 @@
         <v>480</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>482</v>
@@ -5284,7 +5290,7 @@
         <v>480</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>482</v>
@@ -5432,7 +5438,7 @@
         <v>480</v>
       </c>
       <c r="B13" s="109" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>66</v>
@@ -5580,7 +5586,7 @@
         <v>480</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>66</v>
@@ -5726,7 +5732,7 @@
         <v>480</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5872,7 +5878,7 @@
         <v>443</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
@@ -6007,7 +6013,7 @@
       <c r="AS16" s="149"/>
       <c r="AT16" s="126"/>
       <c r="AU16" s="31" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -8119,7 +8125,7 @@
         <v>390</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C31" s="38">
         <v>5915</v>
@@ -8415,7 +8421,7 @@
         <v>390</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -8564,7 +8570,7 @@
         <v>390</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -8854,7 +8860,7 @@
       </c>
       <c r="AT35" s="126"/>
       <c r="AU35" s="93" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9003,7 +9009,7 @@
       </c>
       <c r="AT36" s="126"/>
       <c r="AU36" s="93" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -9011,7 +9017,7 @@
         <v>390</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -9301,7 +9307,7 @@
         <v>82</v>
       </c>
       <c r="AU38" s="33" t="s">
-        <v>590</v>
+        <v>681</v>
       </c>
     </row>
     <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -9450,7 +9456,7 @@
       </c>
       <c r="AT39" s="143"/>
       <c r="AU39" s="33" t="s">
-        <v>591</v>
+        <v>679</v>
       </c>
     </row>
     <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9599,7 +9605,7 @@
       </c>
       <c r="AT40" s="126"/>
       <c r="AU40" s="31" t="s">
-        <v>592</v>
+        <v>680</v>
       </c>
     </row>
     <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
@@ -9759,7 +9765,7 @@
         <v>74</v>
       </c>
       <c r="B42" s="109" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C42" s="38">
         <v>2274</v>
@@ -9902,7 +9908,7 @@
       </c>
       <c r="AT42" s="126"/>
       <c r="AU42" s="31" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10053,7 +10059,7 @@
       </c>
       <c r="AT43" s="143"/>
       <c r="AU43" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10204,7 +10210,7 @@
       </c>
       <c r="AT44" s="143"/>
       <c r="AU44" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -10212,7 +10218,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>121</v>
@@ -10357,7 +10363,7 @@
         <v>127</v>
       </c>
       <c r="AU45" s="33" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10508,7 +10514,7 @@
       </c>
       <c r="AT46" s="143"/>
       <c r="AU46" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
@@ -10516,13 +10522,13 @@
         <v>74</v>
       </c>
       <c r="B47" s="113" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>61</v>
@@ -10651,7 +10657,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
       <c r="AU47" s="31" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -10800,7 +10806,7 @@
       </c>
       <c r="AT48" s="126"/>
       <c r="AU48" s="31" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49" spans="1:49" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10949,7 +10955,7 @@
       </c>
       <c r="AT49" s="126"/>
       <c r="AU49" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="50" spans="1:49" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -11098,7 +11104,7 @@
       </c>
       <c r="AT50" s="126"/>
       <c r="AU50" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="51" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11247,7 +11253,7 @@
       </c>
       <c r="AT51" s="143"/>
       <c r="AU51" s="33" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="52" spans="1:49" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -11549,7 +11555,7 @@
       </c>
       <c r="AT53" s="126"/>
       <c r="AU53" s="31" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="54" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11557,14 +11563,14 @@
         <v>74</v>
       </c>
       <c r="B54" s="109" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="39" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F54" s="38">
         <v>0</v>
@@ -11671,13 +11677,13 @@
         <v>1153</v>
       </c>
       <c r="AL54" s="41" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="AM54" s="109" t="s">
+        <v>636</v>
+      </c>
+      <c r="AN54" s="25" t="s">
         <v>639</v>
-      </c>
-      <c r="AN54" s="25" t="s">
-        <v>642</v>
       </c>
       <c r="AO54" s="8">
         <v>2018</v>
@@ -11688,10 +11694,10 @@
       <c r="AS54" s="157"/>
       <c r="AT54" s="126"/>
       <c r="AU54" s="31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AW54" s="32" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="55" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11840,7 +11846,7 @@
       </c>
       <c r="AT55" s="142"/>
       <c r="AU55" s="28" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="56" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11848,13 +11854,13 @@
         <v>74</v>
       </c>
       <c r="B56" s="113" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E56" s="39" t="s">
         <v>168</v>
@@ -11982,7 +11988,7 @@
       <c r="AS56" s="158"/>
       <c r="AT56" s="142"/>
       <c r="AU56" s="28" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="57" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12128,7 +12134,7 @@
       <c r="AS57" s="157"/>
       <c r="AT57" s="142"/>
       <c r="AU57" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="58" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12273,7 +12279,7 @@
       <c r="AS58" s="157"/>
       <c r="AT58" s="142"/>
       <c r="AU58" s="28" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="59" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12419,7 +12425,7 @@
       <c r="AS59" s="157"/>
       <c r="AT59" s="126"/>
       <c r="AU59" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.15">
@@ -12543,28 +12549,28 @@
         <v>1106</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AM60" s="33" t="s">
         <v>187</v>
       </c>
       <c r="AN60" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="AO60" s="4">
         <v>2019</v>
       </c>
       <c r="AP60" s="3" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AQ60" s="34"/>
       <c r="AR60" s="35"/>
       <c r="AT60" s="142"/>
       <c r="AU60" s="28" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="AW60" s="31" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="61" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -12709,7 +12715,7 @@
       <c r="AS61" s="157"/>
       <c r="AT61" s="142"/>
       <c r="AU61" s="28" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="62" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12856,7 +12862,7 @@
       <c r="AS62" s="157"/>
       <c r="AT62" s="126"/>
       <c r="AU62" s="28" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.15">
@@ -13000,10 +13006,10 @@
       </c>
       <c r="AT63" s="126"/>
       <c r="AU63" s="28" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="AW63" s="31" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.15">
@@ -13149,10 +13155,10 @@
       </c>
       <c r="AT64" s="126"/>
       <c r="AU64" s="31" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="AW64" s="31" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -13301,7 +13307,7 @@
       </c>
       <c r="AT65" s="142"/>
       <c r="AU65" s="28" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="66" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -13447,10 +13453,10 @@
       <c r="AS66" s="157"/>
       <c r="AT66" s="142"/>
       <c r="AU66" s="28" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="AW66" s="32" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="67" spans="1:49" ht="56" x14ac:dyDescent="0.15">
@@ -13599,7 +13605,7 @@
       </c>
       <c r="AT67" s="126"/>
       <c r="AU67" s="31" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.15">
@@ -13742,7 +13748,7 @@
       <c r="AR68" s="35"/>
       <c r="AT68" s="142"/>
       <c r="AU68" s="28" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="69" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -13867,7 +13873,7 @@
         <v>1087</v>
       </c>
       <c r="AL69" s="41" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AM69" s="25" t="s">
         <v>224</v>
@@ -13890,10 +13896,10 @@
       <c r="AS69" s="157"/>
       <c r="AT69" s="142"/>
       <c r="AU69" s="28" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="AW69" s="31" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="70" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14037,7 +14043,7 @@
       </c>
       <c r="AT70" s="142"/>
       <c r="AU70" s="90" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="71" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14181,7 +14187,7 @@
       </c>
       <c r="AT71" s="142"/>
       <c r="AU71" s="90" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="72" spans="1:49" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -14329,10 +14335,10 @@
       </c>
       <c r="AT72" s="142"/>
       <c r="AU72" s="162" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="AW72" s="31" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="73" spans="1:49" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -14484,10 +14490,10 @@
         <v>245</v>
       </c>
       <c r="AU73" s="162" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="AW73" s="31" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="74" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -14638,7 +14644,7 @@
         <v>251</v>
       </c>
       <c r="AU74" s="161" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="75" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14646,7 +14652,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C75" s="38">
         <v>5922</v>
@@ -14789,7 +14795,7 @@
       </c>
       <c r="AT75" s="142"/>
       <c r="AU75" s="28" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="AV75" s="131"/>
     </row>
@@ -14798,7 +14804,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="122" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C76" s="38" t="s">
         <v>66</v>
@@ -14932,7 +14938,7 @@
         <v>260</v>
       </c>
       <c r="AU76" s="28" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="AV76" s="131"/>
     </row>
@@ -15084,7 +15090,7 @@
         <v>245</v>
       </c>
       <c r="AU77" s="31" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AV77" s="131"/>
     </row>
@@ -15238,7 +15244,7 @@
         <v>245</v>
       </c>
       <c r="AU78" s="28" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="AV78" s="131"/>
     </row>
@@ -15390,7 +15396,7 @@
       </c>
       <c r="AT79" s="142"/>
       <c r="AU79" s="28" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="AV79" s="131"/>
     </row>
@@ -15540,7 +15546,7 @@
       </c>
       <c r="AT80" s="144"/>
       <c r="AU80" s="43" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AV80" s="131"/>
     </row>
@@ -15692,7 +15698,7 @@
         <v>286</v>
       </c>
       <c r="AU81" s="43" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AV81" s="131"/>
     </row>
@@ -15842,7 +15848,7 @@
       </c>
       <c r="AT82" s="141"/>
       <c r="AU82" s="32" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="AV82" s="131"/>
     </row>
@@ -15994,7 +16000,7 @@
       </c>
       <c r="AT83" s="141"/>
       <c r="AU83" s="32" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="AV83" s="131"/>
     </row>
@@ -16003,7 +16009,7 @@
         <v>74</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C84" s="38">
         <v>1752</v>
@@ -16148,7 +16154,7 @@
         <v>286</v>
       </c>
       <c r="AU84" s="32" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="AV84" s="131"/>
     </row>
@@ -16275,24 +16281,24 @@
         <v>307</v>
       </c>
       <c r="AN85" s="3" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AO85" s="4">
         <v>2011</v>
       </c>
       <c r="AP85" s="164" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="AQ85" s="4"/>
       <c r="AR85" s="12"/>
       <c r="AS85" s="159"/>
       <c r="AT85" s="141"/>
       <c r="AU85" s="32" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="AV85" s="131"/>
       <c r="AW85" s="31" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="86" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -16438,7 +16444,7 @@
       </c>
       <c r="AT86" s="141"/>
       <c r="AU86" s="32" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="AV86" s="131"/>
     </row>
@@ -16584,7 +16590,7 @@
       </c>
       <c r="AT87" s="141"/>
       <c r="AU87" s="32" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="AV87" s="131"/>
     </row>
@@ -16729,7 +16735,7 @@
       </c>
       <c r="AT88" s="141"/>
       <c r="AU88" s="32" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="AV88" s="131"/>
     </row>
@@ -16874,7 +16880,7 @@
       </c>
       <c r="AT89" s="126"/>
       <c r="AU89" s="31" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="AV89" s="131"/>
     </row>
@@ -16883,7 +16889,7 @@
         <v>303</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C90" s="38">
         <v>6607</v>
@@ -17019,7 +17025,7 @@
       </c>
       <c r="AT90" s="145"/>
       <c r="AU90" s="32" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="AV90" s="131"/>
     </row>
@@ -17164,7 +17170,7 @@
       </c>
       <c r="AT91" s="141"/>
       <c r="AU91" s="31" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="AV91" s="131"/>
     </row>
@@ -17309,7 +17315,7 @@
       </c>
       <c r="AT92" s="126"/>
       <c r="AU92" s="31" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="AV92" s="131"/>
     </row>
@@ -17454,7 +17460,7 @@
       </c>
       <c r="AT93" s="126"/>
       <c r="AU93" s="31" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="AV93" s="131"/>
     </row>
@@ -17599,7 +17605,7 @@
       </c>
       <c r="AT94" s="141"/>
       <c r="AU94" s="31" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="95" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17743,7 +17749,7 @@
       </c>
       <c r="AT95" s="141"/>
       <c r="AU95" s="32" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="96" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17887,7 +17893,7 @@
       </c>
       <c r="AT96" s="126"/>
       <c r="AU96" s="31" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17895,7 +17901,7 @@
         <v>303</v>
       </c>
       <c r="B97" s="123" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C97" s="38">
         <v>6609</v>
@@ -18031,7 +18037,7 @@
       </c>
       <c r="AT97" s="126"/>
       <c r="AU97" s="32" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="98" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18175,7 +18181,7 @@
         <v>357</v>
       </c>
       <c r="AU98" s="32" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="99" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18183,7 +18189,7 @@
         <v>380</v>
       </c>
       <c r="B99" s="122" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>382</v>
@@ -18317,7 +18323,7 @@
         <v>386</v>
       </c>
       <c r="AU99" s="28" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="100" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18325,7 +18331,7 @@
         <v>380</v>
       </c>
       <c r="B100" s="122" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>382</v>
@@ -18457,7 +18463,7 @@
         <v>389</v>
       </c>
       <c r="AU100" s="28" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="101" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18606,7 +18612,7 @@
       </c>
       <c r="AT101" s="141"/>
       <c r="AU101" s="160" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="AV101" s="95"/>
     </row>
@@ -18756,7 +18762,7 @@
       </c>
       <c r="AT102" s="126"/>
       <c r="AU102" s="160" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="AV102" s="95"/>
     </row>
@@ -18906,7 +18912,7 @@
       </c>
       <c r="AT103" s="141"/>
       <c r="AU103" s="160" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="AV103" s="95"/>
     </row>

</xml_diff>

<commit_message>
small fixes to references
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73897524-68F6-B640-814A-1BC3B032684B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF4E3B9-5171-5741-8E5E-65A03A840461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-600" yWindow="460" windowWidth="27820" windowHeight="16280" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="16280" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -1799,9 +1799,6 @@
     <t>\cite{Symons1999a}</t>
   </si>
   <si>
-    <t>\cite{Kilian2016a}</t>
-  </si>
-  <si>
     <t>\cite{Kilian2015a}</t>
   </si>
   <si>
@@ -1921,9 +1918,6 @@
     <t>\cite{Fairchild2017a}</t>
   </si>
   <si>
-    <t>\cite{Donadini2011a}</t>
-  </si>
-  <si>
     <t>\cite{Weil2003a}</t>
   </si>
   <si>
@@ -1948,9 +1942,6 @@
     <t>\cite{Park1989a}</t>
   </si>
   <si>
-    <t>\cite{Weil2006a}</t>
-  </si>
-  <si>
     <t>\cite{Denyszyn2009a}</t>
   </si>
   <si>
@@ -2162,6 +2153,15 @@
   </si>
   <si>
     <t>\cite{Park1973a}</t>
+  </si>
+  <si>
+    <t>\cite{Donadini2011b}</t>
+  </si>
+  <si>
+    <t>\cite{Kilian2016b}</t>
+  </si>
+  <si>
+    <t>\cite{Weil2006b}</t>
   </si>
 </sst>
 </file>
@@ -3609,10 +3609,10 @@
   <dimension ref="A1:AW103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AL32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AM68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU38" sqref="AU38"/>
+      <selection pane="bottomRight" activeCell="AU77" sqref="AU77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3804,7 +3804,7 @@
         <v>556</v>
       </c>
       <c r="AW1" s="24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -3812,7 +3812,7 @@
         <v>447</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C2" s="38">
         <v>2629</v>
@@ -3957,7 +3957,7 @@
         <v>457</v>
       </c>
       <c r="AU2" s="160" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:49" s="105" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -3965,7 +3965,7 @@
         <v>447</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>66</v>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="AT3" s="126"/>
       <c r="AU3" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4111,7 +4111,7 @@
         <v>447</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>66</v>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="AT4" s="141"/>
       <c r="AU4" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4257,7 +4257,7 @@
         <v>447</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>66</v>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="AT5" s="126"/>
       <c r="AU5" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:49" s="108" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -4403,7 +4403,7 @@
         <v>447</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>468</v>
@@ -4543,10 +4543,10 @@
       </c>
       <c r="AT6" s="141"/>
       <c r="AU6" s="160" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AW6" s="160" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -4554,7 +4554,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>146</v>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="AT7" s="141"/>
       <c r="AU7" s="160" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8" spans="1:49" s="108" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4700,7 +4700,7 @@
         <v>447</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="AT8" s="141"/>
       <c r="AU8" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4848,7 +4848,7 @@
         <v>447</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>66</v>
@@ -4988,7 +4988,7 @@
         <v>457</v>
       </c>
       <c r="AU9" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -4996,7 +4996,7 @@
         <v>447</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>66</v>
@@ -5136,7 +5136,7 @@
         <v>386</v>
       </c>
       <c r="AU10" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:49" ht="70" x14ac:dyDescent="0.15">
@@ -5144,7 +5144,7 @@
         <v>480</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>482</v>
@@ -5282,7 +5282,7 @@
         <v>386</v>
       </c>
       <c r="AU11" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:49" s="33" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -5290,7 +5290,7 @@
         <v>480</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>482</v>
@@ -5430,7 +5430,7 @@
         <v>489</v>
       </c>
       <c r="AU12" s="161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:49" ht="28" x14ac:dyDescent="0.15">
@@ -5438,7 +5438,7 @@
         <v>480</v>
       </c>
       <c r="B13" s="109" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>66</v>
@@ -5578,7 +5578,7 @@
         <v>489</v>
       </c>
       <c r="AU13" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="14" spans="1:49" s="33" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -5586,7 +5586,7 @@
         <v>480</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>66</v>
@@ -5724,7 +5724,7 @@
         <v>386</v>
       </c>
       <c r="AU14" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="15" spans="1:49" s="94" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -5732,7 +5732,7 @@
         <v>480</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5870,7 +5870,7 @@
       </c>
       <c r="AT15" s="126"/>
       <c r="AU15" s="161" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="16" spans="1:49" s="94" customFormat="1" x14ac:dyDescent="0.15">
@@ -5878,7 +5878,7 @@
         <v>443</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
@@ -6013,7 +6013,7 @@
       <c r="AS16" s="149"/>
       <c r="AT16" s="126"/>
       <c r="AU16" s="31" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="17" spans="1:49" s="33" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -6160,7 +6160,7 @@
         <v>536</v>
       </c>
       <c r="AU17" s="162" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="18" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.15">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="AT18" s="142"/>
       <c r="AU18" s="90" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="19" spans="1:49" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6456,7 +6456,7 @@
         <v>552</v>
       </c>
       <c r="AU19" s="90" t="s">
-        <v>561</v>
+        <v>680</v>
       </c>
     </row>
     <row r="20" spans="1:49" ht="70" x14ac:dyDescent="0.15">
@@ -6902,13 +6902,13 @@
       </c>
       <c r="AT22" s="142"/>
       <c r="AU22" s="162" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AV22" s="33" t="s">
         <v>558</v>
       </c>
       <c r="AW22" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="23" spans="1:49" s="33" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -7057,10 +7057,10 @@
       </c>
       <c r="AT23" s="126"/>
       <c r="AU23" s="31" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AV23" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="42" x14ac:dyDescent="0.15">
@@ -7211,7 +7211,7 @@
         <v>373</v>
       </c>
       <c r="AU24" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="25" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7362,7 +7362,7 @@
         <v>373</v>
       </c>
       <c r="AU25" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="26" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7510,10 +7510,10 @@
       </c>
       <c r="AT26" s="141"/>
       <c r="AU26" s="32" t="s">
+        <v>576</v>
+      </c>
+      <c r="AV26" s="32" t="s">
         <v>577</v>
-      </c>
-      <c r="AV26" s="32" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="27" spans="1:49" s="28" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -7663,10 +7663,10 @@
         <v>401</v>
       </c>
       <c r="AU27" s="28" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AV27" s="31" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="28" spans="1:49" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -7814,10 +7814,10 @@
       </c>
       <c r="AT28" s="141"/>
       <c r="AU28" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AV28" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="98" x14ac:dyDescent="0.15">
@@ -7962,10 +7962,10 @@
       </c>
       <c r="AT29" s="141"/>
       <c r="AU29" s="105" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AV29" s="31" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="30" spans="1:49" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -8114,10 +8114,10 @@
       </c>
       <c r="AT30" s="141"/>
       <c r="AU30" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="AV30" s="32" t="s">
         <v>579</v>
-      </c>
-      <c r="AV30" s="32" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="31" spans="1:49" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -8125,7 +8125,7 @@
         <v>390</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C31" s="38">
         <v>5915</v>
@@ -8264,7 +8264,7 @@
       </c>
       <c r="AT31" s="141"/>
       <c r="AU31" s="108" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="32" spans="1:49" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -8413,7 +8413,7 @@
         <v>427</v>
       </c>
       <c r="AU32" s="105" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="33" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -8421,7 +8421,7 @@
         <v>390</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -8562,7 +8562,7 @@
       </c>
       <c r="AT33" s="126"/>
       <c r="AU33" s="93" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -8570,7 +8570,7 @@
         <v>390</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="AT34" s="126"/>
       <c r="AU34" s="93" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -8860,7 +8860,7 @@
       </c>
       <c r="AT35" s="126"/>
       <c r="AU35" s="93" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="36" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9009,7 +9009,7 @@
       </c>
       <c r="AT36" s="126"/>
       <c r="AU36" s="93" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="37" spans="1:48" ht="56" x14ac:dyDescent="0.15">
@@ -9017,7 +9017,7 @@
         <v>390</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -9156,7 +9156,7 @@
       </c>
       <c r="AT37" s="126"/>
       <c r="AU37" s="93" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9307,7 +9307,7 @@
         <v>82</v>
       </c>
       <c r="AU38" s="33" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="39" spans="1:48" s="28" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -9456,7 +9456,7 @@
       </c>
       <c r="AT39" s="143"/>
       <c r="AU39" s="33" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="40" spans="1:48" s="90" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -9605,7 +9605,7 @@
       </c>
       <c r="AT40" s="126"/>
       <c r="AU40" s="31" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="41" spans="1:48" s="90" customFormat="1" ht="154" x14ac:dyDescent="0.15">
@@ -9754,10 +9754,10 @@
       </c>
       <c r="AT41" s="143"/>
       <c r="AU41" s="33" t="s">
+        <v>586</v>
+      </c>
+      <c r="AV41" s="142" t="s">
         <v>587</v>
-      </c>
-      <c r="AV41" s="142" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="42" spans="1:48" s="87" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -9765,7 +9765,7 @@
         <v>74</v>
       </c>
       <c r="B42" s="109" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C42" s="38">
         <v>2274</v>
@@ -9908,7 +9908,7 @@
       </c>
       <c r="AT42" s="126"/>
       <c r="AU42" s="31" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="43" spans="1:48" s="87" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10059,7 +10059,7 @@
       </c>
       <c r="AT43" s="143"/>
       <c r="AU43" s="33" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="44" spans="1:48" s="93" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10210,7 +10210,7 @@
       </c>
       <c r="AT44" s="143"/>
       <c r="AU44" s="33" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="45" spans="1:48" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -10218,7 +10218,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="112" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>121</v>
@@ -10363,7 +10363,7 @@
         <v>127</v>
       </c>
       <c r="AU45" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="46" spans="1:48" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="AT46" s="143"/>
       <c r="AU46" s="33" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
@@ -10522,13 +10522,13 @@
         <v>74</v>
       </c>
       <c r="B47" s="113" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>61</v>
@@ -10657,7 +10657,7 @@
       <c r="AS47" s="158"/>
       <c r="AT47" s="126"/>
       <c r="AU47" s="31" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="48" spans="1:48" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -10806,7 +10806,7 @@
       </c>
       <c r="AT48" s="126"/>
       <c r="AU48" s="31" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="49" spans="1:49" s="28" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -10955,7 +10955,7 @@
       </c>
       <c r="AT49" s="126"/>
       <c r="AU49" s="33" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="50" spans="1:49" s="43" customFormat="1" ht="84" x14ac:dyDescent="0.15">
@@ -11104,7 +11104,7 @@
       </c>
       <c r="AT50" s="126"/>
       <c r="AU50" s="33" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="51" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11253,7 +11253,7 @@
       </c>
       <c r="AT51" s="143"/>
       <c r="AU51" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="52" spans="1:49" s="32" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -11404,7 +11404,7 @@
       </c>
       <c r="AT52" s="143"/>
       <c r="AU52" s="33" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="53" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11555,7 +11555,7 @@
       </c>
       <c r="AT53" s="126"/>
       <c r="AU53" s="31" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="54" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11563,14 +11563,14 @@
         <v>74</v>
       </c>
       <c r="B54" s="109" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="39" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F54" s="38">
         <v>0</v>
@@ -11677,13 +11677,13 @@
         <v>1153</v>
       </c>
       <c r="AL54" s="41" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="AM54" s="109" t="s">
+        <v>633</v>
+      </c>
+      <c r="AN54" s="25" t="s">
         <v>636</v>
-      </c>
-      <c r="AN54" s="25" t="s">
-        <v>639</v>
       </c>
       <c r="AO54" s="8">
         <v>2018</v>
@@ -11694,10 +11694,10 @@
       <c r="AS54" s="157"/>
       <c r="AT54" s="126"/>
       <c r="AU54" s="31" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="AW54" s="32" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="55" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -11846,7 +11846,7 @@
       </c>
       <c r="AT55" s="142"/>
       <c r="AU55" s="28" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="56" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -11854,13 +11854,13 @@
         <v>74</v>
       </c>
       <c r="B56" s="113" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E56" s="39" t="s">
         <v>168</v>
@@ -11988,7 +11988,7 @@
       <c r="AS56" s="158"/>
       <c r="AT56" s="142"/>
       <c r="AU56" s="28" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="57" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12134,7 +12134,7 @@
       <c r="AS57" s="157"/>
       <c r="AT57" s="142"/>
       <c r="AU57" s="28" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="58" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12279,7 +12279,7 @@
       <c r="AS58" s="157"/>
       <c r="AT58" s="142"/>
       <c r="AU58" s="28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="59" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12425,7 +12425,7 @@
       <c r="AS59" s="157"/>
       <c r="AT59" s="126"/>
       <c r="AU59" s="28" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.15">
@@ -12549,28 +12549,28 @@
         <v>1106</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AM60" s="33" t="s">
         <v>187</v>
       </c>
       <c r="AN60" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AO60" s="4">
         <v>2019</v>
       </c>
       <c r="AP60" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="AQ60" s="34"/>
       <c r="AR60" s="35"/>
       <c r="AT60" s="142"/>
       <c r="AU60" s="28" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="AW60" s="31" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="61" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -12715,7 +12715,7 @@
       <c r="AS61" s="157"/>
       <c r="AT61" s="142"/>
       <c r="AU61" s="28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="62" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -12862,7 +12862,7 @@
       <c r="AS62" s="157"/>
       <c r="AT62" s="126"/>
       <c r="AU62" s="28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.15">
@@ -13006,10 +13006,10 @@
       </c>
       <c r="AT63" s="126"/>
       <c r="AU63" s="28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AW63" s="31" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.15">
@@ -13155,10 +13155,10 @@
       </c>
       <c r="AT64" s="126"/>
       <c r="AU64" s="31" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="AW64" s="31" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -13307,7 +13307,7 @@
       </c>
       <c r="AT65" s="142"/>
       <c r="AU65" s="28" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="66" spans="1:49" s="32" customFormat="1" x14ac:dyDescent="0.15">
@@ -13453,10 +13453,10 @@
       <c r="AS66" s="157"/>
       <c r="AT66" s="142"/>
       <c r="AU66" s="28" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="AW66" s="32" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="67" spans="1:49" ht="56" x14ac:dyDescent="0.15">
@@ -13605,7 +13605,7 @@
       </c>
       <c r="AT67" s="126"/>
       <c r="AU67" s="31" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.15">
@@ -13748,7 +13748,7 @@
       <c r="AR68" s="35"/>
       <c r="AT68" s="142"/>
       <c r="AU68" s="28" t="s">
-        <v>601</v>
+        <v>679</v>
       </c>
     </row>
     <row r="69" spans="1:49" s="46" customFormat="1" x14ac:dyDescent="0.15">
@@ -13873,7 +13873,7 @@
         <v>1087</v>
       </c>
       <c r="AL69" s="41" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AM69" s="25" t="s">
         <v>224</v>
@@ -13896,10 +13896,10 @@
       <c r="AS69" s="157"/>
       <c r="AT69" s="142"/>
       <c r="AU69" s="28" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="AW69" s="31" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="70" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14043,7 +14043,7 @@
       </c>
       <c r="AT70" s="142"/>
       <c r="AU70" s="90" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="71" spans="1:49" s="32" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -14187,7 +14187,7 @@
       </c>
       <c r="AT71" s="142"/>
       <c r="AU71" s="90" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="72" spans="1:49" s="108" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -14335,10 +14335,10 @@
       </c>
       <c r="AT72" s="142"/>
       <c r="AU72" s="162" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AW72" s="31" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="73" spans="1:49" s="93" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -14490,10 +14490,10 @@
         <v>245</v>
       </c>
       <c r="AU73" s="162" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AW73" s="31" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="74" spans="1:49" s="108" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -14644,7 +14644,7 @@
         <v>251</v>
       </c>
       <c r="AU74" s="161" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="75" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -14652,7 +14652,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C75" s="38">
         <v>5922</v>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="AT75" s="142"/>
       <c r="AU75" s="28" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="AV75" s="131"/>
     </row>
@@ -14804,7 +14804,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="122" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C76" s="38" t="s">
         <v>66</v>
@@ -14938,7 +14938,7 @@
         <v>260</v>
       </c>
       <c r="AU76" s="28" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="AV76" s="131"/>
     </row>
@@ -15090,7 +15090,7 @@
         <v>245</v>
       </c>
       <c r="AU77" s="31" t="s">
-        <v>610</v>
+        <v>681</v>
       </c>
       <c r="AV77" s="131"/>
     </row>
@@ -15244,7 +15244,7 @@
         <v>245</v>
       </c>
       <c r="AU78" s="28" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="AV78" s="131"/>
     </row>
@@ -15396,7 +15396,7 @@
       </c>
       <c r="AT79" s="142"/>
       <c r="AU79" s="28" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="AV79" s="131"/>
     </row>
@@ -15546,7 +15546,7 @@
       </c>
       <c r="AT80" s="144"/>
       <c r="AU80" s="43" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AV80" s="131"/>
     </row>
@@ -15698,7 +15698,7 @@
         <v>286</v>
       </c>
       <c r="AU81" s="43" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AV81" s="131"/>
     </row>
@@ -15848,7 +15848,7 @@
       </c>
       <c r="AT82" s="141"/>
       <c r="AU82" s="32" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="AV82" s="131"/>
     </row>
@@ -16000,7 +16000,7 @@
       </c>
       <c r="AT83" s="141"/>
       <c r="AU83" s="32" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="AV83" s="131"/>
     </row>
@@ -16009,7 +16009,7 @@
         <v>74</v>
       </c>
       <c r="B84" s="109" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C84" s="38">
         <v>1752</v>
@@ -16154,7 +16154,7 @@
         <v>286</v>
       </c>
       <c r="AU84" s="32" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="AV84" s="131"/>
     </row>
@@ -16281,24 +16281,24 @@
         <v>307</v>
       </c>
       <c r="AN85" s="3" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AO85" s="4">
         <v>2011</v>
       </c>
       <c r="AP85" s="164" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="AQ85" s="4"/>
       <c r="AR85" s="12"/>
       <c r="AS85" s="159"/>
       <c r="AT85" s="141"/>
       <c r="AU85" s="32" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="AV85" s="131"/>
       <c r="AW85" s="31" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="86" spans="1:49" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -16444,7 +16444,7 @@
       </c>
       <c r="AT86" s="141"/>
       <c r="AU86" s="32" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AV86" s="131"/>
     </row>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="AT87" s="141"/>
       <c r="AU87" s="32" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="AV87" s="131"/>
     </row>
@@ -16735,7 +16735,7 @@
       </c>
       <c r="AT88" s="141"/>
       <c r="AU88" s="32" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="AV88" s="131"/>
     </row>
@@ -16880,7 +16880,7 @@
       </c>
       <c r="AT89" s="126"/>
       <c r="AU89" s="31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AV89" s="131"/>
     </row>
@@ -16889,7 +16889,7 @@
         <v>303</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C90" s="38">
         <v>6607</v>
@@ -17025,7 +17025,7 @@
       </c>
       <c r="AT90" s="145"/>
       <c r="AU90" s="32" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="AV90" s="131"/>
     </row>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="AT91" s="141"/>
       <c r="AU91" s="31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AV91" s="131"/>
     </row>
@@ -17315,7 +17315,7 @@
       </c>
       <c r="AT92" s="126"/>
       <c r="AU92" s="31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AV92" s="131"/>
     </row>
@@ -17460,7 +17460,7 @@
       </c>
       <c r="AT93" s="126"/>
       <c r="AU93" s="31" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="AV93" s="131"/>
     </row>
@@ -17605,7 +17605,7 @@
       </c>
       <c r="AT94" s="141"/>
       <c r="AU94" s="31" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="95" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17749,7 +17749,7 @@
       </c>
       <c r="AT95" s="141"/>
       <c r="AU95" s="32" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="96" spans="1:49" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17893,7 +17893,7 @@
       </c>
       <c r="AT96" s="126"/>
       <c r="AU96" s="31" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="97" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -17901,7 +17901,7 @@
         <v>303</v>
       </c>
       <c r="B97" s="123" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C97" s="38">
         <v>6609</v>
@@ -18037,7 +18037,7 @@
       </c>
       <c r="AT97" s="126"/>
       <c r="AU97" s="32" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="98" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18181,7 +18181,7 @@
         <v>357</v>
       </c>
       <c r="AU98" s="32" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="99" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18189,7 +18189,7 @@
         <v>380</v>
       </c>
       <c r="B99" s="122" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>382</v>
@@ -18323,7 +18323,7 @@
         <v>386</v>
       </c>
       <c r="AU99" s="28" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="100" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18331,7 +18331,7 @@
         <v>380</v>
       </c>
       <c r="B100" s="122" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>382</v>
@@ -18463,7 +18463,7 @@
         <v>389</v>
       </c>
       <c r="AU100" s="28" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="101" spans="1:48" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -18612,7 +18612,7 @@
       </c>
       <c r="AT101" s="141"/>
       <c r="AU101" s="160" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AV101" s="95"/>
     </row>
@@ -18762,7 +18762,7 @@
       </c>
       <c r="AT102" s="126"/>
       <c r="AU102" s="160" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AV102" s="95"/>
     </row>
@@ -18912,7 +18912,7 @@
       </c>
       <c r="AT103" s="141"/>
       <c r="AU103" s="160" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AV103" s="95"/>
     </row>

</xml_diff>

<commit_message>
update table with Chuar poles
</commit_message>
<xml_diff>
--- a/Data/Leirubakki_Laurentia.xlsx
+++ b/Data/Leirubakki_Laurentia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5A2A54-D5FB-404D-A019-CDD9C5EDD1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7314A3-C617-EB4B-9DBD-4DFB1D4E7010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-940" yWindow="1200" windowWidth="28800" windowHeight="12360" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="12900" windowWidth="28800" windowHeight="12360" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leirubakki-all" sheetId="1" r:id="rId1"/>
@@ -3685,10 +3685,10 @@
   <dimension ref="A1:BD107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AW95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U93" sqref="U93"/>
+      <selection pane="bottomRight" activeCell="BB96" sqref="BB96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>